<commit_message>
Update BAU battery subsidies based on ITC expiration year
</commit_message>
<xml_diff>
--- a/InputData/elec/BPSpUGBCD/BAU Subsidy per Unit Grid Battery Capacity Deployed.xlsx
+++ b/InputData/elec/BPSpUGBCD/BAU Subsidy per Unit Grid Battery Capacity Deployed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\BSpUGBCD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\BPSpUGBCD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50321F0-A6F9-48AB-8C5A-98FD513AF3DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7AAA04-DC71-48D8-A62F-D6E4D2525FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -283,6 +283,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -920,7 +921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -977,8 +978,8 @@
   </sheetPr>
   <dimension ref="A1:AJ534"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A72" sqref="A72:XFD73"/>
+    <sheetView tabSelected="1" topLeftCell="C62" workbookViewId="0">
+      <selection activeCell="P75" sqref="P75:W75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4598,22 +4599,22 @@
         <v>1</v>
       </c>
       <c r="Q75" s="37">
+        <v>1</v>
+      </c>
+      <c r="R75" s="37">
+        <v>1</v>
+      </c>
+      <c r="S75" s="37">
+        <v>1</v>
+      </c>
+      <c r="T75" s="37">
+        <v>1</v>
+      </c>
+      <c r="U75" s="37">
         <v>0.75</v>
       </c>
-      <c r="R75" s="37">
+      <c r="V75" s="37">
         <v>0.5</v>
-      </c>
-      <c r="S75" s="37">
-        <v>0</v>
-      </c>
-      <c r="T75" s="37">
-        <v>0</v>
-      </c>
-      <c r="U75" s="37">
-        <v>0</v>
-      </c>
-      <c r="V75" s="37">
-        <v>0</v>
       </c>
       <c r="W75" s="37">
         <v>0</v>
@@ -5250,27 +5251,27 @@
       </c>
       <c r="P88" s="38">
         <f t="shared" si="5"/>
-        <v>0.31218750000000001</v>
+        <v>0.41625000000000001</v>
       </c>
       <c r="Q88" s="38">
         <f t="shared" si="5"/>
-        <v>0.208125</v>
+        <v>0.41625000000000001</v>
       </c>
       <c r="R88" s="38">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.41625000000000001</v>
       </c>
       <c r="S88" s="38">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.41625000000000001</v>
       </c>
       <c r="T88" s="38">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.31218750000000001</v>
       </c>
       <c r="U88" s="38">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.208125</v>
       </c>
       <c r="V88" s="38">
         <f t="shared" si="5"/>
@@ -22450,27 +22451,27 @@
       </c>
       <c r="R2" s="2">
         <f>'Inflation Reduction Act'!P88</f>
-        <v>0.31218750000000001</v>
+        <v>0.41625000000000001</v>
       </c>
       <c r="S2" s="2">
         <f>'Inflation Reduction Act'!Q88</f>
-        <v>0.208125</v>
+        <v>0.41625000000000001</v>
       </c>
       <c r="T2">
         <f>'Inflation Reduction Act'!R88</f>
-        <v>0</v>
+        <v>0.41625000000000001</v>
       </c>
       <c r="U2">
         <f>'Inflation Reduction Act'!S88</f>
-        <v>0</v>
+        <v>0.41625000000000001</v>
       </c>
       <c r="V2">
         <f>'Inflation Reduction Act'!T88</f>
-        <v>0</v>
+        <v>0.31218750000000001</v>
       </c>
       <c r="W2">
         <f>'Inflation Reduction Act'!U88</f>
-        <v>0</v>
+        <v>0.208125</v>
       </c>
       <c r="X2">
         <f>'Inflation Reduction Act'!V88</f>

</xml_diff>

<commit_message>
Correct error in IRA phase out schedule for battery storage
</commit_message>
<xml_diff>
--- a/InputData/elec/BPSpUGBCD/BAU Subsidy per Unit Grid Battery Capacity Deployed.xlsx
+++ b/InputData/elec/BPSpUGBCD/BAU Subsidy per Unit Grid Battery Capacity Deployed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\BPSpUGBCD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\BPSpUGBCD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7AAA04-DC71-48D8-A62F-D6E4D2525FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05BA5FBF-5F9B-49F9-9A89-22A14C777523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -978,8 +978,8 @@
   </sheetPr>
   <dimension ref="A1:AJ534"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C62" workbookViewId="0">
-      <selection activeCell="P75" sqref="P75:W75"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="J77" sqref="J77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4596,25 +4596,25 @@
         <v>1</v>
       </c>
       <c r="P75" s="37">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="Q75" s="37">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="R75" s="37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S75" s="37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T75" s="37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U75" s="37">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="V75" s="37">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="W75" s="37">
         <v>0</v>
@@ -5247,31 +5247,31 @@
       </c>
       <c r="O88" s="38">
         <f t="shared" si="5"/>
-        <v>0.41625000000000001</v>
+        <v>0.31218750000000001</v>
       </c>
       <c r="P88" s="38">
         <f t="shared" si="5"/>
-        <v>0.41625000000000001</v>
+        <v>0.208125</v>
       </c>
       <c r="Q88" s="38">
         <f t="shared" si="5"/>
-        <v>0.41625000000000001</v>
+        <v>0</v>
       </c>
       <c r="R88" s="38">
         <f t="shared" si="5"/>
-        <v>0.41625000000000001</v>
+        <v>0</v>
       </c>
       <c r="S88" s="38">
         <f t="shared" si="5"/>
-        <v>0.41625000000000001</v>
+        <v>0</v>
       </c>
       <c r="T88" s="38">
         <f t="shared" si="5"/>
-        <v>0.31218750000000001</v>
+        <v>0</v>
       </c>
       <c r="U88" s="38">
         <f t="shared" si="5"/>
-        <v>0.208125</v>
+        <v>0</v>
       </c>
       <c r="V88" s="38">
         <f t="shared" si="5"/>
@@ -22279,7 +22279,7 @@
   </sheetPr>
   <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
@@ -22447,31 +22447,31 @@
       </c>
       <c r="Q2" s="2">
         <f>'Inflation Reduction Act'!O88</f>
-        <v>0.41625000000000001</v>
+        <v>0.31218750000000001</v>
       </c>
       <c r="R2" s="2">
         <f>'Inflation Reduction Act'!P88</f>
-        <v>0.41625000000000001</v>
+        <v>0.208125</v>
       </c>
       <c r="S2" s="2">
         <f>'Inflation Reduction Act'!Q88</f>
-        <v>0.41625000000000001</v>
+        <v>0</v>
       </c>
       <c r="T2">
         <f>'Inflation Reduction Act'!R88</f>
-        <v>0.41625000000000001</v>
+        <v>0</v>
       </c>
       <c r="U2">
         <f>'Inflation Reduction Act'!S88</f>
-        <v>0.41625000000000001</v>
+        <v>0</v>
       </c>
       <c r="V2">
         <f>'Inflation Reduction Act'!T88</f>
-        <v>0.31218750000000001</v>
+        <v>0</v>
       </c>
       <c r="W2">
         <f>'Inflation Reduction Act'!U88</f>
-        <v>0.208125</v>
+        <v>0</v>
       </c>
       <c r="X2">
         <f>'Inflation Reduction Act'!V88</f>

</xml_diff>

<commit_message>
Update to ATB 2024, including reevaluating IRA tax credit expiration year
</commit_message>
<xml_diff>
--- a/InputData/elec/BPSpUGBCD/BAU Subsidy per Unit Grid Battery Capacity Deployed.xlsx
+++ b/InputData/elec/BPSpUGBCD/BAU Subsidy per Unit Grid Battery Capacity Deployed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\BPSpUGBCD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05BA5FBF-5F9B-49F9-9A89-22A14C777523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF88EF0F-F5FD-4CFA-A405-3A4735CD1843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -978,8 +978,8 @@
   </sheetPr>
   <dimension ref="A1:AJ534"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="J77" sqref="J77"/>
+    <sheetView tabSelected="1" topLeftCell="B52" workbookViewId="0">
+      <selection activeCell="Y75" sqref="Y75:AD75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4596,31 +4596,32 @@
         <v>1</v>
       </c>
       <c r="P75" s="37">
+        <v>1</v>
+      </c>
+      <c r="Q75" s="37">
+        <v>1</v>
+      </c>
+      <c r="R75" s="37">
+        <v>1</v>
+      </c>
+      <c r="S75" s="37">
+        <v>1</v>
+      </c>
+      <c r="T75" s="37">
+        <v>1</v>
+      </c>
+      <c r="U75" s="37">
+        <v>1</v>
+      </c>
+      <c r="V75" s="37">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="W75" s="37">
         <v>0.75</v>
       </c>
-      <c r="Q75" s="37">
+      <c r="X75" s="37">
         <v>0.5</v>
-      </c>
-      <c r="R75" s="37">
-        <v>0</v>
-      </c>
-      <c r="S75" s="37">
-        <v>0</v>
-      </c>
-      <c r="T75" s="37">
-        <v>0</v>
-      </c>
-      <c r="U75" s="37">
-        <v>0</v>
-      </c>
-      <c r="V75" s="37">
-        <v>0</v>
-      </c>
-      <c r="W75" s="37">
-        <v>0</v>
-      </c>
-      <c r="X75" s="37">
-        <v>0</v>
       </c>
       <c r="Y75" s="37">
         <v>0</v>
@@ -5247,39 +5248,39 @@
       </c>
       <c r="O88" s="38">
         <f t="shared" si="5"/>
-        <v>0.31218750000000001</v>
+        <v>0.41625000000000001</v>
       </c>
       <c r="P88" s="38">
         <f t="shared" si="5"/>
-        <v>0.208125</v>
+        <v>0.41625000000000001</v>
       </c>
       <c r="Q88" s="38">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.41625000000000001</v>
       </c>
       <c r="R88" s="38">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.41625000000000001</v>
       </c>
       <c r="S88" s="38">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.41625000000000001</v>
       </c>
       <c r="T88" s="38">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.41625000000000001</v>
       </c>
       <c r="U88" s="38">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.41625000000000001</v>
       </c>
       <c r="V88" s="38">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.31218750000000001</v>
       </c>
       <c r="W88" s="31">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.208125</v>
       </c>
       <c r="X88" s="31">
         <f t="shared" si="5"/>
@@ -22279,8 +22280,8 @@
   </sheetPr>
   <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2:AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22447,61 +22448,61 @@
       </c>
       <c r="Q2" s="2">
         <f>'Inflation Reduction Act'!O88</f>
-        <v>0.31218750000000001</v>
+        <v>0.41625000000000001</v>
       </c>
       <c r="R2" s="2">
         <f>'Inflation Reduction Act'!P88</f>
-        <v>0.208125</v>
+        <v>0.41625000000000001</v>
       </c>
       <c r="S2" s="2">
         <f>'Inflation Reduction Act'!Q88</f>
-        <v>0</v>
-      </c>
-      <c r="T2">
+        <v>0.41625000000000001</v>
+      </c>
+      <c r="T2" s="2">
         <f>'Inflation Reduction Act'!R88</f>
-        <v>0</v>
-      </c>
-      <c r="U2">
+        <v>0.41625000000000001</v>
+      </c>
+      <c r="U2" s="2">
         <f>'Inflation Reduction Act'!S88</f>
-        <v>0</v>
-      </c>
-      <c r="V2">
+        <v>0.41625000000000001</v>
+      </c>
+      <c r="V2" s="2">
         <f>'Inflation Reduction Act'!T88</f>
-        <v>0</v>
-      </c>
-      <c r="W2">
+        <v>0.41625000000000001</v>
+      </c>
+      <c r="W2" s="2">
         <f>'Inflation Reduction Act'!U88</f>
-        <v>0</v>
-      </c>
-      <c r="X2">
+        <v>0.41625000000000001</v>
+      </c>
+      <c r="X2" s="2">
         <f>'Inflation Reduction Act'!V88</f>
-        <v>0</v>
-      </c>
-      <c r="Y2">
+        <v>0.31218750000000001</v>
+      </c>
+      <c r="Y2" s="2">
         <f>'Inflation Reduction Act'!W88</f>
-        <v>0</v>
-      </c>
-      <c r="Z2">
+        <v>0.208125</v>
+      </c>
+      <c r="Z2" s="2">
         <f>'Inflation Reduction Act'!X88</f>
         <v>0</v>
       </c>
-      <c r="AA2">
+      <c r="AA2" s="2">
         <f>'Inflation Reduction Act'!Y88</f>
         <v>0</v>
       </c>
-      <c r="AB2">
+      <c r="AB2" s="2">
         <f>'Inflation Reduction Act'!Z88</f>
         <v>0</v>
       </c>
-      <c r="AC2">
+      <c r="AC2" s="2">
         <f>'Inflation Reduction Act'!AA88</f>
         <v>0</v>
       </c>
-      <c r="AD2">
+      <c r="AD2" s="2">
         <f>'Inflation Reduction Act'!AB88</f>
         <v>0</v>
       </c>
-      <c r="AE2">
+      <c r="AE2" s="2">
         <f>'Inflation Reduction Act'!AC88</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Update IRA tax credit expiration year after recent edits
</commit_message>
<xml_diff>
--- a/InputData/elec/BPSpUGBCD/BAU Subsidy per Unit Grid Battery Capacity Deployed.xlsx
+++ b/InputData/elec/BPSpUGBCD/BAU Subsidy per Unit Grid Battery Capacity Deployed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\BPSpUGBCD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF88EF0F-F5FD-4CFA-A405-3A4735CD1843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0232F932-1A86-4F1A-9321-F34C4882B4D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -979,7 +979,7 @@
   <dimension ref="A1:AJ534"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B52" workbookViewId="0">
-      <selection activeCell="Y75" sqref="Y75:AD75"/>
+      <selection activeCell="AC80" sqref="AC80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4618,13 +4618,14 @@
         <v>1</v>
       </c>
       <c r="W75" s="37">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="X75" s="37">
         <v>0.75</v>
       </c>
-      <c r="X75" s="37">
+      <c r="Y75" s="37">
         <v>0.5</v>
-      </c>
-      <c r="Y75" s="37">
-        <v>0</v>
       </c>
       <c r="Z75" s="37">
         <v>0</v>
@@ -4641,7 +4642,7 @@
       <c r="AD75" s="37">
         <v>0</v>
       </c>
-      <c r="AE75" s="5"/>
+      <c r="AE75" s="37"/>
       <c r="AF75" s="5"/>
       <c r="AG75" s="5"/>
       <c r="AH75" s="5"/>
@@ -5276,15 +5277,15 @@
       </c>
       <c r="V88" s="38">
         <f t="shared" si="5"/>
-        <v>0.31218750000000001</v>
+        <v>0.41625000000000001</v>
       </c>
       <c r="W88" s="31">
         <f t="shared" si="5"/>
-        <v>0.208125</v>
+        <v>0.31218750000000001</v>
       </c>
       <c r="X88" s="31">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.208125</v>
       </c>
       <c r="Y88" s="31">
         <f t="shared" si="5"/>
@@ -22476,15 +22477,15 @@
       </c>
       <c r="X2" s="2">
         <f>'Inflation Reduction Act'!V88</f>
-        <v>0.31218750000000001</v>
+        <v>0.41625000000000001</v>
       </c>
       <c r="Y2" s="2">
         <f>'Inflation Reduction Act'!W88</f>
-        <v>0.208125</v>
+        <v>0.31218750000000001</v>
       </c>
       <c r="Z2" s="2">
         <f>'Inflation Reduction Act'!X88</f>
-        <v>0</v>
+        <v>0.208125</v>
       </c>
       <c r="AA2" s="2">
         <f>'Inflation Reduction Act'!Y88</f>

</xml_diff>

<commit_message>
Update IRA tax credit phase out based on latest calibration
</commit_message>
<xml_diff>
--- a/InputData/elec/BPSpUGBCD/BAU Subsidy per Unit Grid Battery Capacity Deployed.xlsx
+++ b/InputData/elec/BPSpUGBCD/BAU Subsidy per Unit Grid Battery Capacity Deployed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\BPSpUGBCD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0232F932-1A86-4F1A-9321-F34C4882B4D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B12ED1-AB15-4AB1-8E79-3D118EA1D7B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -921,7 +921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -978,8 +978,8 @@
   </sheetPr>
   <dimension ref="A1:AJ534"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B52" workbookViewId="0">
-      <selection activeCell="AC80" sqref="AC80"/>
+    <sheetView topLeftCell="B48" workbookViewId="0">
+      <selection activeCell="S79" sqref="S79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4605,27 +4605,25 @@
         <v>1</v>
       </c>
       <c r="S75" s="37">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="T75" s="37">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="U75" s="37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V75" s="37">
-        <f>1</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W75" s="37">
-        <f>1</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X75" s="37">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="Y75" s="37">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="Z75" s="37">
         <v>0</v>
@@ -5261,31 +5259,31 @@
       </c>
       <c r="R88" s="38">
         <f t="shared" si="5"/>
-        <v>0.41625000000000001</v>
+        <v>0.31218750000000001</v>
       </c>
       <c r="S88" s="38">
         <f t="shared" si="5"/>
-        <v>0.41625000000000001</v>
+        <v>0.208125</v>
       </c>
       <c r="T88" s="38">
         <f t="shared" si="5"/>
-        <v>0.41625000000000001</v>
+        <v>0</v>
       </c>
       <c r="U88" s="38">
         <f t="shared" si="5"/>
-        <v>0.41625000000000001</v>
+        <v>0</v>
       </c>
       <c r="V88" s="38">
         <f t="shared" si="5"/>
-        <v>0.41625000000000001</v>
+        <v>0</v>
       </c>
       <c r="W88" s="31">
         <f t="shared" si="5"/>
-        <v>0.31218750000000001</v>
+        <v>0</v>
       </c>
       <c r="X88" s="31">
         <f t="shared" si="5"/>
-        <v>0.208125</v>
+        <v>0</v>
       </c>
       <c r="Y88" s="31">
         <f t="shared" si="5"/>
@@ -22461,31 +22459,31 @@
       </c>
       <c r="T2" s="2">
         <f>'Inflation Reduction Act'!R88</f>
-        <v>0.41625000000000001</v>
+        <v>0.31218750000000001</v>
       </c>
       <c r="U2" s="2">
         <f>'Inflation Reduction Act'!S88</f>
-        <v>0.41625000000000001</v>
+        <v>0.208125</v>
       </c>
       <c r="V2" s="2">
         <f>'Inflation Reduction Act'!T88</f>
-        <v>0.41625000000000001</v>
+        <v>0</v>
       </c>
       <c r="W2" s="2">
         <f>'Inflation Reduction Act'!U88</f>
-        <v>0.41625000000000001</v>
+        <v>0</v>
       </c>
       <c r="X2" s="2">
         <f>'Inflation Reduction Act'!V88</f>
-        <v>0.41625000000000001</v>
+        <v>0</v>
       </c>
       <c r="Y2" s="2">
         <f>'Inflation Reduction Act'!W88</f>
-        <v>0.31218750000000001</v>
+        <v>0</v>
       </c>
       <c r="Z2" s="2">
         <f>'Inflation Reduction Act'!X88</f>
-        <v>0.208125</v>
+        <v>0</v>
       </c>
       <c r="AA2" s="2">
         <f>'Inflation Reduction Act'!Y88</f>

</xml_diff>

<commit_message>
Recalibrate elec sector and remove unused csv file
</commit_message>
<xml_diff>
--- a/InputData/elec/BPSpUGBCD/BAU Subsidy per Unit Grid Battery Capacity Deployed.xlsx
+++ b/InputData/elec/BPSpUGBCD/BAU Subsidy per Unit Grid Battery Capacity Deployed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\BPSpUGBCD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55147085-948F-463F-A843-EC7B4EB4DFC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90B21F7-7DC3-4F30-BB66-A9166A9537C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -257,7 +257,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -925,14 +925,14 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -940,27 +940,27 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -979,10 +979,10 @@
   <dimension ref="A1:AJ534"/>
   <sheetViews>
     <sheetView topLeftCell="B48" workbookViewId="0">
-      <selection activeCell="R75" sqref="R75:S75"/>
+      <selection activeCell="V79" sqref="V79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="94.42578125" style="6" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" style="6" customWidth="1"/>
@@ -995,7 +995,7 @@
     <col min="37" max="16384" width="12.5703125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="12.75">
+    <row r="1" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -1035,7 +1035,7 @@
       <c r="AI1" s="5"/>
       <c r="AJ1" s="5"/>
     </row>
-    <row r="2" spans="1:36" ht="305.25" customHeight="1">
+    <row r="2" spans="1:36" ht="305.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
@@ -1075,7 +1075,7 @@
       <c r="AI2" s="5"/>
       <c r="AJ2" s="5"/>
     </row>
-    <row r="3" spans="1:36" ht="12.75">
+    <row r="3" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -1113,7 +1113,7 @@
       <c r="AI3" s="5"/>
       <c r="AJ3" s="5"/>
     </row>
-    <row r="4" spans="1:36" ht="12.75">
+    <row r="4" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -1153,7 +1153,7 @@
       <c r="AI4" s="8"/>
       <c r="AJ4" s="8"/>
     </row>
-    <row r="5" spans="1:36" ht="12.75">
+    <row r="5" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
@@ -1193,7 +1193,7 @@
       <c r="AI5" s="10"/>
       <c r="AJ5" s="10"/>
     </row>
-    <row r="6" spans="1:36" ht="12.75">
+    <row r="6" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>12</v>
       </c>
@@ -1233,7 +1233,7 @@
       <c r="AI6" s="5"/>
       <c r="AJ6" s="5"/>
     </row>
-    <row r="7" spans="1:36" ht="12.75">
+    <row r="7" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>13</v>
       </c>
@@ -1273,7 +1273,7 @@
       <c r="AI7" s="5"/>
       <c r="AJ7" s="5"/>
     </row>
-    <row r="8" spans="1:36" ht="12.75">
+    <row r="8" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="13"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1311,7 +1311,7 @@
       <c r="AI8" s="5"/>
       <c r="AJ8" s="5"/>
     </row>
-    <row r="9" spans="1:36" ht="12.75">
+    <row r="9" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="13"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -1349,7 +1349,7 @@
       <c r="AI9" s="5"/>
       <c r="AJ9" s="5"/>
     </row>
-    <row r="10" spans="1:36" ht="12.75">
+    <row r="10" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="13"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -1387,7 +1387,7 @@
       <c r="AI10" s="5"/>
       <c r="AJ10" s="5"/>
     </row>
-    <row r="11" spans="1:36" ht="12.75">
+    <row r="11" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="13"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -1425,7 +1425,7 @@
       <c r="AI11" s="5"/>
       <c r="AJ11" s="5"/>
     </row>
-    <row r="12" spans="1:36" ht="12.75">
+    <row r="12" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="13"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1463,7 +1463,7 @@
       <c r="AI12" s="5"/>
       <c r="AJ12" s="5"/>
     </row>
-    <row r="13" spans="1:36" ht="12.75">
+    <row r="13" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -1501,7 +1501,7 @@
       <c r="AI13" s="5"/>
       <c r="AJ13" s="5"/>
     </row>
-    <row r="14" spans="1:36" ht="12.75">
+    <row r="14" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="13"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1539,7 +1539,7 @@
       <c r="AI14" s="5"/>
       <c r="AJ14" s="5"/>
     </row>
-    <row r="15" spans="1:36" ht="12.75">
+    <row r="15" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="13"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -1577,7 +1577,7 @@
       <c r="AI15" s="5"/>
       <c r="AJ15" s="5"/>
     </row>
-    <row r="16" spans="1:36" ht="12.75">
+    <row r="16" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1615,7 +1615,7 @@
       <c r="AI16" s="5"/>
       <c r="AJ16" s="5"/>
     </row>
-    <row r="17" spans="1:36" ht="12.75">
+    <row r="17" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -1653,7 +1653,7 @@
       <c r="AI17" s="5"/>
       <c r="AJ17" s="5"/>
     </row>
-    <row r="18" spans="1:36" ht="12.75">
+    <row r="18" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="13"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1691,7 +1691,7 @@
       <c r="AI18" s="5"/>
       <c r="AJ18" s="5"/>
     </row>
-    <row r="19" spans="1:36" ht="12.75">
+    <row r="19" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="13"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -1729,7 +1729,7 @@
       <c r="AI19" s="5"/>
       <c r="AJ19" s="5"/>
     </row>
-    <row r="20" spans="1:36" ht="12.75">
+    <row r="20" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="13"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -1767,7 +1767,7 @@
       <c r="AI20" s="5"/>
       <c r="AJ20" s="5"/>
     </row>
-    <row r="21" spans="1:36" ht="12.75">
+    <row r="21" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="13"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -1805,7 +1805,7 @@
       <c r="AI21" s="5"/>
       <c r="AJ21" s="5"/>
     </row>
-    <row r="22" spans="1:36" ht="12.75">
+    <row r="22" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="13"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -1843,7 +1843,7 @@
       <c r="AI22" s="5"/>
       <c r="AJ22" s="5"/>
     </row>
-    <row r="23" spans="1:36" ht="12.75">
+    <row r="23" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="13"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1881,7 +1881,7 @@
       <c r="AI23" s="5"/>
       <c r="AJ23" s="5"/>
     </row>
-    <row r="24" spans="1:36" ht="12.75">
+    <row r="24" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="13"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -1919,7 +1919,7 @@
       <c r="AI24" s="5"/>
       <c r="AJ24" s="5"/>
     </row>
-    <row r="25" spans="1:36" ht="12.75">
+    <row r="25" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="13"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -1957,7 +1957,7 @@
       <c r="AI25" s="5"/>
       <c r="AJ25" s="5"/>
     </row>
-    <row r="26" spans="1:36" ht="12.75">
+    <row r="26" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>14</v>
       </c>
@@ -1997,7 +1997,7 @@
       <c r="AI26" s="5"/>
       <c r="AJ26" s="5"/>
     </row>
-    <row r="27" spans="1:36" ht="12.75">
+    <row r="27" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>15</v>
       </c>
@@ -2037,7 +2037,7 @@
       <c r="AI27" s="5"/>
       <c r="AJ27" s="5"/>
     </row>
-    <row r="28" spans="1:36" ht="12.75">
+    <row r="28" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>16</v>
       </c>
@@ -2077,7 +2077,7 @@
       <c r="AI28" s="5"/>
       <c r="AJ28" s="5"/>
     </row>
-    <row r="29" spans="1:36" ht="12.75">
+    <row r="29" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>17</v>
       </c>
@@ -2119,7 +2119,7 @@
       <c r="AI29" s="5"/>
       <c r="AJ29" s="5"/>
     </row>
-    <row r="30" spans="1:36" ht="12.75">
+    <row r="30" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>18</v>
       </c>
@@ -2162,7 +2162,7 @@
       <c r="AI30" s="5"/>
       <c r="AJ30" s="5"/>
     </row>
-    <row r="31" spans="1:36" ht="12.75">
+    <row r="31" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="13"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -2200,7 +2200,7 @@
       <c r="AI31" s="5"/>
       <c r="AJ31" s="5"/>
     </row>
-    <row r="32" spans="1:36" ht="12.75">
+    <row r="32" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="13"/>
       <c r="B32" s="13">
         <v>2022</v>
@@ -2296,7 +2296,7 @@
       <c r="AI32" s="5"/>
       <c r="AJ32" s="5"/>
     </row>
-    <row r="33" spans="1:36" ht="12.75">
+    <row r="33" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="16" t="s">
         <v>19</v>
       </c>
@@ -2394,7 +2394,7 @@
       <c r="AI33" s="5"/>
       <c r="AJ33" s="5"/>
     </row>
-    <row r="34" spans="1:36" ht="12.75">
+    <row r="34" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="s">
         <v>20</v>
       </c>
@@ -2493,7 +2493,7 @@
       <c r="AI34" s="5"/>
       <c r="AJ34" s="5"/>
     </row>
-    <row r="35" spans="1:36" ht="12.75">
+    <row r="35" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="13"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -2531,7 +2531,7 @@
       <c r="AI35" s="5"/>
       <c r="AJ35" s="5"/>
     </row>
-    <row r="36" spans="1:36" ht="12.75">
+    <row r="36" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
         <v>21</v>
       </c>
@@ -2571,7 +2571,7 @@
       <c r="AI36" s="10"/>
       <c r="AJ36" s="10"/>
     </row>
-    <row r="37" spans="1:36" ht="12.75">
+    <row r="37" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>22</v>
       </c>
@@ -2611,7 +2611,7 @@
       <c r="AI37" s="5"/>
       <c r="AJ37" s="5"/>
     </row>
-    <row r="38" spans="1:36" ht="12.75">
+    <row r="38" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
         <v>23</v>
       </c>
@@ -2651,7 +2651,7 @@
       <c r="AI38" s="5"/>
       <c r="AJ38" s="5"/>
     </row>
-    <row r="39" spans="1:36" ht="12.75">
+    <row r="39" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="13"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -2689,7 +2689,7 @@
       <c r="AI39" s="5"/>
       <c r="AJ39" s="5"/>
     </row>
-    <row r="40" spans="1:36" ht="12.75">
+    <row r="40" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="18" t="s">
         <v>24</v>
       </c>
@@ -2733,7 +2733,7 @@
       <c r="AI40" s="5"/>
       <c r="AJ40" s="5"/>
     </row>
-    <row r="41" spans="1:36" ht="12.75">
+    <row r="41" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="20" t="s">
         <v>27</v>
       </c>
@@ -2775,7 +2775,7 @@
       <c r="AI41" s="5"/>
       <c r="AJ41" s="5"/>
     </row>
-    <row r="42" spans="1:36" ht="12.75">
+    <row r="42" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="22" t="s">
         <v>29</v>
       </c>
@@ -2819,7 +2819,7 @@
       <c r="AI42" s="5"/>
       <c r="AJ42" s="5"/>
     </row>
-    <row r="43" spans="1:36" ht="12.75">
+    <row r="43" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="22" t="s">
         <v>30</v>
       </c>
@@ -2863,7 +2863,7 @@
       <c r="AI43" s="5"/>
       <c r="AJ43" s="5"/>
     </row>
-    <row r="44" spans="1:36" ht="12.75">
+    <row r="44" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="22" t="s">
         <v>31</v>
       </c>
@@ -2907,7 +2907,7 @@
       <c r="AI44" s="5"/>
       <c r="AJ44" s="5"/>
     </row>
-    <row r="45" spans="1:36" ht="12.75">
+    <row r="45" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="22" t="s">
         <v>32</v>
       </c>
@@ -2949,7 +2949,7 @@
       <c r="AI45" s="5"/>
       <c r="AJ45" s="5"/>
     </row>
-    <row r="46" spans="1:36" ht="12.75">
+    <row r="46" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="22" t="s">
         <v>33</v>
       </c>
@@ -2991,7 +2991,7 @@
       <c r="AI46" s="5"/>
       <c r="AJ46" s="5"/>
     </row>
-    <row r="47" spans="1:36" ht="12.75">
+    <row r="47" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="22" t="s">
         <v>34</v>
       </c>
@@ -3033,7 +3033,7 @@
       <c r="AI47" s="5"/>
       <c r="AJ47" s="5"/>
     </row>
-    <row r="48" spans="1:36" ht="12.75">
+    <row r="48" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="22" t="s">
         <v>35</v>
       </c>
@@ -3075,7 +3075,7 @@
       <c r="AI48" s="5"/>
       <c r="AJ48" s="5"/>
     </row>
-    <row r="49" spans="1:36" ht="12.75">
+    <row r="49" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="22" t="s">
         <v>36</v>
       </c>
@@ -3117,7 +3117,7 @@
       <c r="AI49" s="5"/>
       <c r="AJ49" s="5"/>
     </row>
-    <row r="50" spans="1:36" ht="12.75">
+    <row r="50" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="22" t="s">
         <v>37</v>
       </c>
@@ -3159,7 +3159,7 @@
       <c r="AI50" s="5"/>
       <c r="AJ50" s="5"/>
     </row>
-    <row r="51" spans="1:36" ht="12.75">
+    <row r="51" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="25" t="s">
         <v>38</v>
       </c>
@@ -3201,7 +3201,7 @@
       <c r="AI51" s="5"/>
       <c r="AJ51" s="5"/>
     </row>
-    <row r="52" spans="1:36" ht="12.75">
+    <row r="52" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="13"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
@@ -3239,7 +3239,7 @@
       <c r="AI52" s="5"/>
       <c r="AJ52" s="5"/>
     </row>
-    <row r="53" spans="1:36" ht="12.75">
+    <row r="53" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
         <v>39</v>
       </c>
@@ -3282,7 +3282,7 @@
       <c r="AI53" s="5"/>
       <c r="AJ53" s="5"/>
     </row>
-    <row r="54" spans="1:36" ht="12.75">
+    <row r="54" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
         <v>40</v>
       </c>
@@ -3325,7 +3325,7 @@
       <c r="AI54" s="5"/>
       <c r="AJ54" s="5"/>
     </row>
-    <row r="55" spans="1:36" ht="12.75">
+    <row r="55" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="5"/>
       <c r="B55" s="24"/>
       <c r="C55" s="5"/>
@@ -3363,7 +3363,7 @@
       <c r="AI55" s="5"/>
       <c r="AJ55" s="5"/>
     </row>
-    <row r="56" spans="1:36" ht="12.75">
+    <row r="56" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="5"/>
       <c r="B56" s="13">
         <v>2022</v>
@@ -3415,7 +3415,7 @@
       <c r="AI56" s="5"/>
       <c r="AJ56" s="5"/>
     </row>
-    <row r="57" spans="1:36" ht="12.75">
+    <row r="57" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
         <v>41</v>
       </c>
@@ -3475,7 +3475,7 @@
       <c r="AI57" s="5"/>
       <c r="AJ57" s="5"/>
     </row>
-    <row r="58" spans="1:36" ht="12.75">
+    <row r="58" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="7"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
@@ -3513,7 +3513,7 @@
       <c r="AI58" s="5"/>
       <c r="AJ58" s="5"/>
     </row>
-    <row r="59" spans="1:36" ht="25.5">
+    <row r="59" spans="1:36" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
         <v>42</v>
       </c>
@@ -3553,7 +3553,7 @@
       <c r="AI59" s="5"/>
       <c r="AJ59" s="5"/>
     </row>
-    <row r="60" spans="1:36" ht="12.75">
+    <row r="60" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="7"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
@@ -3591,7 +3591,7 @@
       <c r="AI60" s="13"/>
       <c r="AJ60" s="13"/>
     </row>
-    <row r="61" spans="1:36" s="27" customFormat="1" ht="12.75">
+    <row r="61" spans="1:36" s="27" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="16"/>
       <c r="B61" s="16">
         <v>2022</v>
@@ -3687,7 +3687,7 @@
       <c r="AI61" s="13"/>
       <c r="AJ61" s="13"/>
     </row>
-    <row r="62" spans="1:36" ht="12.75">
+    <row r="62" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="24" t="s">
         <v>43</v>
       </c>
@@ -3785,7 +3785,7 @@
       <c r="AI62" s="24"/>
       <c r="AJ62" s="24"/>
     </row>
-    <row r="63" spans="1:36" ht="12.75">
+    <row r="63" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="24" t="s">
         <v>44</v>
       </c>
@@ -3912,7 +3912,7 @@
       <c r="AI63" s="24"/>
       <c r="AJ63" s="24"/>
     </row>
-    <row r="64" spans="1:36" ht="12.75">
+    <row r="64" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
         <v>45</v>
       </c>
@@ -4039,7 +4039,7 @@
       <c r="AI64" s="5"/>
       <c r="AJ64" s="5"/>
     </row>
-    <row r="65" spans="1:36" ht="12.75">
+    <row r="65" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="11"/>
       <c r="B65" s="28"/>
       <c r="C65" s="28"/>
@@ -4077,7 +4077,7 @@
       <c r="AI65" s="13"/>
       <c r="AJ65" s="13"/>
     </row>
-    <row r="66" spans="1:36" s="30" customFormat="1" ht="25.5">
+    <row r="66" spans="1:36" s="30" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
         <v>46</v>
       </c>
@@ -4175,7 +4175,7 @@
       <c r="AI66" s="16"/>
       <c r="AJ66" s="16"/>
     </row>
-    <row r="67" spans="1:36" ht="12.75">
+    <row r="67" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="13"/>
       <c r="B67" s="13"/>
       <c r="C67" s="13"/>
@@ -4213,7 +4213,7 @@
       <c r="AI67" s="13"/>
       <c r="AJ67" s="13"/>
     </row>
-    <row r="68" spans="1:36" ht="12.75">
+    <row r="68" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="9" t="s">
         <v>1</v>
       </c>
@@ -4253,7 +4253,7 @@
       <c r="AI68" s="10"/>
       <c r="AJ68" s="10"/>
     </row>
-    <row r="69" spans="1:36" ht="12.75">
+    <row r="69" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="11" t="s">
         <v>47</v>
       </c>
@@ -4293,7 +4293,7 @@
       <c r="AI69" s="5"/>
       <c r="AJ69" s="5"/>
     </row>
-    <row r="70" spans="1:36" ht="12.75">
+    <row r="70" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="11" t="s">
         <v>48</v>
       </c>
@@ -4333,7 +4333,7 @@
       <c r="AI70" s="5"/>
       <c r="AJ70" s="5"/>
     </row>
-    <row r="71" spans="1:36" ht="12.75">
+    <row r="71" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="11" t="s">
         <v>49</v>
       </c>
@@ -4373,7 +4373,7 @@
       <c r="AI71" s="5"/>
       <c r="AJ71" s="5"/>
     </row>
-    <row r="72" spans="1:36" ht="12.75">
+    <row r="72" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="5"/>
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
@@ -4411,7 +4411,7 @@
       <c r="AI72" s="5"/>
       <c r="AJ72" s="5"/>
     </row>
-    <row r="73" spans="1:36" s="36" customFormat="1" ht="12.75">
+    <row r="73" spans="1:36" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="33" t="s">
         <v>55</v>
       </c>
@@ -4451,7 +4451,7 @@
       <c r="AI73" s="35"/>
       <c r="AJ73" s="35"/>
     </row>
-    <row r="74" spans="1:36" ht="12.75">
+    <row r="74" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="31" t="s">
         <v>56</v>
       </c>
@@ -4549,7 +4549,7 @@
       <c r="AI74" s="5"/>
       <c r="AJ74" s="5"/>
     </row>
-    <row r="75" spans="1:36" ht="12.75">
+    <row r="75" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="31" t="s">
         <v>57</v>
       </c>
@@ -4611,13 +4611,13 @@
         <v>1</v>
       </c>
       <c r="U75" s="37">
+        <v>1</v>
+      </c>
+      <c r="V75" s="37">
         <v>0.75</v>
       </c>
-      <c r="V75" s="37">
+      <c r="W75" s="37">
         <v>0.5</v>
-      </c>
-      <c r="W75" s="37">
-        <v>0</v>
       </c>
       <c r="X75" s="37">
         <v>0</v>
@@ -4647,7 +4647,7 @@
       <c r="AI75" s="5"/>
       <c r="AJ75" s="5"/>
     </row>
-    <row r="76" spans="1:36" ht="12.75">
+    <row r="76" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="13"/>
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
@@ -4685,7 +4685,7 @@
       <c r="AI76" s="5"/>
       <c r="AJ76" s="5"/>
     </row>
-    <row r="77" spans="1:36" ht="12.75">
+    <row r="77" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="31" t="s">
         <v>58</v>
       </c>
@@ -4727,7 +4727,7 @@
       <c r="AI77" s="5"/>
       <c r="AJ77" s="5"/>
     </row>
-    <row r="78" spans="1:36" ht="12.75">
+    <row r="78" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="31" t="s">
         <v>59</v>
       </c>
@@ -4769,7 +4769,7 @@
       <c r="AI78" s="5"/>
       <c r="AJ78" s="5"/>
     </row>
-    <row r="79" spans="1:36" ht="12.75">
+    <row r="79" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="31" t="s">
         <v>50</v>
       </c>
@@ -4811,7 +4811,7 @@
       <c r="AI79" s="5"/>
       <c r="AJ79" s="5"/>
     </row>
-    <row r="80" spans="1:36" ht="12.75">
+    <row r="80" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="31" t="s">
         <v>51</v>
       </c>
@@ -4853,7 +4853,7 @@
       <c r="AI80" s="5"/>
       <c r="AJ80" s="5"/>
     </row>
-    <row r="81" spans="1:36" ht="12.75">
+    <row r="81" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="5" t="s">
         <v>52</v>
       </c>
@@ -4895,7 +4895,7 @@
       <c r="AI81" s="5"/>
       <c r="AJ81" s="5"/>
     </row>
-    <row r="82" spans="1:36" ht="12.75">
+    <row r="82" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="31" t="s">
         <v>53</v>
       </c>
@@ -4937,7 +4937,7 @@
       <c r="AI82" s="5"/>
       <c r="AJ82" s="5"/>
     </row>
-    <row r="83" spans="1:36" ht="12.75">
+    <row r="83" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="31" t="s">
         <v>54</v>
       </c>
@@ -4979,7 +4979,7 @@
       <c r="AI83" s="5"/>
       <c r="AJ83" s="5"/>
     </row>
-    <row r="84" spans="1:36" ht="12.75">
+    <row r="84" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="13"/>
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
@@ -5017,7 +5017,7 @@
       <c r="AI84" s="5"/>
       <c r="AJ84" s="5"/>
     </row>
-    <row r="85" spans="1:36" ht="12.75">
+    <row r="85" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="41" t="s">
         <v>60</v>
       </c>
@@ -5057,7 +5057,7 @@
       <c r="AI85" s="5"/>
       <c r="AJ85" s="5"/>
     </row>
-    <row r="86" spans="1:36" ht="12.75">
+    <row r="86" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="31"/>
       <c r="B86" s="31"/>
       <c r="C86" s="31"/>
@@ -5095,7 +5095,7 @@
       <c r="AI86" s="5"/>
       <c r="AJ86" s="5"/>
     </row>
-    <row r="87" spans="1:36" ht="12.75">
+    <row r="87" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="31"/>
       <c r="B87" s="31">
         <v>2023</v>
@@ -5189,7 +5189,7 @@
       <c r="AI87" s="5"/>
       <c r="AJ87" s="5"/>
     </row>
-    <row r="88" spans="1:36" ht="12.75">
+    <row r="88" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="5" t="s">
         <v>61</v>
       </c>
@@ -5267,15 +5267,15 @@
       </c>
       <c r="T88" s="38">
         <f t="shared" si="5"/>
-        <v>0.31218750000000001</v>
+        <v>0.41625000000000001</v>
       </c>
       <c r="U88" s="38">
         <f t="shared" si="5"/>
-        <v>0.208125</v>
+        <v>0.31218750000000001</v>
       </c>
       <c r="V88" s="38">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.208125</v>
       </c>
       <c r="W88" s="31">
         <f t="shared" si="5"/>
@@ -5313,7 +5313,7 @@
       <c r="AI88" s="5"/>
       <c r="AJ88" s="5"/>
     </row>
-    <row r="89" spans="1:36" ht="12.75">
+    <row r="89" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="13"/>
       <c r="B89" s="13"/>
       <c r="C89" s="13"/>
@@ -5351,7 +5351,7 @@
       <c r="AI89" s="13"/>
       <c r="AJ89" s="13"/>
     </row>
-    <row r="90" spans="1:36" ht="12.75">
+    <row r="90" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="5"/>
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
@@ -5389,7 +5389,7 @@
       <c r="AI90" s="5"/>
       <c r="AJ90" s="5"/>
     </row>
-    <row r="91" spans="1:36" ht="12.75">
+    <row r="91" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="5"/>
       <c r="B91" s="5"/>
       <c r="C91" s="5"/>
@@ -5427,7 +5427,7 @@
       <c r="AI91" s="5"/>
       <c r="AJ91" s="5"/>
     </row>
-    <row r="92" spans="1:36" ht="12.75">
+    <row r="92" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="5"/>
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
@@ -5465,7 +5465,7 @@
       <c r="AI92" s="5"/>
       <c r="AJ92" s="5"/>
     </row>
-    <row r="93" spans="1:36" ht="12.75">
+    <row r="93" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="5"/>
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
@@ -5503,7 +5503,7 @@
       <c r="AI93" s="5"/>
       <c r="AJ93" s="5"/>
     </row>
-    <row r="94" spans="1:36" ht="12.75">
+    <row r="94" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="5"/>
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
@@ -5541,7 +5541,7 @@
       <c r="AI94" s="5"/>
       <c r="AJ94" s="5"/>
     </row>
-    <row r="95" spans="1:36" ht="12.75">
+    <row r="95" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="5"/>
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
@@ -5579,7 +5579,7 @@
       <c r="AI95" s="5"/>
       <c r="AJ95" s="5"/>
     </row>
-    <row r="96" spans="1:36" ht="12.75">
+    <row r="96" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="5"/>
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>
@@ -5617,7 +5617,7 @@
       <c r="AI96" s="5"/>
       <c r="AJ96" s="5"/>
     </row>
-    <row r="97" spans="1:36" ht="12.75">
+    <row r="97" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="5"/>
       <c r="B97" s="5"/>
       <c r="C97" s="5"/>
@@ -5655,7 +5655,7 @@
       <c r="AI97" s="5"/>
       <c r="AJ97" s="5"/>
     </row>
-    <row r="98" spans="1:36" ht="12.75">
+    <row r="98" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="5"/>
       <c r="B98" s="5"/>
       <c r="C98" s="5"/>
@@ -5693,7 +5693,7 @@
       <c r="AI98" s="5"/>
       <c r="AJ98" s="5"/>
     </row>
-    <row r="99" spans="1:36" ht="12.75">
+    <row r="99" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="5"/>
       <c r="B99" s="5"/>
       <c r="C99" s="5"/>
@@ -5731,7 +5731,7 @@
       <c r="AI99" s="5"/>
       <c r="AJ99" s="5"/>
     </row>
-    <row r="100" spans="1:36" ht="12.75">
+    <row r="100" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="5"/>
       <c r="B100" s="5"/>
       <c r="C100" s="5"/>
@@ -5769,7 +5769,7 @@
       <c r="AI100" s="5"/>
       <c r="AJ100" s="5"/>
     </row>
-    <row r="101" spans="1:36" ht="12.75">
+    <row r="101" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" s="5"/>
       <c r="B101" s="5"/>
       <c r="C101" s="5"/>
@@ -5807,7 +5807,7 @@
       <c r="AI101" s="5"/>
       <c r="AJ101" s="5"/>
     </row>
-    <row r="102" spans="1:36" ht="12.75">
+    <row r="102" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="5"/>
       <c r="B102" s="5"/>
       <c r="C102" s="5"/>
@@ -5845,7 +5845,7 @@
       <c r="AI102" s="5"/>
       <c r="AJ102" s="5"/>
     </row>
-    <row r="103" spans="1:36" ht="12.75">
+    <row r="103" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="5"/>
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
@@ -5883,7 +5883,7 @@
       <c r="AI103" s="5"/>
       <c r="AJ103" s="5"/>
     </row>
-    <row r="104" spans="1:36" ht="12.75">
+    <row r="104" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" s="5"/>
       <c r="B104" s="5"/>
       <c r="C104" s="5"/>
@@ -5921,7 +5921,7 @@
       <c r="AI104" s="5"/>
       <c r="AJ104" s="5"/>
     </row>
-    <row r="105" spans="1:36" ht="12.75">
+    <row r="105" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="5"/>
       <c r="B105" s="5"/>
       <c r="C105" s="5"/>
@@ -5959,7 +5959,7 @@
       <c r="AI105" s="5"/>
       <c r="AJ105" s="5"/>
     </row>
-    <row r="106" spans="1:36" ht="12.75">
+    <row r="106" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A106" s="5"/>
       <c r="B106" s="5"/>
       <c r="C106" s="5"/>
@@ -5997,7 +5997,7 @@
       <c r="AI106" s="5"/>
       <c r="AJ106" s="5"/>
     </row>
-    <row r="107" spans="1:36" ht="12.75">
+    <row r="107" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" s="5"/>
       <c r="B107" s="5"/>
       <c r="C107" s="5"/>
@@ -6035,7 +6035,7 @@
       <c r="AI107" s="5"/>
       <c r="AJ107" s="5"/>
     </row>
-    <row r="108" spans="1:36" ht="12.75">
+    <row r="108" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="5"/>
       <c r="B108" s="5"/>
       <c r="C108" s="5"/>
@@ -6073,7 +6073,7 @@
       <c r="AI108" s="5"/>
       <c r="AJ108" s="5"/>
     </row>
-    <row r="109" spans="1:36" ht="12.75">
+    <row r="109" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A109" s="5"/>
       <c r="B109" s="5"/>
       <c r="C109" s="5"/>
@@ -6111,7 +6111,7 @@
       <c r="AI109" s="5"/>
       <c r="AJ109" s="5"/>
     </row>
-    <row r="110" spans="1:36" ht="12.75">
+    <row r="110" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A110" s="5"/>
       <c r="B110" s="5"/>
       <c r="C110" s="5"/>
@@ -6149,7 +6149,7 @@
       <c r="AI110" s="5"/>
       <c r="AJ110" s="5"/>
     </row>
-    <row r="111" spans="1:36" ht="12.75">
+    <row r="111" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A111" s="5"/>
       <c r="B111" s="5"/>
       <c r="C111" s="5"/>
@@ -6187,7 +6187,7 @@
       <c r="AI111" s="5"/>
       <c r="AJ111" s="5"/>
     </row>
-    <row r="112" spans="1:36" ht="12.75">
+    <row r="112" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A112" s="5"/>
       <c r="B112" s="5"/>
       <c r="C112" s="5"/>
@@ -6225,7 +6225,7 @@
       <c r="AI112" s="5"/>
       <c r="AJ112" s="5"/>
     </row>
-    <row r="113" spans="1:36" ht="12.75">
+    <row r="113" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A113" s="5"/>
       <c r="B113" s="5"/>
       <c r="C113" s="5"/>
@@ -6263,7 +6263,7 @@
       <c r="AI113" s="5"/>
       <c r="AJ113" s="5"/>
     </row>
-    <row r="114" spans="1:36" ht="12.75">
+    <row r="114" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A114" s="5"/>
       <c r="B114" s="5"/>
       <c r="C114" s="5"/>
@@ -6301,7 +6301,7 @@
       <c r="AI114" s="5"/>
       <c r="AJ114" s="5"/>
     </row>
-    <row r="115" spans="1:36" ht="12.75">
+    <row r="115" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A115" s="5"/>
       <c r="B115" s="5"/>
       <c r="C115" s="5"/>
@@ -6339,7 +6339,7 @@
       <c r="AI115" s="5"/>
       <c r="AJ115" s="5"/>
     </row>
-    <row r="116" spans="1:36" ht="12.75">
+    <row r="116" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A116" s="5"/>
       <c r="B116" s="5"/>
       <c r="C116" s="5"/>
@@ -6377,7 +6377,7 @@
       <c r="AI116" s="5"/>
       <c r="AJ116" s="5"/>
     </row>
-    <row r="117" spans="1:36" ht="12.75">
+    <row r="117" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A117" s="5"/>
       <c r="B117" s="5"/>
       <c r="C117" s="5"/>
@@ -6415,7 +6415,7 @@
       <c r="AI117" s="5"/>
       <c r="AJ117" s="5"/>
     </row>
-    <row r="118" spans="1:36" ht="12.75">
+    <row r="118" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A118" s="5"/>
       <c r="B118" s="5"/>
       <c r="C118" s="5"/>
@@ -6453,7 +6453,7 @@
       <c r="AI118" s="5"/>
       <c r="AJ118" s="5"/>
     </row>
-    <row r="119" spans="1:36" ht="12.75">
+    <row r="119" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A119" s="5"/>
       <c r="B119" s="5"/>
       <c r="C119" s="5"/>
@@ -6491,7 +6491,7 @@
       <c r="AI119" s="5"/>
       <c r="AJ119" s="5"/>
     </row>
-    <row r="120" spans="1:36" ht="12.75">
+    <row r="120" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A120" s="5"/>
       <c r="B120" s="5"/>
       <c r="C120" s="5"/>
@@ -6529,7 +6529,7 @@
       <c r="AI120" s="5"/>
       <c r="AJ120" s="5"/>
     </row>
-    <row r="121" spans="1:36" ht="12.75">
+    <row r="121" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A121" s="5"/>
       <c r="B121" s="5"/>
       <c r="C121" s="5"/>
@@ -6567,7 +6567,7 @@
       <c r="AI121" s="5"/>
       <c r="AJ121" s="5"/>
     </row>
-    <row r="122" spans="1:36" ht="12.75">
+    <row r="122" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A122" s="5"/>
       <c r="B122" s="5"/>
       <c r="C122" s="5"/>
@@ -6605,7 +6605,7 @@
       <c r="AI122" s="5"/>
       <c r="AJ122" s="5"/>
     </row>
-    <row r="123" spans="1:36" ht="12.75">
+    <row r="123" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A123" s="5"/>
       <c r="B123" s="5"/>
       <c r="C123" s="5"/>
@@ -6643,7 +6643,7 @@
       <c r="AI123" s="5"/>
       <c r="AJ123" s="5"/>
     </row>
-    <row r="124" spans="1:36" ht="12.75">
+    <row r="124" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A124" s="5"/>
       <c r="B124" s="5"/>
       <c r="C124" s="5"/>
@@ -6681,7 +6681,7 @@
       <c r="AI124" s="5"/>
       <c r="AJ124" s="5"/>
     </row>
-    <row r="125" spans="1:36" ht="12.75">
+    <row r="125" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A125" s="5"/>
       <c r="B125" s="5"/>
       <c r="C125" s="5"/>
@@ -6719,7 +6719,7 @@
       <c r="AI125" s="5"/>
       <c r="AJ125" s="5"/>
     </row>
-    <row r="126" spans="1:36" ht="12.75">
+    <row r="126" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A126" s="5"/>
       <c r="B126" s="5"/>
       <c r="C126" s="5"/>
@@ -6757,7 +6757,7 @@
       <c r="AI126" s="5"/>
       <c r="AJ126" s="5"/>
     </row>
-    <row r="127" spans="1:36" ht="12.75">
+    <row r="127" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A127" s="5"/>
       <c r="B127" s="5"/>
       <c r="C127" s="5"/>
@@ -6795,7 +6795,7 @@
       <c r="AI127" s="5"/>
       <c r="AJ127" s="5"/>
     </row>
-    <row r="128" spans="1:36" ht="12.75">
+    <row r="128" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A128" s="5"/>
       <c r="B128" s="5"/>
       <c r="C128" s="5"/>
@@ -6833,7 +6833,7 @@
       <c r="AI128" s="5"/>
       <c r="AJ128" s="5"/>
     </row>
-    <row r="129" spans="1:36" ht="12.75">
+    <row r="129" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A129" s="5"/>
       <c r="B129" s="5"/>
       <c r="C129" s="5"/>
@@ -6871,7 +6871,7 @@
       <c r="AI129" s="5"/>
       <c r="AJ129" s="5"/>
     </row>
-    <row r="130" spans="1:36" ht="12.75">
+    <row r="130" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A130" s="5"/>
       <c r="B130" s="5"/>
       <c r="C130" s="5"/>
@@ -6909,7 +6909,7 @@
       <c r="AI130" s="5"/>
       <c r="AJ130" s="5"/>
     </row>
-    <row r="131" spans="1:36" ht="12.75">
+    <row r="131" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A131" s="5"/>
       <c r="B131" s="5"/>
       <c r="C131" s="5"/>
@@ -6947,7 +6947,7 @@
       <c r="AI131" s="5"/>
       <c r="AJ131" s="5"/>
     </row>
-    <row r="132" spans="1:36" ht="12.75">
+    <row r="132" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A132" s="5"/>
       <c r="B132" s="5"/>
       <c r="C132" s="5"/>
@@ -6985,7 +6985,7 @@
       <c r="AI132" s="5"/>
       <c r="AJ132" s="5"/>
     </row>
-    <row r="133" spans="1:36" ht="12.75">
+    <row r="133" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A133" s="5"/>
       <c r="B133" s="5"/>
       <c r="C133" s="5"/>
@@ -7023,7 +7023,7 @@
       <c r="AI133" s="5"/>
       <c r="AJ133" s="5"/>
     </row>
-    <row r="134" spans="1:36" ht="12.75">
+    <row r="134" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A134" s="5"/>
       <c r="B134" s="5"/>
       <c r="C134" s="5"/>
@@ -7061,7 +7061,7 @@
       <c r="AI134" s="5"/>
       <c r="AJ134" s="5"/>
     </row>
-    <row r="135" spans="1:36" ht="12.75">
+    <row r="135" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A135" s="5"/>
       <c r="B135" s="5"/>
       <c r="C135" s="5"/>
@@ -7099,7 +7099,7 @@
       <c r="AI135" s="5"/>
       <c r="AJ135" s="5"/>
     </row>
-    <row r="136" spans="1:36" ht="12.75">
+    <row r="136" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A136" s="5"/>
       <c r="B136" s="5"/>
       <c r="C136" s="5"/>
@@ -7137,7 +7137,7 @@
       <c r="AI136" s="5"/>
       <c r="AJ136" s="5"/>
     </row>
-    <row r="137" spans="1:36" ht="12.75">
+    <row r="137" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A137" s="5"/>
       <c r="B137" s="5"/>
       <c r="C137" s="5"/>
@@ -7175,7 +7175,7 @@
       <c r="AI137" s="5"/>
       <c r="AJ137" s="5"/>
     </row>
-    <row r="138" spans="1:36" ht="12.75">
+    <row r="138" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A138" s="5"/>
       <c r="B138" s="5"/>
       <c r="C138" s="5"/>
@@ -7213,7 +7213,7 @@
       <c r="AI138" s="5"/>
       <c r="AJ138" s="5"/>
     </row>
-    <row r="139" spans="1:36" ht="12.75">
+    <row r="139" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A139" s="5"/>
       <c r="B139" s="5"/>
       <c r="C139" s="5"/>
@@ -7251,7 +7251,7 @@
       <c r="AI139" s="5"/>
       <c r="AJ139" s="5"/>
     </row>
-    <row r="140" spans="1:36" ht="12.75">
+    <row r="140" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A140" s="5"/>
       <c r="B140" s="5"/>
       <c r="C140" s="5"/>
@@ -7289,7 +7289,7 @@
       <c r="AI140" s="5"/>
       <c r="AJ140" s="5"/>
     </row>
-    <row r="141" spans="1:36" ht="12.75">
+    <row r="141" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A141" s="5"/>
       <c r="B141" s="5"/>
       <c r="C141" s="5"/>
@@ -7327,7 +7327,7 @@
       <c r="AI141" s="5"/>
       <c r="AJ141" s="5"/>
     </row>
-    <row r="142" spans="1:36" ht="12.75">
+    <row r="142" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A142" s="5"/>
       <c r="B142" s="5"/>
       <c r="C142" s="5"/>
@@ -7365,7 +7365,7 @@
       <c r="AI142" s="5"/>
       <c r="AJ142" s="5"/>
     </row>
-    <row r="143" spans="1:36" ht="12.75">
+    <row r="143" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A143" s="5"/>
       <c r="B143" s="5"/>
       <c r="C143" s="5"/>
@@ -7403,7 +7403,7 @@
       <c r="AI143" s="5"/>
       <c r="AJ143" s="5"/>
     </row>
-    <row r="144" spans="1:36" ht="12.75">
+    <row r="144" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A144" s="5"/>
       <c r="B144" s="5"/>
       <c r="C144" s="5"/>
@@ -7441,7 +7441,7 @@
       <c r="AI144" s="5"/>
       <c r="AJ144" s="5"/>
     </row>
-    <row r="145" spans="1:36" ht="12.75">
+    <row r="145" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A145" s="5"/>
       <c r="B145" s="5"/>
       <c r="C145" s="5"/>
@@ -7479,7 +7479,7 @@
       <c r="AI145" s="5"/>
       <c r="AJ145" s="5"/>
     </row>
-    <row r="146" spans="1:36" ht="12.75">
+    <row r="146" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A146" s="5"/>
       <c r="B146" s="5"/>
       <c r="C146" s="5"/>
@@ -7517,7 +7517,7 @@
       <c r="AI146" s="5"/>
       <c r="AJ146" s="5"/>
     </row>
-    <row r="147" spans="1:36" ht="12.75">
+    <row r="147" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A147" s="5"/>
       <c r="B147" s="5"/>
       <c r="C147" s="5"/>
@@ -7555,7 +7555,7 @@
       <c r="AI147" s="5"/>
       <c r="AJ147" s="5"/>
     </row>
-    <row r="148" spans="1:36" ht="12.75">
+    <row r="148" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A148" s="5"/>
       <c r="B148" s="5"/>
       <c r="C148" s="5"/>
@@ -7593,7 +7593,7 @@
       <c r="AI148" s="5"/>
       <c r="AJ148" s="5"/>
     </row>
-    <row r="149" spans="1:36" ht="12.75">
+    <row r="149" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A149" s="5"/>
       <c r="B149" s="5"/>
       <c r="C149" s="5"/>
@@ -7631,7 +7631,7 @@
       <c r="AI149" s="5"/>
       <c r="AJ149" s="5"/>
     </row>
-    <row r="150" spans="1:36" ht="12.75">
+    <row r="150" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A150" s="5"/>
       <c r="B150" s="5"/>
       <c r="C150" s="5"/>
@@ -7669,7 +7669,7 @@
       <c r="AI150" s="5"/>
       <c r="AJ150" s="5"/>
     </row>
-    <row r="151" spans="1:36" ht="12.75">
+    <row r="151" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A151" s="5"/>
       <c r="B151" s="5"/>
       <c r="C151" s="5"/>
@@ -7707,7 +7707,7 @@
       <c r="AI151" s="5"/>
       <c r="AJ151" s="5"/>
     </row>
-    <row r="152" spans="1:36" ht="12.75">
+    <row r="152" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A152" s="5"/>
       <c r="B152" s="5"/>
       <c r="C152" s="5"/>
@@ -7745,7 +7745,7 @@
       <c r="AI152" s="5"/>
       <c r="AJ152" s="5"/>
     </row>
-    <row r="153" spans="1:36" ht="12.75">
+    <row r="153" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A153" s="5"/>
       <c r="B153" s="5"/>
       <c r="C153" s="5"/>
@@ -7783,7 +7783,7 @@
       <c r="AI153" s="5"/>
       <c r="AJ153" s="5"/>
     </row>
-    <row r="154" spans="1:36" ht="12.75">
+    <row r="154" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A154" s="5"/>
       <c r="B154" s="5"/>
       <c r="C154" s="5"/>
@@ -7821,7 +7821,7 @@
       <c r="AI154" s="5"/>
       <c r="AJ154" s="5"/>
     </row>
-    <row r="155" spans="1:36" ht="12.75">
+    <row r="155" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A155" s="5"/>
       <c r="B155" s="5"/>
       <c r="C155" s="5"/>
@@ -7859,7 +7859,7 @@
       <c r="AI155" s="5"/>
       <c r="AJ155" s="5"/>
     </row>
-    <row r="156" spans="1:36" ht="12.75">
+    <row r="156" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A156" s="5"/>
       <c r="B156" s="5"/>
       <c r="C156" s="5"/>
@@ -7897,7 +7897,7 @@
       <c r="AI156" s="5"/>
       <c r="AJ156" s="5"/>
     </row>
-    <row r="157" spans="1:36" ht="12.75">
+    <row r="157" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A157" s="5"/>
       <c r="B157" s="5"/>
       <c r="C157" s="5"/>
@@ -7935,7 +7935,7 @@
       <c r="AI157" s="5"/>
       <c r="AJ157" s="5"/>
     </row>
-    <row r="158" spans="1:36" ht="12.75">
+    <row r="158" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A158" s="5"/>
       <c r="B158" s="5"/>
       <c r="C158" s="5"/>
@@ -7973,7 +7973,7 @@
       <c r="AI158" s="5"/>
       <c r="AJ158" s="5"/>
     </row>
-    <row r="159" spans="1:36" ht="12.75">
+    <row r="159" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A159" s="5"/>
       <c r="B159" s="5"/>
       <c r="C159" s="5"/>
@@ -8011,7 +8011,7 @@
       <c r="AI159" s="5"/>
       <c r="AJ159" s="5"/>
     </row>
-    <row r="160" spans="1:36" ht="12.75">
+    <row r="160" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A160" s="5"/>
       <c r="B160" s="5"/>
       <c r="C160" s="5"/>
@@ -8049,7 +8049,7 @@
       <c r="AI160" s="5"/>
       <c r="AJ160" s="5"/>
     </row>
-    <row r="161" spans="1:36" ht="12.75">
+    <row r="161" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A161" s="5"/>
       <c r="B161" s="5"/>
       <c r="C161" s="5"/>
@@ -8087,7 +8087,7 @@
       <c r="AI161" s="5"/>
       <c r="AJ161" s="5"/>
     </row>
-    <row r="162" spans="1:36" ht="12.75">
+    <row r="162" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A162" s="5"/>
       <c r="B162" s="5"/>
       <c r="C162" s="5"/>
@@ -8125,7 +8125,7 @@
       <c r="AI162" s="5"/>
       <c r="AJ162" s="5"/>
     </row>
-    <row r="163" spans="1:36" ht="12.75">
+    <row r="163" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A163" s="5"/>
       <c r="B163" s="5"/>
       <c r="C163" s="5"/>
@@ -8163,7 +8163,7 @@
       <c r="AI163" s="5"/>
       <c r="AJ163" s="5"/>
     </row>
-    <row r="164" spans="1:36" ht="12.75">
+    <row r="164" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A164" s="5"/>
       <c r="B164" s="5"/>
       <c r="C164" s="5"/>
@@ -8201,7 +8201,7 @@
       <c r="AI164" s="5"/>
       <c r="AJ164" s="5"/>
     </row>
-    <row r="165" spans="1:36" ht="12.75">
+    <row r="165" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A165" s="5"/>
       <c r="B165" s="5"/>
       <c r="C165" s="5"/>
@@ -8239,7 +8239,7 @@
       <c r="AI165" s="5"/>
       <c r="AJ165" s="5"/>
     </row>
-    <row r="166" spans="1:36" ht="12.75">
+    <row r="166" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A166" s="5"/>
       <c r="B166" s="5"/>
       <c r="C166" s="5"/>
@@ -8277,7 +8277,7 @@
       <c r="AI166" s="5"/>
       <c r="AJ166" s="5"/>
     </row>
-    <row r="167" spans="1:36" ht="12.75">
+    <row r="167" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A167" s="5"/>
       <c r="B167" s="5"/>
       <c r="C167" s="5"/>
@@ -8315,7 +8315,7 @@
       <c r="AI167" s="5"/>
       <c r="AJ167" s="5"/>
     </row>
-    <row r="168" spans="1:36" ht="12.75">
+    <row r="168" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A168" s="5"/>
       <c r="B168" s="5"/>
       <c r="C168" s="5"/>
@@ -8353,7 +8353,7 @@
       <c r="AI168" s="5"/>
       <c r="AJ168" s="5"/>
     </row>
-    <row r="169" spans="1:36" ht="12.75">
+    <row r="169" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A169" s="5"/>
       <c r="B169" s="5"/>
       <c r="C169" s="5"/>
@@ -8391,7 +8391,7 @@
       <c r="AI169" s="5"/>
       <c r="AJ169" s="5"/>
     </row>
-    <row r="170" spans="1:36" ht="12.75">
+    <row r="170" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A170" s="5"/>
       <c r="B170" s="5"/>
       <c r="C170" s="5"/>
@@ -8429,7 +8429,7 @@
       <c r="AI170" s="5"/>
       <c r="AJ170" s="5"/>
     </row>
-    <row r="171" spans="1:36" ht="12.75">
+    <row r="171" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A171" s="5"/>
       <c r="B171" s="5"/>
       <c r="C171" s="5"/>
@@ -8467,7 +8467,7 @@
       <c r="AI171" s="5"/>
       <c r="AJ171" s="5"/>
     </row>
-    <row r="172" spans="1:36" ht="12.75">
+    <row r="172" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A172" s="5"/>
       <c r="B172" s="5"/>
       <c r="C172" s="5"/>
@@ -8505,7 +8505,7 @@
       <c r="AI172" s="5"/>
       <c r="AJ172" s="5"/>
     </row>
-    <row r="173" spans="1:36" ht="12.75">
+    <row r="173" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A173" s="5"/>
       <c r="B173" s="5"/>
       <c r="C173" s="5"/>
@@ -8543,7 +8543,7 @@
       <c r="AI173" s="5"/>
       <c r="AJ173" s="5"/>
     </row>
-    <row r="174" spans="1:36" ht="12.75">
+    <row r="174" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A174" s="5"/>
       <c r="B174" s="5"/>
       <c r="C174" s="5"/>
@@ -8581,7 +8581,7 @@
       <c r="AI174" s="5"/>
       <c r="AJ174" s="5"/>
     </row>
-    <row r="175" spans="1:36" ht="12.75">
+    <row r="175" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A175" s="5"/>
       <c r="B175" s="5"/>
       <c r="C175" s="5"/>
@@ -8619,7 +8619,7 @@
       <c r="AI175" s="5"/>
       <c r="AJ175" s="5"/>
     </row>
-    <row r="176" spans="1:36" ht="12.75">
+    <row r="176" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A176" s="5"/>
       <c r="B176" s="5"/>
       <c r="C176" s="5"/>
@@ -8657,7 +8657,7 @@
       <c r="AI176" s="5"/>
       <c r="AJ176" s="5"/>
     </row>
-    <row r="177" spans="1:36" ht="12.75">
+    <row r="177" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A177" s="5"/>
       <c r="B177" s="5"/>
       <c r="C177" s="5"/>
@@ -8695,7 +8695,7 @@
       <c r="AI177" s="5"/>
       <c r="AJ177" s="5"/>
     </row>
-    <row r="178" spans="1:36" ht="12.75">
+    <row r="178" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A178" s="5"/>
       <c r="B178" s="5"/>
       <c r="C178" s="5"/>
@@ -8733,7 +8733,7 @@
       <c r="AI178" s="5"/>
       <c r="AJ178" s="5"/>
     </row>
-    <row r="179" spans="1:36" ht="12.75">
+    <row r="179" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A179" s="5"/>
       <c r="B179" s="5"/>
       <c r="C179" s="5"/>
@@ -8771,7 +8771,7 @@
       <c r="AI179" s="5"/>
       <c r="AJ179" s="5"/>
     </row>
-    <row r="180" spans="1:36" ht="12.75">
+    <row r="180" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A180" s="5"/>
       <c r="B180" s="5"/>
       <c r="C180" s="5"/>
@@ -8809,7 +8809,7 @@
       <c r="AI180" s="5"/>
       <c r="AJ180" s="5"/>
     </row>
-    <row r="181" spans="1:36" ht="12.75">
+    <row r="181" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A181" s="5"/>
       <c r="B181" s="5"/>
       <c r="C181" s="5"/>
@@ -8847,7 +8847,7 @@
       <c r="AI181" s="5"/>
       <c r="AJ181" s="5"/>
     </row>
-    <row r="182" spans="1:36" ht="12.75">
+    <row r="182" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A182" s="5"/>
       <c r="B182" s="5"/>
       <c r="C182" s="5"/>
@@ -8885,7 +8885,7 @@
       <c r="AI182" s="5"/>
       <c r="AJ182" s="5"/>
     </row>
-    <row r="183" spans="1:36" ht="12.75">
+    <row r="183" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A183" s="5"/>
       <c r="B183" s="5"/>
       <c r="C183" s="5"/>
@@ -8923,7 +8923,7 @@
       <c r="AI183" s="5"/>
       <c r="AJ183" s="5"/>
     </row>
-    <row r="184" spans="1:36" ht="12.75">
+    <row r="184" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A184" s="5"/>
       <c r="B184" s="5"/>
       <c r="C184" s="5"/>
@@ -8961,7 +8961,7 @@
       <c r="AI184" s="5"/>
       <c r="AJ184" s="5"/>
     </row>
-    <row r="185" spans="1:36" ht="12.75">
+    <row r="185" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A185" s="5"/>
       <c r="B185" s="5"/>
       <c r="C185" s="5"/>
@@ -8999,7 +8999,7 @@
       <c r="AI185" s="5"/>
       <c r="AJ185" s="5"/>
     </row>
-    <row r="186" spans="1:36" ht="12.75">
+    <row r="186" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A186" s="5"/>
       <c r="B186" s="5"/>
       <c r="C186" s="5"/>
@@ -9037,7 +9037,7 @@
       <c r="AI186" s="5"/>
       <c r="AJ186" s="5"/>
     </row>
-    <row r="187" spans="1:36" ht="12.75">
+    <row r="187" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A187" s="5"/>
       <c r="B187" s="5"/>
       <c r="C187" s="5"/>
@@ -9075,7 +9075,7 @@
       <c r="AI187" s="5"/>
       <c r="AJ187" s="5"/>
     </row>
-    <row r="188" spans="1:36" ht="12.75">
+    <row r="188" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A188" s="5"/>
       <c r="B188" s="5"/>
       <c r="C188" s="5"/>
@@ -9113,7 +9113,7 @@
       <c r="AI188" s="5"/>
       <c r="AJ188" s="5"/>
     </row>
-    <row r="189" spans="1:36" ht="12.75">
+    <row r="189" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A189" s="5"/>
       <c r="B189" s="5"/>
       <c r="C189" s="5"/>
@@ -9151,7 +9151,7 @@
       <c r="AI189" s="5"/>
       <c r="AJ189" s="5"/>
     </row>
-    <row r="190" spans="1:36" ht="12.75">
+    <row r="190" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A190" s="5"/>
       <c r="B190" s="5"/>
       <c r="C190" s="5"/>
@@ -9189,7 +9189,7 @@
       <c r="AI190" s="5"/>
       <c r="AJ190" s="5"/>
     </row>
-    <row r="191" spans="1:36" ht="12.75">
+    <row r="191" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A191" s="5"/>
       <c r="B191" s="5"/>
       <c r="C191" s="5"/>
@@ -9227,7 +9227,7 @@
       <c r="AI191" s="5"/>
       <c r="AJ191" s="5"/>
     </row>
-    <row r="192" spans="1:36" ht="12.75">
+    <row r="192" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A192" s="5"/>
       <c r="B192" s="5"/>
       <c r="C192" s="5"/>
@@ -9265,7 +9265,7 @@
       <c r="AI192" s="5"/>
       <c r="AJ192" s="5"/>
     </row>
-    <row r="193" spans="1:36" ht="12.75">
+    <row r="193" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A193" s="5"/>
       <c r="B193" s="5"/>
       <c r="C193" s="5"/>
@@ -9303,7 +9303,7 @@
       <c r="AI193" s="5"/>
       <c r="AJ193" s="5"/>
     </row>
-    <row r="194" spans="1:36" ht="12.75">
+    <row r="194" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A194" s="5"/>
       <c r="B194" s="5"/>
       <c r="C194" s="5"/>
@@ -9341,7 +9341,7 @@
       <c r="AI194" s="5"/>
       <c r="AJ194" s="5"/>
     </row>
-    <row r="195" spans="1:36" ht="12.75">
+    <row r="195" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A195" s="5"/>
       <c r="B195" s="5"/>
       <c r="C195" s="5"/>
@@ -9379,7 +9379,7 @@
       <c r="AI195" s="5"/>
       <c r="AJ195" s="5"/>
     </row>
-    <row r="196" spans="1:36" ht="12.75">
+    <row r="196" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A196" s="5"/>
       <c r="B196" s="5"/>
       <c r="C196" s="5"/>
@@ -9417,7 +9417,7 @@
       <c r="AI196" s="5"/>
       <c r="AJ196" s="5"/>
     </row>
-    <row r="197" spans="1:36" ht="12.75">
+    <row r="197" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A197" s="5"/>
       <c r="B197" s="5"/>
       <c r="C197" s="5"/>
@@ -9455,7 +9455,7 @@
       <c r="AI197" s="5"/>
       <c r="AJ197" s="5"/>
     </row>
-    <row r="198" spans="1:36" ht="12.75">
+    <row r="198" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A198" s="5"/>
       <c r="B198" s="5"/>
       <c r="C198" s="5"/>
@@ -9493,7 +9493,7 @@
       <c r="AI198" s="5"/>
       <c r="AJ198" s="5"/>
     </row>
-    <row r="199" spans="1:36" ht="12.75">
+    <row r="199" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A199" s="5"/>
       <c r="B199" s="5"/>
       <c r="C199" s="5"/>
@@ -9531,7 +9531,7 @@
       <c r="AI199" s="5"/>
       <c r="AJ199" s="5"/>
     </row>
-    <row r="200" spans="1:36" ht="12.75">
+    <row r="200" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A200" s="5"/>
       <c r="B200" s="5"/>
       <c r="C200" s="5"/>
@@ -9569,7 +9569,7 @@
       <c r="AI200" s="5"/>
       <c r="AJ200" s="5"/>
     </row>
-    <row r="201" spans="1:36" ht="12.75">
+    <row r="201" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A201" s="5"/>
       <c r="B201" s="5"/>
       <c r="C201" s="5"/>
@@ -9607,7 +9607,7 @@
       <c r="AI201" s="5"/>
       <c r="AJ201" s="5"/>
     </row>
-    <row r="202" spans="1:36" ht="12.75">
+    <row r="202" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A202" s="5"/>
       <c r="B202" s="5"/>
       <c r="C202" s="5"/>
@@ -9645,7 +9645,7 @@
       <c r="AI202" s="5"/>
       <c r="AJ202" s="5"/>
     </row>
-    <row r="203" spans="1:36" ht="12.75">
+    <row r="203" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A203" s="5"/>
       <c r="B203" s="5"/>
       <c r="C203" s="5"/>
@@ -9683,7 +9683,7 @@
       <c r="AI203" s="5"/>
       <c r="AJ203" s="5"/>
     </row>
-    <row r="204" spans="1:36" ht="12.75">
+    <row r="204" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A204" s="5"/>
       <c r="B204" s="5"/>
       <c r="C204" s="5"/>
@@ -9721,7 +9721,7 @@
       <c r="AI204" s="5"/>
       <c r="AJ204" s="5"/>
     </row>
-    <row r="205" spans="1:36" ht="12.75">
+    <row r="205" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A205" s="5"/>
       <c r="B205" s="5"/>
       <c r="C205" s="5"/>
@@ -9759,7 +9759,7 @@
       <c r="AI205" s="5"/>
       <c r="AJ205" s="5"/>
     </row>
-    <row r="206" spans="1:36" ht="12.75">
+    <row r="206" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A206" s="5"/>
       <c r="B206" s="5"/>
       <c r="C206" s="5"/>
@@ -9797,7 +9797,7 @@
       <c r="AI206" s="5"/>
       <c r="AJ206" s="5"/>
     </row>
-    <row r="207" spans="1:36" ht="12.75">
+    <row r="207" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A207" s="5"/>
       <c r="B207" s="5"/>
       <c r="C207" s="5"/>
@@ -9835,7 +9835,7 @@
       <c r="AI207" s="5"/>
       <c r="AJ207" s="5"/>
     </row>
-    <row r="208" spans="1:36" ht="12.75">
+    <row r="208" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A208" s="5"/>
       <c r="B208" s="5"/>
       <c r="C208" s="5"/>
@@ -9873,7 +9873,7 @@
       <c r="AI208" s="5"/>
       <c r="AJ208" s="5"/>
     </row>
-    <row r="209" spans="1:36" ht="12.75">
+    <row r="209" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A209" s="5"/>
       <c r="B209" s="5"/>
       <c r="C209" s="5"/>
@@ -9911,7 +9911,7 @@
       <c r="AI209" s="5"/>
       <c r="AJ209" s="5"/>
     </row>
-    <row r="210" spans="1:36" ht="12.75">
+    <row r="210" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A210" s="5"/>
       <c r="B210" s="5"/>
       <c r="C210" s="5"/>
@@ -9949,7 +9949,7 @@
       <c r="AI210" s="5"/>
       <c r="AJ210" s="5"/>
     </row>
-    <row r="211" spans="1:36" ht="12.75">
+    <row r="211" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A211" s="5"/>
       <c r="B211" s="5"/>
       <c r="C211" s="5"/>
@@ -9987,7 +9987,7 @@
       <c r="AI211" s="5"/>
       <c r="AJ211" s="5"/>
     </row>
-    <row r="212" spans="1:36" ht="12.75">
+    <row r="212" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A212" s="5"/>
       <c r="B212" s="5"/>
       <c r="C212" s="5"/>
@@ -10025,7 +10025,7 @@
       <c r="AI212" s="5"/>
       <c r="AJ212" s="5"/>
     </row>
-    <row r="213" spans="1:36" ht="12.75">
+    <row r="213" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A213" s="5"/>
       <c r="B213" s="5"/>
       <c r="C213" s="5"/>
@@ -10063,7 +10063,7 @@
       <c r="AI213" s="5"/>
       <c r="AJ213" s="5"/>
     </row>
-    <row r="214" spans="1:36" ht="12.75">
+    <row r="214" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A214" s="5"/>
       <c r="B214" s="5"/>
       <c r="C214" s="5"/>
@@ -10101,7 +10101,7 @@
       <c r="AI214" s="5"/>
       <c r="AJ214" s="5"/>
     </row>
-    <row r="215" spans="1:36" ht="12.75">
+    <row r="215" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A215" s="5"/>
       <c r="B215" s="5"/>
       <c r="C215" s="5"/>
@@ -10139,7 +10139,7 @@
       <c r="AI215" s="5"/>
       <c r="AJ215" s="5"/>
     </row>
-    <row r="216" spans="1:36" ht="12.75">
+    <row r="216" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A216" s="5"/>
       <c r="B216" s="5"/>
       <c r="C216" s="5"/>
@@ -10177,7 +10177,7 @@
       <c r="AI216" s="5"/>
       <c r="AJ216" s="5"/>
     </row>
-    <row r="217" spans="1:36" ht="12.75">
+    <row r="217" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A217" s="5"/>
       <c r="B217" s="5"/>
       <c r="C217" s="5"/>
@@ -10215,7 +10215,7 @@
       <c r="AI217" s="5"/>
       <c r="AJ217" s="5"/>
     </row>
-    <row r="218" spans="1:36" ht="12.75">
+    <row r="218" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A218" s="5"/>
       <c r="B218" s="5"/>
       <c r="C218" s="5"/>
@@ -10253,7 +10253,7 @@
       <c r="AI218" s="5"/>
       <c r="AJ218" s="5"/>
     </row>
-    <row r="219" spans="1:36" ht="12.75">
+    <row r="219" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A219" s="5"/>
       <c r="B219" s="5"/>
       <c r="C219" s="5"/>
@@ -10291,7 +10291,7 @@
       <c r="AI219" s="5"/>
       <c r="AJ219" s="5"/>
     </row>
-    <row r="220" spans="1:36" ht="12.75">
+    <row r="220" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A220" s="5"/>
       <c r="B220" s="5"/>
       <c r="C220" s="5"/>
@@ -10329,7 +10329,7 @@
       <c r="AI220" s="5"/>
       <c r="AJ220" s="5"/>
     </row>
-    <row r="221" spans="1:36" ht="12.75">
+    <row r="221" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A221" s="5"/>
       <c r="B221" s="5"/>
       <c r="C221" s="5"/>
@@ -10367,7 +10367,7 @@
       <c r="AI221" s="5"/>
       <c r="AJ221" s="5"/>
     </row>
-    <row r="222" spans="1:36" ht="12.75">
+    <row r="222" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A222" s="5"/>
       <c r="B222" s="5"/>
       <c r="C222" s="5"/>
@@ -10405,7 +10405,7 @@
       <c r="AI222" s="5"/>
       <c r="AJ222" s="5"/>
     </row>
-    <row r="223" spans="1:36" ht="12.75">
+    <row r="223" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A223" s="5"/>
       <c r="B223" s="5"/>
       <c r="C223" s="5"/>
@@ -10443,7 +10443,7 @@
       <c r="AI223" s="5"/>
       <c r="AJ223" s="5"/>
     </row>
-    <row r="224" spans="1:36" ht="12.75">
+    <row r="224" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A224" s="5"/>
       <c r="B224" s="5"/>
       <c r="C224" s="5"/>
@@ -10481,7 +10481,7 @@
       <c r="AI224" s="5"/>
       <c r="AJ224" s="5"/>
     </row>
-    <row r="225" spans="1:36" ht="12.75">
+    <row r="225" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A225" s="5"/>
       <c r="B225" s="5"/>
       <c r="C225" s="5"/>
@@ -10519,7 +10519,7 @@
       <c r="AI225" s="5"/>
       <c r="AJ225" s="5"/>
     </row>
-    <row r="226" spans="1:36" ht="12.75">
+    <row r="226" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A226" s="5"/>
       <c r="B226" s="5"/>
       <c r="C226" s="5"/>
@@ -10557,7 +10557,7 @@
       <c r="AI226" s="5"/>
       <c r="AJ226" s="5"/>
     </row>
-    <row r="227" spans="1:36" ht="12.75">
+    <row r="227" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A227" s="5"/>
       <c r="B227" s="5"/>
       <c r="C227" s="5"/>
@@ -10595,7 +10595,7 @@
       <c r="AI227" s="5"/>
       <c r="AJ227" s="5"/>
     </row>
-    <row r="228" spans="1:36" ht="12.75">
+    <row r="228" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A228" s="5"/>
       <c r="B228" s="5"/>
       <c r="C228" s="5"/>
@@ -10633,7 +10633,7 @@
       <c r="AI228" s="5"/>
       <c r="AJ228" s="5"/>
     </row>
-    <row r="229" spans="1:36" ht="12.75">
+    <row r="229" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A229" s="5"/>
       <c r="B229" s="5"/>
       <c r="C229" s="5"/>
@@ -10671,7 +10671,7 @@
       <c r="AI229" s="5"/>
       <c r="AJ229" s="5"/>
     </row>
-    <row r="230" spans="1:36" ht="12.75">
+    <row r="230" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A230" s="5"/>
       <c r="B230" s="5"/>
       <c r="C230" s="5"/>
@@ -10709,7 +10709,7 @@
       <c r="AI230" s="5"/>
       <c r="AJ230" s="5"/>
     </row>
-    <row r="231" spans="1:36" ht="12.75">
+    <row r="231" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A231" s="5"/>
       <c r="B231" s="5"/>
       <c r="C231" s="5"/>
@@ -10747,7 +10747,7 @@
       <c r="AI231" s="5"/>
       <c r="AJ231" s="5"/>
     </row>
-    <row r="232" spans="1:36" ht="12.75">
+    <row r="232" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A232" s="5"/>
       <c r="B232" s="5"/>
       <c r="C232" s="5"/>
@@ -10785,7 +10785,7 @@
       <c r="AI232" s="5"/>
       <c r="AJ232" s="5"/>
     </row>
-    <row r="233" spans="1:36" ht="12.75">
+    <row r="233" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A233" s="5"/>
       <c r="B233" s="5"/>
       <c r="C233" s="5"/>
@@ -10823,7 +10823,7 @@
       <c r="AI233" s="5"/>
       <c r="AJ233" s="5"/>
     </row>
-    <row r="234" spans="1:36" ht="12.75">
+    <row r="234" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A234" s="5"/>
       <c r="B234" s="5"/>
       <c r="C234" s="5"/>
@@ -10861,7 +10861,7 @@
       <c r="AI234" s="5"/>
       <c r="AJ234" s="5"/>
     </row>
-    <row r="235" spans="1:36" ht="12.75">
+    <row r="235" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A235" s="5"/>
       <c r="B235" s="5"/>
       <c r="C235" s="5"/>
@@ -10899,7 +10899,7 @@
       <c r="AI235" s="5"/>
       <c r="AJ235" s="5"/>
     </row>
-    <row r="236" spans="1:36" ht="12.75">
+    <row r="236" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A236" s="5"/>
       <c r="B236" s="5"/>
       <c r="C236" s="5"/>
@@ -10937,7 +10937,7 @@
       <c r="AI236" s="5"/>
       <c r="AJ236" s="5"/>
     </row>
-    <row r="237" spans="1:36" ht="12.75">
+    <row r="237" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A237" s="5"/>
       <c r="B237" s="5"/>
       <c r="C237" s="5"/>
@@ -10975,7 +10975,7 @@
       <c r="AI237" s="5"/>
       <c r="AJ237" s="5"/>
     </row>
-    <row r="238" spans="1:36" ht="12.75">
+    <row r="238" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A238" s="5"/>
       <c r="B238" s="5"/>
       <c r="C238" s="5"/>
@@ -11013,7 +11013,7 @@
       <c r="AI238" s="5"/>
       <c r="AJ238" s="5"/>
     </row>
-    <row r="239" spans="1:36" ht="12.75">
+    <row r="239" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A239" s="5"/>
       <c r="B239" s="5"/>
       <c r="C239" s="5"/>
@@ -11051,7 +11051,7 @@
       <c r="AI239" s="5"/>
       <c r="AJ239" s="5"/>
     </row>
-    <row r="240" spans="1:36" ht="12.75">
+    <row r="240" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A240" s="5"/>
       <c r="B240" s="5"/>
       <c r="C240" s="5"/>
@@ -11089,7 +11089,7 @@
       <c r="AI240" s="5"/>
       <c r="AJ240" s="5"/>
     </row>
-    <row r="241" spans="1:36" ht="12.75">
+    <row r="241" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A241" s="5"/>
       <c r="B241" s="5"/>
       <c r="C241" s="5"/>
@@ -11127,7 +11127,7 @@
       <c r="AI241" s="5"/>
       <c r="AJ241" s="5"/>
     </row>
-    <row r="242" spans="1:36" ht="12.75">
+    <row r="242" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A242" s="5"/>
       <c r="B242" s="5"/>
       <c r="C242" s="5"/>
@@ -11165,7 +11165,7 @@
       <c r="AI242" s="5"/>
       <c r="AJ242" s="5"/>
     </row>
-    <row r="243" spans="1:36" ht="12.75">
+    <row r="243" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A243" s="5"/>
       <c r="B243" s="5"/>
       <c r="C243" s="5"/>
@@ -11203,7 +11203,7 @@
       <c r="AI243" s="5"/>
       <c r="AJ243" s="5"/>
     </row>
-    <row r="244" spans="1:36" ht="12.75">
+    <row r="244" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A244" s="5"/>
       <c r="B244" s="5"/>
       <c r="C244" s="5"/>
@@ -11241,7 +11241,7 @@
       <c r="AI244" s="5"/>
       <c r="AJ244" s="5"/>
     </row>
-    <row r="245" spans="1:36" ht="12.75">
+    <row r="245" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A245" s="5"/>
       <c r="B245" s="5"/>
       <c r="C245" s="5"/>
@@ -11279,7 +11279,7 @@
       <c r="AI245" s="5"/>
       <c r="AJ245" s="5"/>
     </row>
-    <row r="246" spans="1:36" ht="12.75">
+    <row r="246" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A246" s="5"/>
       <c r="B246" s="5"/>
       <c r="C246" s="5"/>
@@ -11317,7 +11317,7 @@
       <c r="AI246" s="5"/>
       <c r="AJ246" s="5"/>
     </row>
-    <row r="247" spans="1:36" ht="12.75">
+    <row r="247" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A247" s="5"/>
       <c r="B247" s="5"/>
       <c r="C247" s="5"/>
@@ -11355,7 +11355,7 @@
       <c r="AI247" s="5"/>
       <c r="AJ247" s="5"/>
     </row>
-    <row r="248" spans="1:36" ht="12.75">
+    <row r="248" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A248" s="5"/>
       <c r="B248" s="5"/>
       <c r="C248" s="5"/>
@@ -11393,7 +11393,7 @@
       <c r="AI248" s="5"/>
       <c r="AJ248" s="5"/>
     </row>
-    <row r="249" spans="1:36" ht="12.75">
+    <row r="249" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A249" s="5"/>
       <c r="B249" s="5"/>
       <c r="C249" s="5"/>
@@ -11431,7 +11431,7 @@
       <c r="AI249" s="5"/>
       <c r="AJ249" s="5"/>
     </row>
-    <row r="250" spans="1:36" ht="12.75">
+    <row r="250" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A250" s="5"/>
       <c r="B250" s="5"/>
       <c r="C250" s="5"/>
@@ -11469,7 +11469,7 @@
       <c r="AI250" s="5"/>
       <c r="AJ250" s="5"/>
     </row>
-    <row r="251" spans="1:36" ht="12.75">
+    <row r="251" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A251" s="5"/>
       <c r="B251" s="5"/>
       <c r="C251" s="5"/>
@@ -11507,7 +11507,7 @@
       <c r="AI251" s="5"/>
       <c r="AJ251" s="5"/>
     </row>
-    <row r="252" spans="1:36" ht="12.75">
+    <row r="252" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A252" s="5"/>
       <c r="B252" s="5"/>
       <c r="C252" s="5"/>
@@ -11545,7 +11545,7 @@
       <c r="AI252" s="5"/>
       <c r="AJ252" s="5"/>
     </row>
-    <row r="253" spans="1:36" ht="12.75">
+    <row r="253" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A253" s="5"/>
       <c r="B253" s="5"/>
       <c r="C253" s="5"/>
@@ -11583,7 +11583,7 @@
       <c r="AI253" s="5"/>
       <c r="AJ253" s="5"/>
     </row>
-    <row r="254" spans="1:36" ht="12.75">
+    <row r="254" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A254" s="5"/>
       <c r="B254" s="5"/>
       <c r="C254" s="5"/>
@@ -11621,7 +11621,7 @@
       <c r="AI254" s="5"/>
       <c r="AJ254" s="5"/>
     </row>
-    <row r="255" spans="1:36" ht="12.75">
+    <row r="255" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A255" s="5"/>
       <c r="B255" s="5"/>
       <c r="C255" s="5"/>
@@ -11659,7 +11659,7 @@
       <c r="AI255" s="5"/>
       <c r="AJ255" s="5"/>
     </row>
-    <row r="256" spans="1:36" ht="12.75">
+    <row r="256" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A256" s="5"/>
       <c r="B256" s="5"/>
       <c r="C256" s="5"/>
@@ -11697,7 +11697,7 @@
       <c r="AI256" s="5"/>
       <c r="AJ256" s="5"/>
     </row>
-    <row r="257" spans="1:36" ht="12.75">
+    <row r="257" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A257" s="5"/>
       <c r="B257" s="5"/>
       <c r="C257" s="5"/>
@@ -11735,7 +11735,7 @@
       <c r="AI257" s="5"/>
       <c r="AJ257" s="5"/>
     </row>
-    <row r="258" spans="1:36" ht="12.75">
+    <row r="258" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A258" s="5"/>
       <c r="B258" s="5"/>
       <c r="C258" s="5"/>
@@ -11773,7 +11773,7 @@
       <c r="AI258" s="5"/>
       <c r="AJ258" s="5"/>
     </row>
-    <row r="259" spans="1:36" ht="12.75">
+    <row r="259" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A259" s="5"/>
       <c r="B259" s="5"/>
       <c r="C259" s="5"/>
@@ -11811,7 +11811,7 @@
       <c r="AI259" s="5"/>
       <c r="AJ259" s="5"/>
     </row>
-    <row r="260" spans="1:36" ht="12.75">
+    <row r="260" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A260" s="5"/>
       <c r="B260" s="5"/>
       <c r="C260" s="5"/>
@@ -11849,7 +11849,7 @@
       <c r="AI260" s="5"/>
       <c r="AJ260" s="5"/>
     </row>
-    <row r="261" spans="1:36" ht="12.75">
+    <row r="261" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A261" s="5"/>
       <c r="B261" s="5"/>
       <c r="C261" s="5"/>
@@ -11887,7 +11887,7 @@
       <c r="AI261" s="5"/>
       <c r="AJ261" s="5"/>
     </row>
-    <row r="262" spans="1:36" ht="12.75">
+    <row r="262" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A262" s="5"/>
       <c r="B262" s="5"/>
       <c r="C262" s="5"/>
@@ -11925,7 +11925,7 @@
       <c r="AI262" s="5"/>
       <c r="AJ262" s="5"/>
     </row>
-    <row r="263" spans="1:36" ht="12.75">
+    <row r="263" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A263" s="5"/>
       <c r="B263" s="5"/>
       <c r="C263" s="5"/>
@@ -11963,7 +11963,7 @@
       <c r="AI263" s="5"/>
       <c r="AJ263" s="5"/>
     </row>
-    <row r="264" spans="1:36" ht="12.75">
+    <row r="264" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A264" s="5"/>
       <c r="B264" s="5"/>
       <c r="C264" s="5"/>
@@ -12001,7 +12001,7 @@
       <c r="AI264" s="5"/>
       <c r="AJ264" s="5"/>
     </row>
-    <row r="265" spans="1:36" ht="12.75">
+    <row r="265" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A265" s="5"/>
       <c r="B265" s="5"/>
       <c r="C265" s="5"/>
@@ -12039,7 +12039,7 @@
       <c r="AI265" s="5"/>
       <c r="AJ265" s="5"/>
     </row>
-    <row r="266" spans="1:36" ht="12.75">
+    <row r="266" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A266" s="5"/>
       <c r="B266" s="5"/>
       <c r="C266" s="5"/>
@@ -12077,7 +12077,7 @@
       <c r="AI266" s="5"/>
       <c r="AJ266" s="5"/>
     </row>
-    <row r="267" spans="1:36" ht="12.75">
+    <row r="267" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A267" s="5"/>
       <c r="B267" s="5"/>
       <c r="C267" s="5"/>
@@ -12115,7 +12115,7 @@
       <c r="AI267" s="5"/>
       <c r="AJ267" s="5"/>
     </row>
-    <row r="268" spans="1:36" ht="12.75">
+    <row r="268" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A268" s="5"/>
       <c r="B268" s="5"/>
       <c r="C268" s="5"/>
@@ -12153,7 +12153,7 @@
       <c r="AI268" s="5"/>
       <c r="AJ268" s="5"/>
     </row>
-    <row r="269" spans="1:36" ht="12.75">
+    <row r="269" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A269" s="5"/>
       <c r="B269" s="5"/>
       <c r="C269" s="5"/>
@@ -12191,7 +12191,7 @@
       <c r="AI269" s="5"/>
       <c r="AJ269" s="5"/>
     </row>
-    <row r="270" spans="1:36" ht="12.75">
+    <row r="270" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A270" s="5"/>
       <c r="B270" s="5"/>
       <c r="C270" s="5"/>
@@ -12229,7 +12229,7 @@
       <c r="AI270" s="5"/>
       <c r="AJ270" s="5"/>
     </row>
-    <row r="271" spans="1:36" ht="12.75">
+    <row r="271" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A271" s="5"/>
       <c r="B271" s="5"/>
       <c r="C271" s="5"/>
@@ -12267,7 +12267,7 @@
       <c r="AI271" s="5"/>
       <c r="AJ271" s="5"/>
     </row>
-    <row r="272" spans="1:36" ht="12.75">
+    <row r="272" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A272" s="5"/>
       <c r="B272" s="5"/>
       <c r="C272" s="5"/>
@@ -12305,7 +12305,7 @@
       <c r="AI272" s="5"/>
       <c r="AJ272" s="5"/>
     </row>
-    <row r="273" spans="1:36" ht="12.75">
+    <row r="273" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A273" s="5"/>
       <c r="B273" s="5"/>
       <c r="C273" s="5"/>
@@ -12343,7 +12343,7 @@
       <c r="AI273" s="5"/>
       <c r="AJ273" s="5"/>
     </row>
-    <row r="274" spans="1:36" ht="12.75">
+    <row r="274" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A274" s="5"/>
       <c r="B274" s="5"/>
       <c r="C274" s="5"/>
@@ -12381,7 +12381,7 @@
       <c r="AI274" s="5"/>
       <c r="AJ274" s="5"/>
     </row>
-    <row r="275" spans="1:36" ht="12.75">
+    <row r="275" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A275" s="5"/>
       <c r="B275" s="5"/>
       <c r="C275" s="5"/>
@@ -12419,7 +12419,7 @@
       <c r="AI275" s="5"/>
       <c r="AJ275" s="5"/>
     </row>
-    <row r="276" spans="1:36" ht="12.75">
+    <row r="276" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A276" s="5"/>
       <c r="B276" s="5"/>
       <c r="C276" s="5"/>
@@ -12457,7 +12457,7 @@
       <c r="AI276" s="5"/>
       <c r="AJ276" s="5"/>
     </row>
-    <row r="277" spans="1:36" ht="12.75">
+    <row r="277" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A277" s="5"/>
       <c r="B277" s="5"/>
       <c r="C277" s="5"/>
@@ -12495,7 +12495,7 @@
       <c r="AI277" s="5"/>
       <c r="AJ277" s="5"/>
     </row>
-    <row r="278" spans="1:36" ht="12.75">
+    <row r="278" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A278" s="5"/>
       <c r="B278" s="5"/>
       <c r="C278" s="5"/>
@@ -12533,7 +12533,7 @@
       <c r="AI278" s="5"/>
       <c r="AJ278" s="5"/>
     </row>
-    <row r="279" spans="1:36" ht="12.75">
+    <row r="279" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A279" s="5"/>
       <c r="B279" s="5"/>
       <c r="C279" s="5"/>
@@ -12571,7 +12571,7 @@
       <c r="AI279" s="5"/>
       <c r="AJ279" s="5"/>
     </row>
-    <row r="280" spans="1:36" ht="12.75">
+    <row r="280" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A280" s="5"/>
       <c r="B280" s="5"/>
       <c r="C280" s="5"/>
@@ -12609,7 +12609,7 @@
       <c r="AI280" s="5"/>
       <c r="AJ280" s="5"/>
     </row>
-    <row r="281" spans="1:36" ht="12.75">
+    <row r="281" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A281" s="5"/>
       <c r="B281" s="5"/>
       <c r="C281" s="5"/>
@@ -12647,7 +12647,7 @@
       <c r="AI281" s="5"/>
       <c r="AJ281" s="5"/>
     </row>
-    <row r="282" spans="1:36" ht="12.75">
+    <row r="282" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A282" s="5"/>
       <c r="B282" s="5"/>
       <c r="C282" s="5"/>
@@ -12685,7 +12685,7 @@
       <c r="AI282" s="5"/>
       <c r="AJ282" s="5"/>
     </row>
-    <row r="283" spans="1:36" ht="12.75">
+    <row r="283" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A283" s="5"/>
       <c r="B283" s="5"/>
       <c r="C283" s="5"/>
@@ -12723,7 +12723,7 @@
       <c r="AI283" s="5"/>
       <c r="AJ283" s="5"/>
     </row>
-    <row r="284" spans="1:36" ht="12.75">
+    <row r="284" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A284" s="5"/>
       <c r="B284" s="5"/>
       <c r="C284" s="5"/>
@@ -12761,7 +12761,7 @@
       <c r="AI284" s="5"/>
       <c r="AJ284" s="5"/>
     </row>
-    <row r="285" spans="1:36" ht="12.75">
+    <row r="285" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A285" s="5"/>
       <c r="B285" s="5"/>
       <c r="C285" s="5"/>
@@ -12799,7 +12799,7 @@
       <c r="AI285" s="5"/>
       <c r="AJ285" s="5"/>
     </row>
-    <row r="286" spans="1:36" ht="12.75">
+    <row r="286" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A286" s="5"/>
       <c r="B286" s="5"/>
       <c r="C286" s="5"/>
@@ -12837,7 +12837,7 @@
       <c r="AI286" s="5"/>
       <c r="AJ286" s="5"/>
     </row>
-    <row r="287" spans="1:36" ht="12.75">
+    <row r="287" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A287" s="5"/>
       <c r="B287" s="5"/>
       <c r="C287" s="5"/>
@@ -12875,7 +12875,7 @@
       <c r="AI287" s="5"/>
       <c r="AJ287" s="5"/>
     </row>
-    <row r="288" spans="1:36" ht="12.75">
+    <row r="288" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A288" s="5"/>
       <c r="B288" s="5"/>
       <c r="C288" s="5"/>
@@ -12913,7 +12913,7 @@
       <c r="AI288" s="5"/>
       <c r="AJ288" s="5"/>
     </row>
-    <row r="289" spans="1:36" ht="12.75">
+    <row r="289" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A289" s="5"/>
       <c r="B289" s="5"/>
       <c r="C289" s="5"/>
@@ -12951,7 +12951,7 @@
       <c r="AI289" s="5"/>
       <c r="AJ289" s="5"/>
     </row>
-    <row r="290" spans="1:36" ht="12.75">
+    <row r="290" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A290" s="5"/>
       <c r="B290" s="5"/>
       <c r="C290" s="5"/>
@@ -12989,7 +12989,7 @@
       <c r="AI290" s="5"/>
       <c r="AJ290" s="5"/>
     </row>
-    <row r="291" spans="1:36" ht="12.75">
+    <row r="291" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A291" s="5"/>
       <c r="B291" s="5"/>
       <c r="C291" s="5"/>
@@ -13027,7 +13027,7 @@
       <c r="AI291" s="5"/>
       <c r="AJ291" s="5"/>
     </row>
-    <row r="292" spans="1:36" ht="12.75">
+    <row r="292" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A292" s="5"/>
       <c r="B292" s="5"/>
       <c r="C292" s="5"/>
@@ -13065,7 +13065,7 @@
       <c r="AI292" s="5"/>
       <c r="AJ292" s="5"/>
     </row>
-    <row r="293" spans="1:36" ht="12.75">
+    <row r="293" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A293" s="5"/>
       <c r="B293" s="5"/>
       <c r="C293" s="5"/>
@@ -13103,7 +13103,7 @@
       <c r="AI293" s="5"/>
       <c r="AJ293" s="5"/>
     </row>
-    <row r="294" spans="1:36" ht="12.75">
+    <row r="294" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A294" s="5"/>
       <c r="B294" s="5"/>
       <c r="C294" s="5"/>
@@ -13141,7 +13141,7 @@
       <c r="AI294" s="5"/>
       <c r="AJ294" s="5"/>
     </row>
-    <row r="295" spans="1:36" ht="12.75">
+    <row r="295" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A295" s="5"/>
       <c r="B295" s="5"/>
       <c r="C295" s="5"/>
@@ -13179,7 +13179,7 @@
       <c r="AI295" s="5"/>
       <c r="AJ295" s="5"/>
     </row>
-    <row r="296" spans="1:36" ht="12.75">
+    <row r="296" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A296" s="5"/>
       <c r="B296" s="5"/>
       <c r="C296" s="5"/>
@@ -13217,7 +13217,7 @@
       <c r="AI296" s="5"/>
       <c r="AJ296" s="5"/>
     </row>
-    <row r="297" spans="1:36" ht="12.75">
+    <row r="297" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A297" s="5"/>
       <c r="B297" s="5"/>
       <c r="C297" s="5"/>
@@ -13255,7 +13255,7 @@
       <c r="AI297" s="5"/>
       <c r="AJ297" s="5"/>
     </row>
-    <row r="298" spans="1:36" ht="12.75">
+    <row r="298" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A298" s="5"/>
       <c r="B298" s="5"/>
       <c r="C298" s="5"/>
@@ -13293,7 +13293,7 @@
       <c r="AI298" s="5"/>
       <c r="AJ298" s="5"/>
     </row>
-    <row r="299" spans="1:36" ht="12.75">
+    <row r="299" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A299" s="5"/>
       <c r="B299" s="5"/>
       <c r="C299" s="5"/>
@@ -13331,7 +13331,7 @@
       <c r="AI299" s="5"/>
       <c r="AJ299" s="5"/>
     </row>
-    <row r="300" spans="1:36" ht="12.75">
+    <row r="300" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A300" s="5"/>
       <c r="B300" s="5"/>
       <c r="C300" s="5"/>
@@ -13369,7 +13369,7 @@
       <c r="AI300" s="5"/>
       <c r="AJ300" s="5"/>
     </row>
-    <row r="301" spans="1:36" ht="12.75">
+    <row r="301" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A301" s="5"/>
       <c r="B301" s="5"/>
       <c r="C301" s="5"/>
@@ -13407,7 +13407,7 @@
       <c r="AI301" s="5"/>
       <c r="AJ301" s="5"/>
     </row>
-    <row r="302" spans="1:36" ht="12.75">
+    <row r="302" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A302" s="5"/>
       <c r="B302" s="5"/>
       <c r="C302" s="5"/>
@@ -13445,7 +13445,7 @@
       <c r="AI302" s="5"/>
       <c r="AJ302" s="5"/>
     </row>
-    <row r="303" spans="1:36" ht="12.75">
+    <row r="303" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A303" s="5"/>
       <c r="B303" s="5"/>
       <c r="C303" s="5"/>
@@ -13483,7 +13483,7 @@
       <c r="AI303" s="5"/>
       <c r="AJ303" s="5"/>
     </row>
-    <row r="304" spans="1:36" ht="12.75">
+    <row r="304" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A304" s="5"/>
       <c r="B304" s="5"/>
       <c r="C304" s="5"/>
@@ -13521,7 +13521,7 @@
       <c r="AI304" s="5"/>
       <c r="AJ304" s="5"/>
     </row>
-    <row r="305" spans="1:36" ht="12.75">
+    <row r="305" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A305" s="5"/>
       <c r="B305" s="5"/>
       <c r="C305" s="5"/>
@@ -13559,7 +13559,7 @@
       <c r="AI305" s="5"/>
       <c r="AJ305" s="5"/>
     </row>
-    <row r="306" spans="1:36" ht="12.75">
+    <row r="306" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A306" s="5"/>
       <c r="B306" s="5"/>
       <c r="C306" s="5"/>
@@ -13597,7 +13597,7 @@
       <c r="AI306" s="5"/>
       <c r="AJ306" s="5"/>
     </row>
-    <row r="307" spans="1:36" ht="12.75">
+    <row r="307" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A307" s="5"/>
       <c r="B307" s="5"/>
       <c r="C307" s="5"/>
@@ -13635,7 +13635,7 @@
       <c r="AI307" s="5"/>
       <c r="AJ307" s="5"/>
     </row>
-    <row r="308" spans="1:36" ht="12.75">
+    <row r="308" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A308" s="5"/>
       <c r="B308" s="5"/>
       <c r="C308" s="5"/>
@@ -13673,7 +13673,7 @@
       <c r="AI308" s="5"/>
       <c r="AJ308" s="5"/>
     </row>
-    <row r="309" spans="1:36" ht="12.75">
+    <row r="309" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A309" s="5"/>
       <c r="B309" s="5"/>
       <c r="C309" s="5"/>
@@ -13711,7 +13711,7 @@
       <c r="AI309" s="5"/>
       <c r="AJ309" s="5"/>
     </row>
-    <row r="310" spans="1:36" ht="12.75">
+    <row r="310" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A310" s="5"/>
       <c r="B310" s="5"/>
       <c r="C310" s="5"/>
@@ -13749,7 +13749,7 @@
       <c r="AI310" s="5"/>
       <c r="AJ310" s="5"/>
     </row>
-    <row r="311" spans="1:36" ht="12.75">
+    <row r="311" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A311" s="5"/>
       <c r="B311" s="5"/>
       <c r="C311" s="5"/>
@@ -13787,7 +13787,7 @@
       <c r="AI311" s="5"/>
       <c r="AJ311" s="5"/>
     </row>
-    <row r="312" spans="1:36" ht="12.75">
+    <row r="312" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A312" s="5"/>
       <c r="B312" s="5"/>
       <c r="C312" s="5"/>
@@ -13825,7 +13825,7 @@
       <c r="AI312" s="5"/>
       <c r="AJ312" s="5"/>
     </row>
-    <row r="313" spans="1:36" ht="12.75">
+    <row r="313" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A313" s="5"/>
       <c r="B313" s="5"/>
       <c r="C313" s="5"/>
@@ -13863,7 +13863,7 @@
       <c r="AI313" s="5"/>
       <c r="AJ313" s="5"/>
     </row>
-    <row r="314" spans="1:36" ht="12.75">
+    <row r="314" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A314" s="5"/>
       <c r="B314" s="5"/>
       <c r="C314" s="5"/>
@@ -13901,7 +13901,7 @@
       <c r="AI314" s="5"/>
       <c r="AJ314" s="5"/>
     </row>
-    <row r="315" spans="1:36" ht="12.75">
+    <row r="315" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A315" s="5"/>
       <c r="B315" s="5"/>
       <c r="C315" s="5"/>
@@ -13939,7 +13939,7 @@
       <c r="AI315" s="5"/>
       <c r="AJ315" s="5"/>
     </row>
-    <row r="316" spans="1:36" ht="12.75">
+    <row r="316" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A316" s="5"/>
       <c r="B316" s="5"/>
       <c r="C316" s="5"/>
@@ -13977,7 +13977,7 @@
       <c r="AI316" s="5"/>
       <c r="AJ316" s="5"/>
     </row>
-    <row r="317" spans="1:36" ht="12.75">
+    <row r="317" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A317" s="5"/>
       <c r="B317" s="5"/>
       <c r="C317" s="5"/>
@@ -14015,7 +14015,7 @@
       <c r="AI317" s="5"/>
       <c r="AJ317" s="5"/>
     </row>
-    <row r="318" spans="1:36" ht="12.75">
+    <row r="318" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A318" s="5"/>
       <c r="B318" s="5"/>
       <c r="C318" s="5"/>
@@ -14053,7 +14053,7 @@
       <c r="AI318" s="5"/>
       <c r="AJ318" s="5"/>
     </row>
-    <row r="319" spans="1:36" ht="12.75">
+    <row r="319" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A319" s="5"/>
       <c r="B319" s="5"/>
       <c r="C319" s="5"/>
@@ -14091,7 +14091,7 @@
       <c r="AI319" s="5"/>
       <c r="AJ319" s="5"/>
     </row>
-    <row r="320" spans="1:36" ht="12.75">
+    <row r="320" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A320" s="5"/>
       <c r="B320" s="5"/>
       <c r="C320" s="5"/>
@@ -14129,7 +14129,7 @@
       <c r="AI320" s="5"/>
       <c r="AJ320" s="5"/>
     </row>
-    <row r="321" spans="1:36" ht="12.75">
+    <row r="321" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A321" s="5"/>
       <c r="B321" s="5"/>
       <c r="C321" s="5"/>
@@ -14167,7 +14167,7 @@
       <c r="AI321" s="5"/>
       <c r="AJ321" s="5"/>
     </row>
-    <row r="322" spans="1:36" ht="12.75">
+    <row r="322" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A322" s="5"/>
       <c r="B322" s="5"/>
       <c r="C322" s="5"/>
@@ -14205,7 +14205,7 @@
       <c r="AI322" s="5"/>
       <c r="AJ322" s="5"/>
     </row>
-    <row r="323" spans="1:36" ht="12.75">
+    <row r="323" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A323" s="5"/>
       <c r="B323" s="5"/>
       <c r="C323" s="5"/>
@@ -14243,7 +14243,7 @@
       <c r="AI323" s="5"/>
       <c r="AJ323" s="5"/>
     </row>
-    <row r="324" spans="1:36" ht="12.75">
+    <row r="324" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A324" s="5"/>
       <c r="B324" s="5"/>
       <c r="C324" s="5"/>
@@ -14281,7 +14281,7 @@
       <c r="AI324" s="5"/>
       <c r="AJ324" s="5"/>
     </row>
-    <row r="325" spans="1:36" ht="12.75">
+    <row r="325" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A325" s="5"/>
       <c r="B325" s="5"/>
       <c r="C325" s="5"/>
@@ -14319,7 +14319,7 @@
       <c r="AI325" s="5"/>
       <c r="AJ325" s="5"/>
     </row>
-    <row r="326" spans="1:36" ht="12.75">
+    <row r="326" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A326" s="5"/>
       <c r="B326" s="5"/>
       <c r="C326" s="5"/>
@@ -14357,7 +14357,7 @@
       <c r="AI326" s="5"/>
       <c r="AJ326" s="5"/>
     </row>
-    <row r="327" spans="1:36" ht="12.75">
+    <row r="327" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A327" s="5"/>
       <c r="B327" s="5"/>
       <c r="C327" s="5"/>
@@ -14395,7 +14395,7 @@
       <c r="AI327" s="5"/>
       <c r="AJ327" s="5"/>
     </row>
-    <row r="328" spans="1:36" ht="12.75">
+    <row r="328" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A328" s="5"/>
       <c r="B328" s="5"/>
       <c r="C328" s="5"/>
@@ -14433,7 +14433,7 @@
       <c r="AI328" s="5"/>
       <c r="AJ328" s="5"/>
     </row>
-    <row r="329" spans="1:36" ht="12.75">
+    <row r="329" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A329" s="5"/>
       <c r="B329" s="5"/>
       <c r="C329" s="5"/>
@@ -14471,7 +14471,7 @@
       <c r="AI329" s="5"/>
       <c r="AJ329" s="5"/>
     </row>
-    <row r="330" spans="1:36" ht="12.75">
+    <row r="330" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A330" s="5"/>
       <c r="B330" s="5"/>
       <c r="C330" s="5"/>
@@ -14509,7 +14509,7 @@
       <c r="AI330" s="5"/>
       <c r="AJ330" s="5"/>
     </row>
-    <row r="331" spans="1:36" ht="12.75">
+    <row r="331" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A331" s="5"/>
       <c r="B331" s="5"/>
       <c r="C331" s="5"/>
@@ -14547,7 +14547,7 @@
       <c r="AI331" s="5"/>
       <c r="AJ331" s="5"/>
     </row>
-    <row r="332" spans="1:36" ht="12.75">
+    <row r="332" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A332" s="5"/>
       <c r="B332" s="5"/>
       <c r="C332" s="5"/>
@@ -14585,7 +14585,7 @@
       <c r="AI332" s="5"/>
       <c r="AJ332" s="5"/>
     </row>
-    <row r="333" spans="1:36" ht="12.75">
+    <row r="333" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A333" s="5"/>
       <c r="B333" s="5"/>
       <c r="C333" s="5"/>
@@ -14623,7 +14623,7 @@
       <c r="AI333" s="5"/>
       <c r="AJ333" s="5"/>
     </row>
-    <row r="334" spans="1:36" ht="12.75">
+    <row r="334" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A334" s="5"/>
       <c r="B334" s="5"/>
       <c r="C334" s="5"/>
@@ -14661,7 +14661,7 @@
       <c r="AI334" s="5"/>
       <c r="AJ334" s="5"/>
     </row>
-    <row r="335" spans="1:36" ht="12.75">
+    <row r="335" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A335" s="5"/>
       <c r="B335" s="5"/>
       <c r="C335" s="5"/>
@@ -14699,7 +14699,7 @@
       <c r="AI335" s="5"/>
       <c r="AJ335" s="5"/>
     </row>
-    <row r="336" spans="1:36" ht="12.75">
+    <row r="336" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A336" s="5"/>
       <c r="B336" s="5"/>
       <c r="C336" s="5"/>
@@ -14737,7 +14737,7 @@
       <c r="AI336" s="5"/>
       <c r="AJ336" s="5"/>
     </row>
-    <row r="337" spans="1:36" ht="12.75">
+    <row r="337" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A337" s="5"/>
       <c r="B337" s="5"/>
       <c r="C337" s="5"/>
@@ -14775,7 +14775,7 @@
       <c r="AI337" s="5"/>
       <c r="AJ337" s="5"/>
     </row>
-    <row r="338" spans="1:36" ht="12.75">
+    <row r="338" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A338" s="5"/>
       <c r="B338" s="5"/>
       <c r="C338" s="5"/>
@@ -14813,7 +14813,7 @@
       <c r="AI338" s="5"/>
       <c r="AJ338" s="5"/>
     </row>
-    <row r="339" spans="1:36" ht="12.75">
+    <row r="339" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A339" s="5"/>
       <c r="B339" s="5"/>
       <c r="C339" s="5"/>
@@ -14851,7 +14851,7 @@
       <c r="AI339" s="5"/>
       <c r="AJ339" s="5"/>
     </row>
-    <row r="340" spans="1:36" ht="12.75">
+    <row r="340" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A340" s="5"/>
       <c r="B340" s="5"/>
       <c r="C340" s="5"/>
@@ -14889,7 +14889,7 @@
       <c r="AI340" s="5"/>
       <c r="AJ340" s="5"/>
     </row>
-    <row r="341" spans="1:36" ht="12.75">
+    <row r="341" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A341" s="5"/>
       <c r="B341" s="5"/>
       <c r="C341" s="5"/>
@@ -14927,7 +14927,7 @@
       <c r="AI341" s="5"/>
       <c r="AJ341" s="5"/>
     </row>
-    <row r="342" spans="1:36" ht="12.75">
+    <row r="342" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A342" s="5"/>
       <c r="B342" s="5"/>
       <c r="C342" s="5"/>
@@ -14965,7 +14965,7 @@
       <c r="AI342" s="5"/>
       <c r="AJ342" s="5"/>
     </row>
-    <row r="343" spans="1:36" ht="12.75">
+    <row r="343" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A343" s="5"/>
       <c r="B343" s="5"/>
       <c r="C343" s="5"/>
@@ -15003,7 +15003,7 @@
       <c r="AI343" s="5"/>
       <c r="AJ343" s="5"/>
     </row>
-    <row r="344" spans="1:36" ht="12.75">
+    <row r="344" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A344" s="5"/>
       <c r="B344" s="5"/>
       <c r="C344" s="5"/>
@@ -15041,7 +15041,7 @@
       <c r="AI344" s="5"/>
       <c r="AJ344" s="5"/>
     </row>
-    <row r="345" spans="1:36" ht="12.75">
+    <row r="345" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A345" s="5"/>
       <c r="B345" s="5"/>
       <c r="C345" s="5"/>
@@ -15079,7 +15079,7 @@
       <c r="AI345" s="5"/>
       <c r="AJ345" s="5"/>
     </row>
-    <row r="346" spans="1:36" ht="12.75">
+    <row r="346" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A346" s="5"/>
       <c r="B346" s="5"/>
       <c r="C346" s="5"/>
@@ -15117,7 +15117,7 @@
       <c r="AI346" s="5"/>
       <c r="AJ346" s="5"/>
     </row>
-    <row r="347" spans="1:36" ht="12.75">
+    <row r="347" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A347" s="5"/>
       <c r="B347" s="5"/>
       <c r="C347" s="5"/>
@@ -15155,7 +15155,7 @@
       <c r="AI347" s="5"/>
       <c r="AJ347" s="5"/>
     </row>
-    <row r="348" spans="1:36" ht="12.75">
+    <row r="348" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A348" s="5"/>
       <c r="B348" s="5"/>
       <c r="C348" s="5"/>
@@ -15193,7 +15193,7 @@
       <c r="AI348" s="5"/>
       <c r="AJ348" s="5"/>
     </row>
-    <row r="349" spans="1:36" ht="12.75">
+    <row r="349" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A349" s="5"/>
       <c r="B349" s="5"/>
       <c r="C349" s="5"/>
@@ -15231,7 +15231,7 @@
       <c r="AI349" s="5"/>
       <c r="AJ349" s="5"/>
     </row>
-    <row r="350" spans="1:36" ht="12.75">
+    <row r="350" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A350" s="5"/>
       <c r="B350" s="5"/>
       <c r="C350" s="5"/>
@@ -15269,7 +15269,7 @@
       <c r="AI350" s="5"/>
       <c r="AJ350" s="5"/>
     </row>
-    <row r="351" spans="1:36" ht="12.75">
+    <row r="351" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A351" s="5"/>
       <c r="B351" s="5"/>
       <c r="C351" s="5"/>
@@ -15307,7 +15307,7 @@
       <c r="AI351" s="5"/>
       <c r="AJ351" s="5"/>
     </row>
-    <row r="352" spans="1:36" ht="12.75">
+    <row r="352" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A352" s="5"/>
       <c r="B352" s="5"/>
       <c r="C352" s="5"/>
@@ -15345,7 +15345,7 @@
       <c r="AI352" s="5"/>
       <c r="AJ352" s="5"/>
     </row>
-    <row r="353" spans="1:36" ht="12.75">
+    <row r="353" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A353" s="5"/>
       <c r="B353" s="5"/>
       <c r="C353" s="5"/>
@@ -15383,7 +15383,7 @@
       <c r="AI353" s="5"/>
       <c r="AJ353" s="5"/>
     </row>
-    <row r="354" spans="1:36" ht="12.75">
+    <row r="354" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A354" s="5"/>
       <c r="B354" s="5"/>
       <c r="C354" s="5"/>
@@ -15421,7 +15421,7 @@
       <c r="AI354" s="5"/>
       <c r="AJ354" s="5"/>
     </row>
-    <row r="355" spans="1:36" ht="12.75">
+    <row r="355" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A355" s="5"/>
       <c r="B355" s="5"/>
       <c r="C355" s="5"/>
@@ -15459,7 +15459,7 @@
       <c r="AI355" s="5"/>
       <c r="AJ355" s="5"/>
     </row>
-    <row r="356" spans="1:36" ht="12.75">
+    <row r="356" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A356" s="5"/>
       <c r="B356" s="5"/>
       <c r="C356" s="5"/>
@@ -15497,7 +15497,7 @@
       <c r="AI356" s="5"/>
       <c r="AJ356" s="5"/>
     </row>
-    <row r="357" spans="1:36" ht="12.75">
+    <row r="357" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A357" s="5"/>
       <c r="B357" s="5"/>
       <c r="C357" s="5"/>
@@ -15535,7 +15535,7 @@
       <c r="AI357" s="5"/>
       <c r="AJ357" s="5"/>
     </row>
-    <row r="358" spans="1:36" ht="12.75">
+    <row r="358" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A358" s="5"/>
       <c r="B358" s="5"/>
       <c r="C358" s="5"/>
@@ -15573,7 +15573,7 @@
       <c r="AI358" s="5"/>
       <c r="AJ358" s="5"/>
     </row>
-    <row r="359" spans="1:36" ht="12.75">
+    <row r="359" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A359" s="5"/>
       <c r="B359" s="5"/>
       <c r="C359" s="5"/>
@@ -15611,7 +15611,7 @@
       <c r="AI359" s="5"/>
       <c r="AJ359" s="5"/>
     </row>
-    <row r="360" spans="1:36" ht="12.75">
+    <row r="360" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A360" s="5"/>
       <c r="B360" s="5"/>
       <c r="C360" s="5"/>
@@ -15649,7 +15649,7 @@
       <c r="AI360" s="5"/>
       <c r="AJ360" s="5"/>
     </row>
-    <row r="361" spans="1:36" ht="12.75">
+    <row r="361" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A361" s="5"/>
       <c r="B361" s="5"/>
       <c r="C361" s="5"/>
@@ -15687,7 +15687,7 @@
       <c r="AI361" s="5"/>
       <c r="AJ361" s="5"/>
     </row>
-    <row r="362" spans="1:36" ht="12.75">
+    <row r="362" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A362" s="5"/>
       <c r="B362" s="5"/>
       <c r="C362" s="5"/>
@@ -15725,7 +15725,7 @@
       <c r="AI362" s="5"/>
       <c r="AJ362" s="5"/>
     </row>
-    <row r="363" spans="1:36" ht="12.75">
+    <row r="363" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A363" s="5"/>
       <c r="B363" s="5"/>
       <c r="C363" s="5"/>
@@ -15763,7 +15763,7 @@
       <c r="AI363" s="5"/>
       <c r="AJ363" s="5"/>
     </row>
-    <row r="364" spans="1:36" ht="12.75">
+    <row r="364" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A364" s="5"/>
       <c r="B364" s="5"/>
       <c r="C364" s="5"/>
@@ -15801,7 +15801,7 @@
       <c r="AI364" s="5"/>
       <c r="AJ364" s="5"/>
     </row>
-    <row r="365" spans="1:36" ht="12.75">
+    <row r="365" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A365" s="5"/>
       <c r="B365" s="5"/>
       <c r="C365" s="5"/>
@@ -15839,7 +15839,7 @@
       <c r="AI365" s="5"/>
       <c r="AJ365" s="5"/>
     </row>
-    <row r="366" spans="1:36" ht="12.75">
+    <row r="366" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A366" s="5"/>
       <c r="B366" s="5"/>
       <c r="C366" s="5"/>
@@ -15877,7 +15877,7 @@
       <c r="AI366" s="5"/>
       <c r="AJ366" s="5"/>
     </row>
-    <row r="367" spans="1:36" ht="12.75">
+    <row r="367" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A367" s="5"/>
       <c r="B367" s="5"/>
       <c r="C367" s="5"/>
@@ -15915,7 +15915,7 @@
       <c r="AI367" s="5"/>
       <c r="AJ367" s="5"/>
     </row>
-    <row r="368" spans="1:36" ht="12.75">
+    <row r="368" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A368" s="5"/>
       <c r="B368" s="5"/>
       <c r="C368" s="5"/>
@@ -15953,7 +15953,7 @@
       <c r="AI368" s="5"/>
       <c r="AJ368" s="5"/>
     </row>
-    <row r="369" spans="1:36" ht="12.75">
+    <row r="369" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A369" s="5"/>
       <c r="B369" s="5"/>
       <c r="C369" s="5"/>
@@ -15991,7 +15991,7 @@
       <c r="AI369" s="5"/>
       <c r="AJ369" s="5"/>
     </row>
-    <row r="370" spans="1:36" ht="12.75">
+    <row r="370" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A370" s="5"/>
       <c r="B370" s="5"/>
       <c r="C370" s="5"/>
@@ -16029,7 +16029,7 @@
       <c r="AI370" s="5"/>
       <c r="AJ370" s="5"/>
     </row>
-    <row r="371" spans="1:36" ht="12.75">
+    <row r="371" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A371" s="5"/>
       <c r="B371" s="5"/>
       <c r="C371" s="5"/>
@@ -16067,7 +16067,7 @@
       <c r="AI371" s="5"/>
       <c r="AJ371" s="5"/>
     </row>
-    <row r="372" spans="1:36" ht="12.75">
+    <row r="372" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A372" s="5"/>
       <c r="B372" s="5"/>
       <c r="C372" s="5"/>
@@ -16105,7 +16105,7 @@
       <c r="AI372" s="5"/>
       <c r="AJ372" s="5"/>
     </row>
-    <row r="373" spans="1:36" ht="12.75">
+    <row r="373" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A373" s="5"/>
       <c r="B373" s="5"/>
       <c r="C373" s="5"/>
@@ -16143,7 +16143,7 @@
       <c r="AI373" s="5"/>
       <c r="AJ373" s="5"/>
     </row>
-    <row r="374" spans="1:36" ht="12.75">
+    <row r="374" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A374" s="5"/>
       <c r="B374" s="5"/>
       <c r="C374" s="5"/>
@@ -16181,7 +16181,7 @@
       <c r="AI374" s="5"/>
       <c r="AJ374" s="5"/>
     </row>
-    <row r="375" spans="1:36" ht="12.75">
+    <row r="375" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A375" s="5"/>
       <c r="B375" s="5"/>
       <c r="C375" s="5"/>
@@ -16219,7 +16219,7 @@
       <c r="AI375" s="5"/>
       <c r="AJ375" s="5"/>
     </row>
-    <row r="376" spans="1:36" ht="12.75">
+    <row r="376" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A376" s="5"/>
       <c r="B376" s="5"/>
       <c r="C376" s="5"/>
@@ -16257,7 +16257,7 @@
       <c r="AI376" s="5"/>
       <c r="AJ376" s="5"/>
     </row>
-    <row r="377" spans="1:36" ht="12.75">
+    <row r="377" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A377" s="5"/>
       <c r="B377" s="5"/>
       <c r="C377" s="5"/>
@@ -16295,7 +16295,7 @@
       <c r="AI377" s="5"/>
       <c r="AJ377" s="5"/>
     </row>
-    <row r="378" spans="1:36" ht="12.75">
+    <row r="378" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A378" s="5"/>
       <c r="B378" s="5"/>
       <c r="C378" s="5"/>
@@ -16333,7 +16333,7 @@
       <c r="AI378" s="5"/>
       <c r="AJ378" s="5"/>
     </row>
-    <row r="379" spans="1:36" ht="12.75">
+    <row r="379" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A379" s="5"/>
       <c r="B379" s="5"/>
       <c r="C379" s="5"/>
@@ -16371,7 +16371,7 @@
       <c r="AI379" s="5"/>
       <c r="AJ379" s="5"/>
     </row>
-    <row r="380" spans="1:36" ht="12.75">
+    <row r="380" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A380" s="5"/>
       <c r="B380" s="5"/>
       <c r="C380" s="5"/>
@@ -16409,7 +16409,7 @@
       <c r="AI380" s="5"/>
       <c r="AJ380" s="5"/>
     </row>
-    <row r="381" spans="1:36" ht="12.75">
+    <row r="381" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A381" s="5"/>
       <c r="B381" s="5"/>
       <c r="C381" s="5"/>
@@ -16447,7 +16447,7 @@
       <c r="AI381" s="5"/>
       <c r="AJ381" s="5"/>
     </row>
-    <row r="382" spans="1:36" ht="12.75">
+    <row r="382" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A382" s="5"/>
       <c r="B382" s="5"/>
       <c r="C382" s="5"/>
@@ -16485,7 +16485,7 @@
       <c r="AI382" s="5"/>
       <c r="AJ382" s="5"/>
     </row>
-    <row r="383" spans="1:36" ht="12.75">
+    <row r="383" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A383" s="5"/>
       <c r="B383" s="5"/>
       <c r="C383" s="5"/>
@@ -16523,7 +16523,7 @@
       <c r="AI383" s="5"/>
       <c r="AJ383" s="5"/>
     </row>
-    <row r="384" spans="1:36" ht="12.75">
+    <row r="384" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A384" s="5"/>
       <c r="B384" s="5"/>
       <c r="C384" s="5"/>
@@ -16561,7 +16561,7 @@
       <c r="AI384" s="5"/>
       <c r="AJ384" s="5"/>
     </row>
-    <row r="385" spans="1:36" ht="12.75">
+    <row r="385" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A385" s="5"/>
       <c r="B385" s="5"/>
       <c r="C385" s="5"/>
@@ -16599,7 +16599,7 @@
       <c r="AI385" s="5"/>
       <c r="AJ385" s="5"/>
     </row>
-    <row r="386" spans="1:36" ht="12.75">
+    <row r="386" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A386" s="5"/>
       <c r="B386" s="5"/>
       <c r="C386" s="5"/>
@@ -16637,7 +16637,7 @@
       <c r="AI386" s="5"/>
       <c r="AJ386" s="5"/>
     </row>
-    <row r="387" spans="1:36" ht="12.75">
+    <row r="387" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A387" s="5"/>
       <c r="B387" s="5"/>
       <c r="C387" s="5"/>
@@ -16675,7 +16675,7 @@
       <c r="AI387" s="5"/>
       <c r="AJ387" s="5"/>
     </row>
-    <row r="388" spans="1:36" ht="12.75">
+    <row r="388" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A388" s="5"/>
       <c r="B388" s="5"/>
       <c r="C388" s="5"/>
@@ -16713,7 +16713,7 @@
       <c r="AI388" s="5"/>
       <c r="AJ388" s="5"/>
     </row>
-    <row r="389" spans="1:36" ht="12.75">
+    <row r="389" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A389" s="5"/>
       <c r="B389" s="5"/>
       <c r="C389" s="5"/>
@@ -16751,7 +16751,7 @@
       <c r="AI389" s="5"/>
       <c r="AJ389" s="5"/>
     </row>
-    <row r="390" spans="1:36" ht="12.75">
+    <row r="390" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A390" s="5"/>
       <c r="B390" s="5"/>
       <c r="C390" s="5"/>
@@ -16789,7 +16789,7 @@
       <c r="AI390" s="5"/>
       <c r="AJ390" s="5"/>
     </row>
-    <row r="391" spans="1:36" ht="12.75">
+    <row r="391" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A391" s="5"/>
       <c r="B391" s="5"/>
       <c r="C391" s="5"/>
@@ -16827,7 +16827,7 @@
       <c r="AI391" s="5"/>
       <c r="AJ391" s="5"/>
     </row>
-    <row r="392" spans="1:36" ht="12.75">
+    <row r="392" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A392" s="5"/>
       <c r="B392" s="5"/>
       <c r="C392" s="5"/>
@@ -16865,7 +16865,7 @@
       <c r="AI392" s="5"/>
       <c r="AJ392" s="5"/>
     </row>
-    <row r="393" spans="1:36" ht="12.75">
+    <row r="393" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A393" s="5"/>
       <c r="B393" s="5"/>
       <c r="C393" s="5"/>
@@ -16903,7 +16903,7 @@
       <c r="AI393" s="5"/>
       <c r="AJ393" s="5"/>
     </row>
-    <row r="394" spans="1:36" ht="12.75">
+    <row r="394" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A394" s="5"/>
       <c r="B394" s="5"/>
       <c r="C394" s="5"/>
@@ -16941,7 +16941,7 @@
       <c r="AI394" s="5"/>
       <c r="AJ394" s="5"/>
     </row>
-    <row r="395" spans="1:36" ht="12.75">
+    <row r="395" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A395" s="5"/>
       <c r="B395" s="5"/>
       <c r="C395" s="5"/>
@@ -16979,7 +16979,7 @@
       <c r="AI395" s="5"/>
       <c r="AJ395" s="5"/>
     </row>
-    <row r="396" spans="1:36" ht="12.75">
+    <row r="396" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A396" s="5"/>
       <c r="B396" s="5"/>
       <c r="C396" s="5"/>
@@ -17017,7 +17017,7 @@
       <c r="AI396" s="5"/>
       <c r="AJ396" s="5"/>
     </row>
-    <row r="397" spans="1:36" ht="12.75">
+    <row r="397" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A397" s="5"/>
       <c r="B397" s="5"/>
       <c r="C397" s="5"/>
@@ -17055,7 +17055,7 @@
       <c r="AI397" s="5"/>
       <c r="AJ397" s="5"/>
     </row>
-    <row r="398" spans="1:36" ht="12.75">
+    <row r="398" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A398" s="5"/>
       <c r="B398" s="5"/>
       <c r="C398" s="5"/>
@@ -17093,7 +17093,7 @@
       <c r="AI398" s="5"/>
       <c r="AJ398" s="5"/>
     </row>
-    <row r="399" spans="1:36" ht="12.75">
+    <row r="399" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A399" s="5"/>
       <c r="B399" s="5"/>
       <c r="C399" s="5"/>
@@ -17131,7 +17131,7 @@
       <c r="AI399" s="5"/>
       <c r="AJ399" s="5"/>
     </row>
-    <row r="400" spans="1:36" ht="12.75">
+    <row r="400" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A400" s="5"/>
       <c r="B400" s="5"/>
       <c r="C400" s="5"/>
@@ -17169,7 +17169,7 @@
       <c r="AI400" s="5"/>
       <c r="AJ400" s="5"/>
     </row>
-    <row r="401" spans="1:36" ht="12.75">
+    <row r="401" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A401" s="5"/>
       <c r="B401" s="5"/>
       <c r="C401" s="5"/>
@@ -17207,7 +17207,7 @@
       <c r="AI401" s="5"/>
       <c r="AJ401" s="5"/>
     </row>
-    <row r="402" spans="1:36" ht="12.75">
+    <row r="402" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A402" s="5"/>
       <c r="B402" s="5"/>
       <c r="C402" s="5"/>
@@ -17245,7 +17245,7 @@
       <c r="AI402" s="5"/>
       <c r="AJ402" s="5"/>
     </row>
-    <row r="403" spans="1:36" ht="12.75">
+    <row r="403" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A403" s="5"/>
       <c r="B403" s="5"/>
       <c r="C403" s="5"/>
@@ -17283,7 +17283,7 @@
       <c r="AI403" s="5"/>
       <c r="AJ403" s="5"/>
     </row>
-    <row r="404" spans="1:36" ht="12.75">
+    <row r="404" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A404" s="5"/>
       <c r="B404" s="5"/>
       <c r="C404" s="5"/>
@@ -17321,7 +17321,7 @@
       <c r="AI404" s="5"/>
       <c r="AJ404" s="5"/>
     </row>
-    <row r="405" spans="1:36" ht="12.75">
+    <row r="405" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A405" s="5"/>
       <c r="B405" s="5"/>
       <c r="C405" s="5"/>
@@ -17359,7 +17359,7 @@
       <c r="AI405" s="5"/>
       <c r="AJ405" s="5"/>
     </row>
-    <row r="406" spans="1:36" ht="12.75">
+    <row r="406" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A406" s="5"/>
       <c r="B406" s="5"/>
       <c r="C406" s="5"/>
@@ -17397,7 +17397,7 @@
       <c r="AI406" s="5"/>
       <c r="AJ406" s="5"/>
     </row>
-    <row r="407" spans="1:36" ht="12.75">
+    <row r="407" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A407" s="5"/>
       <c r="B407" s="5"/>
       <c r="C407" s="5"/>
@@ -17435,7 +17435,7 @@
       <c r="AI407" s="5"/>
       <c r="AJ407" s="5"/>
     </row>
-    <row r="408" spans="1:36" ht="12.75">
+    <row r="408" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A408" s="5"/>
       <c r="B408" s="5"/>
       <c r="C408" s="5"/>
@@ -17473,7 +17473,7 @@
       <c r="AI408" s="5"/>
       <c r="AJ408" s="5"/>
     </row>
-    <row r="409" spans="1:36" ht="12.75">
+    <row r="409" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A409" s="5"/>
       <c r="B409" s="5"/>
       <c r="C409" s="5"/>
@@ -17511,7 +17511,7 @@
       <c r="AI409" s="5"/>
       <c r="AJ409" s="5"/>
     </row>
-    <row r="410" spans="1:36" ht="12.75">
+    <row r="410" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A410" s="5"/>
       <c r="B410" s="5"/>
       <c r="C410" s="5"/>
@@ -17549,7 +17549,7 @@
       <c r="AI410" s="5"/>
       <c r="AJ410" s="5"/>
     </row>
-    <row r="411" spans="1:36" ht="12.75">
+    <row r="411" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A411" s="5"/>
       <c r="B411" s="5"/>
       <c r="C411" s="5"/>
@@ -17587,7 +17587,7 @@
       <c r="AI411" s="5"/>
       <c r="AJ411" s="5"/>
     </row>
-    <row r="412" spans="1:36" ht="12.75">
+    <row r="412" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A412" s="5"/>
       <c r="B412" s="5"/>
       <c r="C412" s="5"/>
@@ -17625,7 +17625,7 @@
       <c r="AI412" s="5"/>
       <c r="AJ412" s="5"/>
     </row>
-    <row r="413" spans="1:36" ht="12.75">
+    <row r="413" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A413" s="5"/>
       <c r="B413" s="5"/>
       <c r="C413" s="5"/>
@@ -17663,7 +17663,7 @@
       <c r="AI413" s="5"/>
       <c r="AJ413" s="5"/>
     </row>
-    <row r="414" spans="1:36" ht="12.75">
+    <row r="414" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A414" s="5"/>
       <c r="B414" s="5"/>
       <c r="C414" s="5"/>
@@ -17701,7 +17701,7 @@
       <c r="AI414" s="5"/>
       <c r="AJ414" s="5"/>
     </row>
-    <row r="415" spans="1:36" ht="12.75">
+    <row r="415" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A415" s="5"/>
       <c r="B415" s="5"/>
       <c r="C415" s="5"/>
@@ -17739,7 +17739,7 @@
       <c r="AI415" s="5"/>
       <c r="AJ415" s="5"/>
     </row>
-    <row r="416" spans="1:36" ht="12.75">
+    <row r="416" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A416" s="5"/>
       <c r="B416" s="5"/>
       <c r="C416" s="5"/>
@@ -17777,7 +17777,7 @@
       <c r="AI416" s="5"/>
       <c r="AJ416" s="5"/>
     </row>
-    <row r="417" spans="1:36" ht="12.75">
+    <row r="417" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A417" s="5"/>
       <c r="B417" s="5"/>
       <c r="C417" s="5"/>
@@ -17815,7 +17815,7 @@
       <c r="AI417" s="5"/>
       <c r="AJ417" s="5"/>
     </row>
-    <row r="418" spans="1:36" ht="12.75">
+    <row r="418" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A418" s="5"/>
       <c r="B418" s="5"/>
       <c r="C418" s="5"/>
@@ -17853,7 +17853,7 @@
       <c r="AI418" s="5"/>
       <c r="AJ418" s="5"/>
     </row>
-    <row r="419" spans="1:36" ht="12.75">
+    <row r="419" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A419" s="5"/>
       <c r="B419" s="5"/>
       <c r="C419" s="5"/>
@@ -17891,7 +17891,7 @@
       <c r="AI419" s="5"/>
       <c r="AJ419" s="5"/>
     </row>
-    <row r="420" spans="1:36" ht="12.75">
+    <row r="420" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A420" s="5"/>
       <c r="B420" s="5"/>
       <c r="C420" s="5"/>
@@ -17929,7 +17929,7 @@
       <c r="AI420" s="5"/>
       <c r="AJ420" s="5"/>
     </row>
-    <row r="421" spans="1:36" ht="12.75">
+    <row r="421" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A421" s="5"/>
       <c r="B421" s="5"/>
       <c r="C421" s="5"/>
@@ -17967,7 +17967,7 @@
       <c r="AI421" s="5"/>
       <c r="AJ421" s="5"/>
     </row>
-    <row r="422" spans="1:36" ht="12.75">
+    <row r="422" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A422" s="5"/>
       <c r="B422" s="5"/>
       <c r="C422" s="5"/>
@@ -18005,7 +18005,7 @@
       <c r="AI422" s="5"/>
       <c r="AJ422" s="5"/>
     </row>
-    <row r="423" spans="1:36" ht="12.75">
+    <row r="423" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A423" s="5"/>
       <c r="B423" s="5"/>
       <c r="C423" s="5"/>
@@ -18043,7 +18043,7 @@
       <c r="AI423" s="5"/>
       <c r="AJ423" s="5"/>
     </row>
-    <row r="424" spans="1:36" ht="12.75">
+    <row r="424" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A424" s="5"/>
       <c r="B424" s="5"/>
       <c r="C424" s="5"/>
@@ -18081,7 +18081,7 @@
       <c r="AI424" s="5"/>
       <c r="AJ424" s="5"/>
     </row>
-    <row r="425" spans="1:36" ht="12.75">
+    <row r="425" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A425" s="5"/>
       <c r="B425" s="5"/>
       <c r="C425" s="5"/>
@@ -18119,7 +18119,7 @@
       <c r="AI425" s="5"/>
       <c r="AJ425" s="5"/>
     </row>
-    <row r="426" spans="1:36" ht="12.75">
+    <row r="426" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A426" s="5"/>
       <c r="B426" s="5"/>
       <c r="C426" s="5"/>
@@ -18157,7 +18157,7 @@
       <c r="AI426" s="5"/>
       <c r="AJ426" s="5"/>
     </row>
-    <row r="427" spans="1:36" ht="12.75">
+    <row r="427" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A427" s="5"/>
       <c r="B427" s="5"/>
       <c r="C427" s="5"/>
@@ -18195,7 +18195,7 @@
       <c r="AI427" s="5"/>
       <c r="AJ427" s="5"/>
     </row>
-    <row r="428" spans="1:36" ht="12.75">
+    <row r="428" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A428" s="5"/>
       <c r="B428" s="5"/>
       <c r="C428" s="5"/>
@@ -18233,7 +18233,7 @@
       <c r="AI428" s="5"/>
       <c r="AJ428" s="5"/>
     </row>
-    <row r="429" spans="1:36" ht="12.75">
+    <row r="429" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A429" s="5"/>
       <c r="B429" s="5"/>
       <c r="C429" s="5"/>
@@ -18271,7 +18271,7 @@
       <c r="AI429" s="5"/>
       <c r="AJ429" s="5"/>
     </row>
-    <row r="430" spans="1:36" ht="12.75">
+    <row r="430" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A430" s="5"/>
       <c r="B430" s="5"/>
       <c r="C430" s="5"/>
@@ -18309,7 +18309,7 @@
       <c r="AI430" s="5"/>
       <c r="AJ430" s="5"/>
     </row>
-    <row r="431" spans="1:36" ht="12.75">
+    <row r="431" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A431" s="5"/>
       <c r="B431" s="5"/>
       <c r="C431" s="5"/>
@@ -18347,7 +18347,7 @@
       <c r="AI431" s="5"/>
       <c r="AJ431" s="5"/>
     </row>
-    <row r="432" spans="1:36" ht="12.75">
+    <row r="432" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A432" s="5"/>
       <c r="B432" s="5"/>
       <c r="C432" s="5"/>
@@ -18385,7 +18385,7 @@
       <c r="AI432" s="5"/>
       <c r="AJ432" s="5"/>
     </row>
-    <row r="433" spans="1:36" ht="12.75">
+    <row r="433" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A433" s="5"/>
       <c r="B433" s="5"/>
       <c r="C433" s="5"/>
@@ -18423,7 +18423,7 @@
       <c r="AI433" s="5"/>
       <c r="AJ433" s="5"/>
     </row>
-    <row r="434" spans="1:36" ht="12.75">
+    <row r="434" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A434" s="5"/>
       <c r="B434" s="5"/>
       <c r="C434" s="5"/>
@@ -18461,7 +18461,7 @@
       <c r="AI434" s="5"/>
       <c r="AJ434" s="5"/>
     </row>
-    <row r="435" spans="1:36" ht="12.75">
+    <row r="435" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A435" s="5"/>
       <c r="B435" s="5"/>
       <c r="C435" s="5"/>
@@ -18499,7 +18499,7 @@
       <c r="AI435" s="5"/>
       <c r="AJ435" s="5"/>
     </row>
-    <row r="436" spans="1:36" ht="12.75">
+    <row r="436" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A436" s="5"/>
       <c r="B436" s="5"/>
       <c r="C436" s="5"/>
@@ -18537,7 +18537,7 @@
       <c r="AI436" s="5"/>
       <c r="AJ436" s="5"/>
     </row>
-    <row r="437" spans="1:36" ht="12.75">
+    <row r="437" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A437" s="5"/>
       <c r="B437" s="5"/>
       <c r="C437" s="5"/>
@@ -18575,7 +18575,7 @@
       <c r="AI437" s="5"/>
       <c r="AJ437" s="5"/>
     </row>
-    <row r="438" spans="1:36" ht="12.75">
+    <row r="438" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A438" s="5"/>
       <c r="B438" s="5"/>
       <c r="C438" s="5"/>
@@ -18613,7 +18613,7 @@
       <c r="AI438" s="5"/>
       <c r="AJ438" s="5"/>
     </row>
-    <row r="439" spans="1:36" ht="12.75">
+    <row r="439" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A439" s="5"/>
       <c r="B439" s="5"/>
       <c r="C439" s="5"/>
@@ -18651,7 +18651,7 @@
       <c r="AI439" s="5"/>
       <c r="AJ439" s="5"/>
     </row>
-    <row r="440" spans="1:36" ht="12.75">
+    <row r="440" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A440" s="5"/>
       <c r="B440" s="5"/>
       <c r="C440" s="5"/>
@@ -18689,7 +18689,7 @@
       <c r="AI440" s="5"/>
       <c r="AJ440" s="5"/>
     </row>
-    <row r="441" spans="1:36" ht="12.75">
+    <row r="441" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A441" s="5"/>
       <c r="B441" s="5"/>
       <c r="C441" s="5"/>
@@ -18727,7 +18727,7 @@
       <c r="AI441" s="5"/>
       <c r="AJ441" s="5"/>
     </row>
-    <row r="442" spans="1:36" ht="12.75">
+    <row r="442" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A442" s="5"/>
       <c r="B442" s="5"/>
       <c r="C442" s="5"/>
@@ -18765,7 +18765,7 @@
       <c r="AI442" s="5"/>
       <c r="AJ442" s="5"/>
     </row>
-    <row r="443" spans="1:36" ht="12.75">
+    <row r="443" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A443" s="5"/>
       <c r="B443" s="5"/>
       <c r="C443" s="5"/>
@@ -18803,7 +18803,7 @@
       <c r="AI443" s="5"/>
       <c r="AJ443" s="5"/>
     </row>
-    <row r="444" spans="1:36" ht="12.75">
+    <row r="444" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A444" s="5"/>
       <c r="B444" s="5"/>
       <c r="C444" s="5"/>
@@ -18841,7 +18841,7 @@
       <c r="AI444" s="5"/>
       <c r="AJ444" s="5"/>
     </row>
-    <row r="445" spans="1:36" ht="12.75">
+    <row r="445" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A445" s="5"/>
       <c r="B445" s="5"/>
       <c r="C445" s="5"/>
@@ -18879,7 +18879,7 @@
       <c r="AI445" s="5"/>
       <c r="AJ445" s="5"/>
     </row>
-    <row r="446" spans="1:36" ht="12.75">
+    <row r="446" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A446" s="5"/>
       <c r="B446" s="5"/>
       <c r="C446" s="5"/>
@@ -18917,7 +18917,7 @@
       <c r="AI446" s="5"/>
       <c r="AJ446" s="5"/>
     </row>
-    <row r="447" spans="1:36" ht="12.75">
+    <row r="447" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A447" s="5"/>
       <c r="B447" s="5"/>
       <c r="C447" s="5"/>
@@ -18955,7 +18955,7 @@
       <c r="AI447" s="5"/>
       <c r="AJ447" s="5"/>
     </row>
-    <row r="448" spans="1:36" ht="12.75">
+    <row r="448" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A448" s="5"/>
       <c r="B448" s="5"/>
       <c r="C448" s="5"/>
@@ -18993,7 +18993,7 @@
       <c r="AI448" s="5"/>
       <c r="AJ448" s="5"/>
     </row>
-    <row r="449" spans="1:36" ht="12.75">
+    <row r="449" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A449" s="5"/>
       <c r="B449" s="5"/>
       <c r="C449" s="5"/>
@@ -19031,7 +19031,7 @@
       <c r="AI449" s="5"/>
       <c r="AJ449" s="5"/>
     </row>
-    <row r="450" spans="1:36" ht="12.75">
+    <row r="450" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A450" s="5"/>
       <c r="B450" s="5"/>
       <c r="C450" s="5"/>
@@ -19069,7 +19069,7 @@
       <c r="AI450" s="5"/>
       <c r="AJ450" s="5"/>
     </row>
-    <row r="451" spans="1:36" ht="12.75">
+    <row r="451" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A451" s="5"/>
       <c r="B451" s="5"/>
       <c r="C451" s="5"/>
@@ -19107,7 +19107,7 @@
       <c r="AI451" s="5"/>
       <c r="AJ451" s="5"/>
     </row>
-    <row r="452" spans="1:36" ht="12.75">
+    <row r="452" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A452" s="5"/>
       <c r="B452" s="5"/>
       <c r="C452" s="5"/>
@@ -19145,7 +19145,7 @@
       <c r="AI452" s="5"/>
       <c r="AJ452" s="5"/>
     </row>
-    <row r="453" spans="1:36" ht="12.75">
+    <row r="453" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A453" s="5"/>
       <c r="B453" s="5"/>
       <c r="C453" s="5"/>
@@ -19183,7 +19183,7 @@
       <c r="AI453" s="5"/>
       <c r="AJ453" s="5"/>
     </row>
-    <row r="454" spans="1:36" ht="12.75">
+    <row r="454" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A454" s="5"/>
       <c r="B454" s="5"/>
       <c r="C454" s="5"/>
@@ -19221,7 +19221,7 @@
       <c r="AI454" s="5"/>
       <c r="AJ454" s="5"/>
     </row>
-    <row r="455" spans="1:36" ht="12.75">
+    <row r="455" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A455" s="5"/>
       <c r="B455" s="5"/>
       <c r="C455" s="5"/>
@@ -19259,7 +19259,7 @@
       <c r="AI455" s="5"/>
       <c r="AJ455" s="5"/>
     </row>
-    <row r="456" spans="1:36" ht="12.75">
+    <row r="456" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A456" s="5"/>
       <c r="B456" s="5"/>
       <c r="C456" s="5"/>
@@ -19297,7 +19297,7 @@
       <c r="AI456" s="5"/>
       <c r="AJ456" s="5"/>
     </row>
-    <row r="457" spans="1:36" ht="12.75">
+    <row r="457" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A457" s="5"/>
       <c r="B457" s="5"/>
       <c r="C457" s="5"/>
@@ -19335,7 +19335,7 @@
       <c r="AI457" s="5"/>
       <c r="AJ457" s="5"/>
     </row>
-    <row r="458" spans="1:36" ht="12.75">
+    <row r="458" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A458" s="5"/>
       <c r="B458" s="5"/>
       <c r="C458" s="5"/>
@@ -19373,7 +19373,7 @@
       <c r="AI458" s="5"/>
       <c r="AJ458" s="5"/>
     </row>
-    <row r="459" spans="1:36" ht="12.75">
+    <row r="459" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A459" s="5"/>
       <c r="B459" s="5"/>
       <c r="C459" s="5"/>
@@ -19411,7 +19411,7 @@
       <c r="AI459" s="5"/>
       <c r="AJ459" s="5"/>
     </row>
-    <row r="460" spans="1:36" ht="12.75">
+    <row r="460" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A460" s="5"/>
       <c r="B460" s="5"/>
       <c r="C460" s="5"/>
@@ -19449,7 +19449,7 @@
       <c r="AI460" s="5"/>
       <c r="AJ460" s="5"/>
     </row>
-    <row r="461" spans="1:36" ht="12.75">
+    <row r="461" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A461" s="5"/>
       <c r="B461" s="5"/>
       <c r="C461" s="5"/>
@@ -19487,7 +19487,7 @@
       <c r="AI461" s="5"/>
       <c r="AJ461" s="5"/>
     </row>
-    <row r="462" spans="1:36" ht="12.75">
+    <row r="462" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A462" s="5"/>
       <c r="B462" s="5"/>
       <c r="C462" s="5"/>
@@ -19525,7 +19525,7 @@
       <c r="AI462" s="5"/>
       <c r="AJ462" s="5"/>
     </row>
-    <row r="463" spans="1:36" ht="12.75">
+    <row r="463" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A463" s="5"/>
       <c r="B463" s="5"/>
       <c r="C463" s="5"/>
@@ -19563,7 +19563,7 @@
       <c r="AI463" s="5"/>
       <c r="AJ463" s="5"/>
     </row>
-    <row r="464" spans="1:36" ht="12.75">
+    <row r="464" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A464" s="5"/>
       <c r="B464" s="5"/>
       <c r="C464" s="5"/>
@@ -19601,7 +19601,7 @@
       <c r="AI464" s="5"/>
       <c r="AJ464" s="5"/>
     </row>
-    <row r="465" spans="1:36" ht="12.75">
+    <row r="465" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A465" s="5"/>
       <c r="B465" s="5"/>
       <c r="C465" s="5"/>
@@ -19639,7 +19639,7 @@
       <c r="AI465" s="5"/>
       <c r="AJ465" s="5"/>
     </row>
-    <row r="466" spans="1:36" ht="12.75">
+    <row r="466" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A466" s="5"/>
       <c r="B466" s="5"/>
       <c r="C466" s="5"/>
@@ -19677,7 +19677,7 @@
       <c r="AI466" s="5"/>
       <c r="AJ466" s="5"/>
     </row>
-    <row r="467" spans="1:36" ht="12.75">
+    <row r="467" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A467" s="5"/>
       <c r="B467" s="5"/>
       <c r="C467" s="5"/>
@@ -19715,7 +19715,7 @@
       <c r="AI467" s="5"/>
       <c r="AJ467" s="5"/>
     </row>
-    <row r="468" spans="1:36" ht="12.75">
+    <row r="468" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A468" s="5"/>
       <c r="B468" s="5"/>
       <c r="C468" s="5"/>
@@ -19753,7 +19753,7 @@
       <c r="AI468" s="5"/>
       <c r="AJ468" s="5"/>
     </row>
-    <row r="469" spans="1:36" ht="12.75">
+    <row r="469" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A469" s="5"/>
       <c r="B469" s="5"/>
       <c r="C469" s="5"/>
@@ -19791,7 +19791,7 @@
       <c r="AI469" s="5"/>
       <c r="AJ469" s="5"/>
     </row>
-    <row r="470" spans="1:36" ht="12.75">
+    <row r="470" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A470" s="5"/>
       <c r="B470" s="5"/>
       <c r="C470" s="5"/>
@@ -19829,7 +19829,7 @@
       <c r="AI470" s="5"/>
       <c r="AJ470" s="5"/>
     </row>
-    <row r="471" spans="1:36" ht="12.75">
+    <row r="471" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A471" s="5"/>
       <c r="B471" s="5"/>
       <c r="C471" s="5"/>
@@ -19867,7 +19867,7 @@
       <c r="AI471" s="5"/>
       <c r="AJ471" s="5"/>
     </row>
-    <row r="472" spans="1:36" ht="12.75">
+    <row r="472" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A472" s="5"/>
       <c r="B472" s="5"/>
       <c r="C472" s="5"/>
@@ -19905,7 +19905,7 @@
       <c r="AI472" s="5"/>
       <c r="AJ472" s="5"/>
     </row>
-    <row r="473" spans="1:36" ht="12.75">
+    <row r="473" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A473" s="5"/>
       <c r="B473" s="5"/>
       <c r="C473" s="5"/>
@@ -19943,7 +19943,7 @@
       <c r="AI473" s="5"/>
       <c r="AJ473" s="5"/>
     </row>
-    <row r="474" spans="1:36" ht="12.75">
+    <row r="474" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A474" s="5"/>
       <c r="B474" s="5"/>
       <c r="C474" s="5"/>
@@ -19981,7 +19981,7 @@
       <c r="AI474" s="5"/>
       <c r="AJ474" s="5"/>
     </row>
-    <row r="475" spans="1:36" ht="12.75">
+    <row r="475" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A475" s="5"/>
       <c r="B475" s="5"/>
       <c r="C475" s="5"/>
@@ -20019,7 +20019,7 @@
       <c r="AI475" s="5"/>
       <c r="AJ475" s="5"/>
     </row>
-    <row r="476" spans="1:36" ht="12.75">
+    <row r="476" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A476" s="5"/>
       <c r="B476" s="5"/>
       <c r="C476" s="5"/>
@@ -20057,7 +20057,7 @@
       <c r="AI476" s="5"/>
       <c r="AJ476" s="5"/>
     </row>
-    <row r="477" spans="1:36" ht="12.75">
+    <row r="477" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A477" s="5"/>
       <c r="B477" s="5"/>
       <c r="C477" s="5"/>
@@ -20095,7 +20095,7 @@
       <c r="AI477" s="5"/>
       <c r="AJ477" s="5"/>
     </row>
-    <row r="478" spans="1:36" ht="12.75">
+    <row r="478" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A478" s="5"/>
       <c r="B478" s="5"/>
       <c r="C478" s="5"/>
@@ -20133,7 +20133,7 @@
       <c r="AI478" s="5"/>
       <c r="AJ478" s="5"/>
     </row>
-    <row r="479" spans="1:36" ht="12.75">
+    <row r="479" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A479" s="5"/>
       <c r="B479" s="5"/>
       <c r="C479" s="5"/>
@@ -20171,7 +20171,7 @@
       <c r="AI479" s="5"/>
       <c r="AJ479" s="5"/>
     </row>
-    <row r="480" spans="1:36" ht="12.75">
+    <row r="480" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A480" s="5"/>
       <c r="B480" s="5"/>
       <c r="C480" s="5"/>
@@ -20209,7 +20209,7 @@
       <c r="AI480" s="5"/>
       <c r="AJ480" s="5"/>
     </row>
-    <row r="481" spans="1:36" ht="12.75">
+    <row r="481" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A481" s="5"/>
       <c r="B481" s="5"/>
       <c r="C481" s="5"/>
@@ -20247,7 +20247,7 @@
       <c r="AI481" s="5"/>
       <c r="AJ481" s="5"/>
     </row>
-    <row r="482" spans="1:36" ht="12.75">
+    <row r="482" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A482" s="5"/>
       <c r="B482" s="5"/>
       <c r="C482" s="5"/>
@@ -20285,7 +20285,7 @@
       <c r="AI482" s="5"/>
       <c r="AJ482" s="5"/>
     </row>
-    <row r="483" spans="1:36" ht="12.75">
+    <row r="483" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A483" s="5"/>
       <c r="B483" s="5"/>
       <c r="C483" s="5"/>
@@ -20323,7 +20323,7 @@
       <c r="AI483" s="5"/>
       <c r="AJ483" s="5"/>
     </row>
-    <row r="484" spans="1:36" ht="12.75">
+    <row r="484" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A484" s="5"/>
       <c r="B484" s="5"/>
       <c r="C484" s="5"/>
@@ -20361,7 +20361,7 @@
       <c r="AI484" s="5"/>
       <c r="AJ484" s="5"/>
     </row>
-    <row r="485" spans="1:36" ht="12.75">
+    <row r="485" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A485" s="5"/>
       <c r="B485" s="5"/>
       <c r="C485" s="5"/>
@@ -20399,7 +20399,7 @@
       <c r="AI485" s="5"/>
       <c r="AJ485" s="5"/>
     </row>
-    <row r="486" spans="1:36" ht="12.75">
+    <row r="486" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A486" s="5"/>
       <c r="B486" s="5"/>
       <c r="C486" s="5"/>
@@ -20437,7 +20437,7 @@
       <c r="AI486" s="5"/>
       <c r="AJ486" s="5"/>
     </row>
-    <row r="487" spans="1:36" ht="12.75">
+    <row r="487" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A487" s="5"/>
       <c r="B487" s="5"/>
       <c r="C487" s="5"/>
@@ -20475,7 +20475,7 @@
       <c r="AI487" s="5"/>
       <c r="AJ487" s="5"/>
     </row>
-    <row r="488" spans="1:36" ht="12.75">
+    <row r="488" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A488" s="5"/>
       <c r="B488" s="5"/>
       <c r="C488" s="5"/>
@@ -20513,7 +20513,7 @@
       <c r="AI488" s="5"/>
       <c r="AJ488" s="5"/>
     </row>
-    <row r="489" spans="1:36" ht="12.75">
+    <row r="489" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A489" s="5"/>
       <c r="B489" s="5"/>
       <c r="C489" s="5"/>
@@ -20551,7 +20551,7 @@
       <c r="AI489" s="5"/>
       <c r="AJ489" s="5"/>
     </row>
-    <row r="490" spans="1:36" ht="12.75">
+    <row r="490" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A490" s="5"/>
       <c r="B490" s="5"/>
       <c r="C490" s="5"/>
@@ -20589,7 +20589,7 @@
       <c r="AI490" s="5"/>
       <c r="AJ490" s="5"/>
     </row>
-    <row r="491" spans="1:36" ht="12.75">
+    <row r="491" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A491" s="5"/>
       <c r="B491" s="5"/>
       <c r="C491" s="5"/>
@@ -20627,7 +20627,7 @@
       <c r="AI491" s="5"/>
       <c r="AJ491" s="5"/>
     </row>
-    <row r="492" spans="1:36" ht="12.75">
+    <row r="492" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A492" s="5"/>
       <c r="B492" s="5"/>
       <c r="C492" s="5"/>
@@ -20665,7 +20665,7 @@
       <c r="AI492" s="5"/>
       <c r="AJ492" s="5"/>
     </row>
-    <row r="493" spans="1:36" ht="12.75">
+    <row r="493" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A493" s="5"/>
       <c r="B493" s="5"/>
       <c r="C493" s="5"/>
@@ -20703,7 +20703,7 @@
       <c r="AI493" s="5"/>
       <c r="AJ493" s="5"/>
     </row>
-    <row r="494" spans="1:36" ht="12.75">
+    <row r="494" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A494" s="5"/>
       <c r="B494" s="5"/>
       <c r="C494" s="5"/>
@@ -20741,7 +20741,7 @@
       <c r="AI494" s="5"/>
       <c r="AJ494" s="5"/>
     </row>
-    <row r="495" spans="1:36" ht="12.75">
+    <row r="495" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A495" s="5"/>
       <c r="B495" s="5"/>
       <c r="C495" s="5"/>
@@ -20779,7 +20779,7 @@
       <c r="AI495" s="5"/>
       <c r="AJ495" s="5"/>
     </row>
-    <row r="496" spans="1:36" ht="12.75">
+    <row r="496" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A496" s="5"/>
       <c r="B496" s="5"/>
       <c r="C496" s="5"/>
@@ -20817,7 +20817,7 @@
       <c r="AI496" s="5"/>
       <c r="AJ496" s="5"/>
     </row>
-    <row r="497" spans="1:36" ht="12.75">
+    <row r="497" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A497" s="5"/>
       <c r="B497" s="5"/>
       <c r="C497" s="5"/>
@@ -20855,7 +20855,7 @@
       <c r="AI497" s="5"/>
       <c r="AJ497" s="5"/>
     </row>
-    <row r="498" spans="1:36" ht="12.75">
+    <row r="498" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A498" s="5"/>
       <c r="B498" s="5"/>
       <c r="C498" s="5"/>
@@ -20893,7 +20893,7 @@
       <c r="AI498" s="5"/>
       <c r="AJ498" s="5"/>
     </row>
-    <row r="499" spans="1:36" ht="12.75">
+    <row r="499" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A499" s="5"/>
       <c r="B499" s="5"/>
       <c r="C499" s="5"/>
@@ -20931,7 +20931,7 @@
       <c r="AI499" s="5"/>
       <c r="AJ499" s="5"/>
     </row>
-    <row r="500" spans="1:36" ht="12.75">
+    <row r="500" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A500" s="5"/>
       <c r="B500" s="5"/>
       <c r="C500" s="5"/>
@@ -20969,7 +20969,7 @@
       <c r="AI500" s="5"/>
       <c r="AJ500" s="5"/>
     </row>
-    <row r="501" spans="1:36" ht="12.75">
+    <row r="501" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A501" s="5"/>
       <c r="B501" s="5"/>
       <c r="C501" s="5"/>
@@ -21007,7 +21007,7 @@
       <c r="AI501" s="5"/>
       <c r="AJ501" s="5"/>
     </row>
-    <row r="502" spans="1:36" ht="12.75">
+    <row r="502" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A502" s="5"/>
       <c r="B502" s="5"/>
       <c r="C502" s="5"/>
@@ -21045,7 +21045,7 @@
       <c r="AI502" s="5"/>
       <c r="AJ502" s="5"/>
     </row>
-    <row r="503" spans="1:36" ht="12.75">
+    <row r="503" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A503" s="5"/>
       <c r="B503" s="5"/>
       <c r="C503" s="5"/>
@@ -21083,7 +21083,7 @@
       <c r="AI503" s="5"/>
       <c r="AJ503" s="5"/>
     </row>
-    <row r="504" spans="1:36" ht="12.75">
+    <row r="504" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A504" s="5"/>
       <c r="B504" s="5"/>
       <c r="C504" s="5"/>
@@ -21121,7 +21121,7 @@
       <c r="AI504" s="5"/>
       <c r="AJ504" s="5"/>
     </row>
-    <row r="505" spans="1:36" ht="12.75">
+    <row r="505" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A505" s="5"/>
       <c r="B505" s="5"/>
       <c r="C505" s="5"/>
@@ -21159,7 +21159,7 @@
       <c r="AI505" s="5"/>
       <c r="AJ505" s="5"/>
     </row>
-    <row r="506" spans="1:36" ht="12.75">
+    <row r="506" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A506" s="5"/>
       <c r="B506" s="5"/>
       <c r="C506" s="5"/>
@@ -21197,7 +21197,7 @@
       <c r="AI506" s="5"/>
       <c r="AJ506" s="5"/>
     </row>
-    <row r="507" spans="1:36" ht="12.75">
+    <row r="507" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A507" s="5"/>
       <c r="B507" s="5"/>
       <c r="C507" s="5"/>
@@ -21235,7 +21235,7 @@
       <c r="AI507" s="5"/>
       <c r="AJ507" s="5"/>
     </row>
-    <row r="508" spans="1:36" ht="12.75">
+    <row r="508" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A508" s="5"/>
       <c r="B508" s="5"/>
       <c r="C508" s="5"/>
@@ -21273,7 +21273,7 @@
       <c r="AI508" s="5"/>
       <c r="AJ508" s="5"/>
     </row>
-    <row r="509" spans="1:36" ht="12.75">
+    <row r="509" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A509" s="5"/>
       <c r="B509" s="5"/>
       <c r="C509" s="5"/>
@@ -21311,7 +21311,7 @@
       <c r="AI509" s="5"/>
       <c r="AJ509" s="5"/>
     </row>
-    <row r="510" spans="1:36" ht="12.75">
+    <row r="510" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A510" s="5"/>
       <c r="B510" s="5"/>
       <c r="C510" s="5"/>
@@ -21349,7 +21349,7 @@
       <c r="AI510" s="5"/>
       <c r="AJ510" s="5"/>
     </row>
-    <row r="511" spans="1:36" ht="12.75">
+    <row r="511" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A511" s="5"/>
       <c r="B511" s="5"/>
       <c r="C511" s="5"/>
@@ -21387,7 +21387,7 @@
       <c r="AI511" s="5"/>
       <c r="AJ511" s="5"/>
     </row>
-    <row r="512" spans="1:36" ht="12.75">
+    <row r="512" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A512" s="5"/>
       <c r="B512" s="5"/>
       <c r="C512" s="5"/>
@@ -21425,7 +21425,7 @@
       <c r="AI512" s="5"/>
       <c r="AJ512" s="5"/>
     </row>
-    <row r="513" spans="1:36" ht="12.75">
+    <row r="513" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A513" s="5"/>
       <c r="B513" s="5"/>
       <c r="C513" s="5"/>
@@ -21463,7 +21463,7 @@
       <c r="AI513" s="5"/>
       <c r="AJ513" s="5"/>
     </row>
-    <row r="514" spans="1:36" ht="12.75">
+    <row r="514" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A514" s="5"/>
       <c r="B514" s="5"/>
       <c r="C514" s="5"/>
@@ -21501,7 +21501,7 @@
       <c r="AI514" s="5"/>
       <c r="AJ514" s="5"/>
     </row>
-    <row r="515" spans="1:36" ht="12.75">
+    <row r="515" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A515" s="5"/>
       <c r="B515" s="5"/>
       <c r="C515" s="5"/>
@@ -21539,7 +21539,7 @@
       <c r="AI515" s="5"/>
       <c r="AJ515" s="5"/>
     </row>
-    <row r="516" spans="1:36" ht="12.75">
+    <row r="516" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A516" s="5"/>
       <c r="B516" s="5"/>
       <c r="C516" s="5"/>
@@ -21577,7 +21577,7 @@
       <c r="AI516" s="5"/>
       <c r="AJ516" s="5"/>
     </row>
-    <row r="517" spans="1:36" ht="12.75">
+    <row r="517" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A517" s="5"/>
       <c r="B517" s="5"/>
       <c r="C517" s="5"/>
@@ -21615,7 +21615,7 @@
       <c r="AI517" s="5"/>
       <c r="AJ517" s="5"/>
     </row>
-    <row r="518" spans="1:36" ht="12.75">
+    <row r="518" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A518" s="5"/>
       <c r="B518" s="5"/>
       <c r="C518" s="5"/>
@@ -21653,7 +21653,7 @@
       <c r="AI518" s="5"/>
       <c r="AJ518" s="5"/>
     </row>
-    <row r="519" spans="1:36" ht="12.75">
+    <row r="519" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A519" s="5"/>
       <c r="B519" s="5"/>
       <c r="C519" s="5"/>
@@ -21691,7 +21691,7 @@
       <c r="AI519" s="5"/>
       <c r="AJ519" s="5"/>
     </row>
-    <row r="520" spans="1:36" ht="12.75">
+    <row r="520" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A520" s="5"/>
       <c r="B520" s="5"/>
       <c r="C520" s="5"/>
@@ -21729,7 +21729,7 @@
       <c r="AI520" s="5"/>
       <c r="AJ520" s="5"/>
     </row>
-    <row r="521" spans="1:36" ht="12.75">
+    <row r="521" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A521" s="5"/>
       <c r="B521" s="5"/>
       <c r="C521" s="5"/>
@@ -21767,7 +21767,7 @@
       <c r="AI521" s="5"/>
       <c r="AJ521" s="5"/>
     </row>
-    <row r="522" spans="1:36" ht="12.75">
+    <row r="522" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A522" s="5"/>
       <c r="B522" s="5"/>
       <c r="C522" s="5"/>
@@ -21805,7 +21805,7 @@
       <c r="AI522" s="5"/>
       <c r="AJ522" s="5"/>
     </row>
-    <row r="523" spans="1:36" ht="12.75">
+    <row r="523" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A523" s="5"/>
       <c r="B523" s="5"/>
       <c r="C523" s="5"/>
@@ -21843,7 +21843,7 @@
       <c r="AI523" s="5"/>
       <c r="AJ523" s="5"/>
     </row>
-    <row r="524" spans="1:36" ht="12.75">
+    <row r="524" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A524" s="5"/>
       <c r="B524" s="5"/>
       <c r="C524" s="5"/>
@@ -21881,7 +21881,7 @@
       <c r="AI524" s="5"/>
       <c r="AJ524" s="5"/>
     </row>
-    <row r="525" spans="1:36" ht="12.75">
+    <row r="525" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A525" s="5"/>
       <c r="B525" s="5"/>
       <c r="C525" s="5"/>
@@ -21919,7 +21919,7 @@
       <c r="AI525" s="5"/>
       <c r="AJ525" s="5"/>
     </row>
-    <row r="526" spans="1:36" ht="12.75">
+    <row r="526" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A526" s="5"/>
       <c r="B526" s="5"/>
       <c r="C526" s="5"/>
@@ -21957,7 +21957,7 @@
       <c r="AI526" s="5"/>
       <c r="AJ526" s="5"/>
     </row>
-    <row r="527" spans="1:36" ht="12.75">
+    <row r="527" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A527" s="5"/>
       <c r="B527" s="5"/>
       <c r="C527" s="5"/>
@@ -21995,7 +21995,7 @@
       <c r="AI527" s="5"/>
       <c r="AJ527" s="5"/>
     </row>
-    <row r="528" spans="1:36" ht="12.75">
+    <row r="528" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A528" s="5"/>
       <c r="B528" s="5"/>
       <c r="C528" s="5"/>
@@ -22033,7 +22033,7 @@
       <c r="AI528" s="5"/>
       <c r="AJ528" s="5"/>
     </row>
-    <row r="529" spans="1:36" ht="12.75">
+    <row r="529" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A529" s="5"/>
       <c r="B529" s="5"/>
       <c r="C529" s="5"/>
@@ -22071,7 +22071,7 @@
       <c r="AI529" s="5"/>
       <c r="AJ529" s="5"/>
     </row>
-    <row r="530" spans="1:36" ht="12.75">
+    <row r="530" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A530" s="5"/>
       <c r="B530" s="5"/>
       <c r="C530" s="5"/>
@@ -22109,7 +22109,7 @@
       <c r="AI530" s="5"/>
       <c r="AJ530" s="5"/>
     </row>
-    <row r="531" spans="1:36" ht="12.75">
+    <row r="531" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A531" s="5"/>
       <c r="B531" s="5"/>
       <c r="C531" s="5"/>
@@ -22147,7 +22147,7 @@
       <c r="AI531" s="5"/>
       <c r="AJ531" s="5"/>
     </row>
-    <row r="532" spans="1:36" ht="12.75">
+    <row r="532" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A532" s="5"/>
       <c r="B532" s="5"/>
       <c r="C532" s="5"/>
@@ -22185,7 +22185,7 @@
       <c r="AI532" s="5"/>
       <c r="AJ532" s="5"/>
     </row>
-    <row r="533" spans="1:36" ht="12.75">
+    <row r="533" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A533" s="5"/>
       <c r="B533" s="5"/>
       <c r="C533" s="5"/>
@@ -22223,7 +22223,7 @@
       <c r="AI533" s="5"/>
       <c r="AJ533" s="5"/>
     </row>
-    <row r="534" spans="1:36" ht="12.75">
+    <row r="534" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A534" s="5"/>
       <c r="B534" s="5"/>
       <c r="C534" s="5"/>
@@ -22283,12 +22283,12 @@
       <selection activeCell="P2" sqref="P2:AE2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -22383,7 +22383,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="30">
+    <row r="2" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -22467,15 +22467,15 @@
       </c>
       <c r="V2" s="2">
         <f>'Inflation Reduction Act'!T88</f>
-        <v>0.31218750000000001</v>
+        <v>0.41625000000000001</v>
       </c>
       <c r="W2" s="2">
         <f>'Inflation Reduction Act'!U88</f>
-        <v>0.208125</v>
+        <v>0.31218750000000001</v>
       </c>
       <c r="X2" s="2">
         <f>'Inflation Reduction Act'!V88</f>
-        <v>0</v>
+        <v>0.208125</v>
       </c>
       <c r="Y2" s="2">
         <f>'Inflation Reduction Act'!W88</f>

</xml_diff>

<commit_message>
Edit IRA tax credit expiration year based on EPS outputs
</commit_message>
<xml_diff>
--- a/InputData/elec/BPSpUGBCD/BAU Subsidy per Unit Grid Battery Capacity Deployed.xlsx
+++ b/InputData/elec/BPSpUGBCD/BAU Subsidy per Unit Grid Battery Capacity Deployed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\BPSpUGBCD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90B21F7-7DC3-4F30-BB66-A9166A9537C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40724972-2873-4441-97DA-52FF5D7F6AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -921,7 +921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -978,8 +978,8 @@
   </sheetPr>
   <dimension ref="A1:AJ534"/>
   <sheetViews>
-    <sheetView topLeftCell="B48" workbookViewId="0">
-      <selection activeCell="V79" sqref="V79"/>
+    <sheetView tabSelected="1" topLeftCell="B48" workbookViewId="0">
+      <selection activeCell="V75" sqref="V75:Y75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4614,13 +4614,13 @@
         <v>1</v>
       </c>
       <c r="V75" s="37">
+        <v>1</v>
+      </c>
+      <c r="W75" s="37">
         <v>0.75</v>
       </c>
-      <c r="W75" s="37">
+      <c r="X75" s="37">
         <v>0.5</v>
-      </c>
-      <c r="X75" s="37">
-        <v>0</v>
       </c>
       <c r="Y75" s="37">
         <v>0</v>
@@ -5271,15 +5271,15 @@
       </c>
       <c r="U88" s="38">
         <f t="shared" si="5"/>
-        <v>0.31218750000000001</v>
+        <v>0.41625000000000001</v>
       </c>
       <c r="V88" s="38">
         <f t="shared" si="5"/>
-        <v>0.208125</v>
+        <v>0.31218750000000001</v>
       </c>
       <c r="W88" s="31">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.208125</v>
       </c>
       <c r="X88" s="31">
         <f t="shared" si="5"/>
@@ -22471,15 +22471,15 @@
       </c>
       <c r="W2" s="2">
         <f>'Inflation Reduction Act'!U88</f>
-        <v>0.31218750000000001</v>
+        <v>0.41625000000000001</v>
       </c>
       <c r="X2" s="2">
         <f>'Inflation Reduction Act'!V88</f>
-        <v>0.208125</v>
+        <v>0.31218750000000001</v>
       </c>
       <c r="Y2" s="2">
         <f>'Inflation Reduction Act'!W88</f>
-        <v>0</v>
+        <v>0.208125</v>
       </c>
       <c r="Z2" s="2">
         <f>'Inflation Reduction Act'!X88</f>

</xml_diff>

<commit_message>
Additional file for IRA expiration year
</commit_message>
<xml_diff>
--- a/InputData/elec/BPSpUGBCD/BAU Subsidy per Unit Grid Battery Capacity Deployed.xlsx
+++ b/InputData/elec/BPSpUGBCD/BAU Subsidy per Unit Grid Battery Capacity Deployed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\BPSpUGBCD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40724972-2873-4441-97DA-52FF5D7F6AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1640CF-E3B7-443F-9523-22E8743CB9F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -979,7 +979,7 @@
   <dimension ref="A1:AJ534"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B48" workbookViewId="0">
-      <selection activeCell="V75" sqref="V75:Y75"/>
+      <selection activeCell="U75" sqref="U75:X75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4614,13 +4614,13 @@
         <v>1</v>
       </c>
       <c r="V75" s="37">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="W75" s="37">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="X75" s="37">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="Y75" s="37">
         <v>0</v>
@@ -5271,15 +5271,15 @@
       </c>
       <c r="U88" s="38">
         <f t="shared" si="5"/>
-        <v>0.41625000000000001</v>
+        <v>0.31218750000000001</v>
       </c>
       <c r="V88" s="38">
         <f t="shared" si="5"/>
-        <v>0.31218750000000001</v>
+        <v>0.208125</v>
       </c>
       <c r="W88" s="31">
         <f t="shared" si="5"/>
-        <v>0.208125</v>
+        <v>0</v>
       </c>
       <c r="X88" s="31">
         <f t="shared" si="5"/>
@@ -22471,15 +22471,15 @@
       </c>
       <c r="W2" s="2">
         <f>'Inflation Reduction Act'!U88</f>
-        <v>0.41625000000000001</v>
+        <v>0.31218750000000001</v>
       </c>
       <c r="X2" s="2">
         <f>'Inflation Reduction Act'!V88</f>
-        <v>0.31218750000000001</v>
+        <v>0.208125</v>
       </c>
       <c r="Y2" s="2">
         <f>'Inflation Reduction Act'!W88</f>
-        <v>0.208125</v>
+        <v>0</v>
       </c>
       <c r="Z2" s="2">
         <f>'Inflation Reduction Act'!X88</f>

</xml_diff>

<commit_message>
Update ITC/PTC expiration year based on recent changes
</commit_message>
<xml_diff>
--- a/InputData/elec/BPSpUGBCD/BAU Subsidy per Unit Grid Battery Capacity Deployed.xlsx
+++ b/InputData/elec/BPSpUGBCD/BAU Subsidy per Unit Grid Battery Capacity Deployed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\BPSpUGBCD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD3E038-2CE1-4B0E-859B-89B6E7160989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF49387-40D7-4827-B5F4-11DFF6188CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -464,7 +464,7 @@
     <t>ITC Phase-out Scheulde, batteries</t>
   </si>
   <si>
-    <t>Latest calibration year target passed: 2035</t>
+    <t>Latest calibration year target passed: 2036</t>
   </si>
 </sst>
 </file>
@@ -479,7 +479,7 @@
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.0"/>
     <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1351,14 +1351,14 @@
       <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1366,27 +1366,27 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1404,11 +1404,11 @@
   </sheetPr>
   <dimension ref="A1:BV252"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="94.42578125" style="6" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" style="6" customWidth="1"/>
@@ -1420,7 +1420,7 @@
     <col min="37" max="16384" width="12.5703125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:37" ht="12.75">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -1460,7 +1460,7 @@
       <c r="AI1" s="5"/>
       <c r="AJ1" s="5"/>
     </row>
-    <row r="2" spans="1:37" ht="305.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" ht="305.25" customHeight="1">
       <c r="A2" s="7" t="s">
         <v>62</v>
       </c>
@@ -1500,7 +1500,7 @@
       <c r="AI2" s="5"/>
       <c r="AJ2" s="5"/>
     </row>
-    <row r="3" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" ht="12.75">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -1538,7 +1538,7 @@
       <c r="AI3" s="5"/>
       <c r="AJ3" s="5"/>
     </row>
-    <row r="4" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:37" ht="12.75">
       <c r="A4" s="4" t="s">
         <v>63</v>
       </c>
@@ -1578,7 +1578,7 @@
       <c r="AI4" s="5"/>
       <c r="AJ4" s="5"/>
     </row>
-    <row r="5" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:37" ht="12.75">
       <c r="A5" s="5" t="s">
         <v>64</v>
       </c>
@@ -1618,7 +1618,7 @@
       <c r="AI5" s="5"/>
       <c r="AJ5" s="5"/>
     </row>
-    <row r="6" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:37" ht="12.75">
       <c r="A6" s="5" t="s">
         <v>65</v>
       </c>
@@ -1658,7 +1658,7 @@
       <c r="AI6" s="5"/>
       <c r="AJ6" s="5"/>
     </row>
-    <row r="7" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:37" ht="12.75">
       <c r="A7" s="5" t="s">
         <v>66</v>
       </c>
@@ -1698,7 +1698,7 @@
       <c r="AI7" s="5"/>
       <c r="AJ7" s="5"/>
     </row>
-    <row r="8" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:37" ht="12.75">
       <c r="A8" s="5">
         <f>1554.4*0.25</f>
         <v>388.6</v>
@@ -1741,7 +1741,7 @@
       <c r="AI8" s="5"/>
       <c r="AJ8" s="5"/>
     </row>
-    <row r="9" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:37" ht="12.75">
       <c r="A9" s="5" t="s">
         <v>130</v>
       </c>
@@ -1781,7 +1781,7 @@
       <c r="AI9" s="5"/>
       <c r="AJ9" s="5"/>
     </row>
-    <row r="10" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:37" ht="12.75">
       <c r="A10" s="5" t="s">
         <v>68</v>
       </c>
@@ -1821,7 +1821,7 @@
       <c r="AI10" s="5"/>
       <c r="AJ10" s="5"/>
     </row>
-    <row r="11" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:37" ht="12.75">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -1859,7 +1859,7 @@
       <c r="AI11" s="5"/>
       <c r="AJ11" s="5"/>
     </row>
-    <row r="12" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:37" ht="12.75">
       <c r="A12" s="5" t="s">
         <v>69</v>
       </c>
@@ -1905,7 +1905,7 @@
       <c r="AI12" s="5"/>
       <c r="AJ12" s="5"/>
     </row>
-    <row r="13" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:37" ht="12.75">
       <c r="A13" s="41">
         <v>1</v>
       </c>
@@ -1951,7 +1951,7 @@
       <c r="AI13" s="5"/>
       <c r="AJ13" s="5"/>
     </row>
-    <row r="14" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:37" ht="12.75">
       <c r="A14" s="41"/>
       <c r="B14" s="41"/>
       <c r="C14" s="41"/>
@@ -1967,19 +1967,19 @@
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
-      <c r="P14" s="5" t="s">
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="Q14" s="5" t="s">
+      <c r="R14" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="R14" s="5" t="s">
+      <c r="S14" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="S14" s="5" t="s">
+      <c r="T14" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="T14" s="5"/>
       <c r="U14" s="5"/>
       <c r="V14" s="5"/>
       <c r="W14" s="5"/>
@@ -1997,7 +1997,7 @@
       <c r="AI14" s="5"/>
       <c r="AJ14" s="5"/>
     </row>
-    <row r="15" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:37" ht="12.75">
       <c r="A15" s="41" t="s">
         <v>77</v>
       </c>
@@ -2037,7 +2037,7 @@
       <c r="AI15" s="5"/>
       <c r="AJ15" s="5"/>
     </row>
-    <row r="16" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:37" ht="12.75">
       <c r="A16" s="6">
         <v>2020</v>
       </c>
@@ -2138,7 +2138,7 @@
       <c r="AJ16" s="42"/>
       <c r="AK16" s="42"/>
     </row>
-    <row r="17" spans="1:51" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:51" ht="12.75">
       <c r="A17" s="41">
         <v>1</v>
       </c>
@@ -2191,13 +2191,13 @@
         <v>1</v>
       </c>
       <c r="R17" s="41">
+        <v>1</v>
+      </c>
+      <c r="S17" s="41">
         <v>0.75</v>
       </c>
-      <c r="S17" s="41">
+      <c r="T17" s="41">
         <v>0.5</v>
-      </c>
-      <c r="T17" s="41">
-        <v>0</v>
       </c>
       <c r="U17" s="41">
         <v>0</v>
@@ -2253,7 +2253,7 @@
       <c r="AX17" s="41"/>
       <c r="AY17" s="41"/>
     </row>
-    <row r="18" spans="1:51" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:51" ht="12.75">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -2291,7 +2291,7 @@
       <c r="AI18" s="5"/>
       <c r="AJ18" s="5"/>
     </row>
-    <row r="19" spans="1:51" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:51" ht="12.75">
       <c r="A19" s="4" t="s">
         <v>9</v>
       </c>
@@ -2331,7 +2331,7 @@
       <c r="AI19" s="8"/>
       <c r="AJ19" s="8"/>
     </row>
-    <row r="20" spans="1:51" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:51" ht="12.75">
       <c r="A20" s="9" t="s">
         <v>10</v>
       </c>
@@ -2371,7 +2371,7 @@
       <c r="AI20" s="10"/>
       <c r="AJ20" s="10"/>
     </row>
-    <row r="21" spans="1:51" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:51" ht="12.75">
       <c r="A21" s="11" t="s">
         <v>11</v>
       </c>
@@ -2411,7 +2411,7 @@
       <c r="AI21" s="5"/>
       <c r="AJ21" s="5"/>
     </row>
-    <row r="22" spans="1:51" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:51" ht="12.75">
       <c r="A22" s="12" t="s">
         <v>12</v>
       </c>
@@ -2451,7 +2451,7 @@
       <c r="AI22" s="5"/>
       <c r="AJ22" s="5"/>
     </row>
-    <row r="23" spans="1:51" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:51" ht="12.75">
       <c r="A23" s="13"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -2489,7 +2489,7 @@
       <c r="AI23" s="5"/>
       <c r="AJ23" s="5"/>
     </row>
-    <row r="24" spans="1:51" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:51" ht="12.75">
       <c r="A24" s="13"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -2527,7 +2527,7 @@
       <c r="AI24" s="5"/>
       <c r="AJ24" s="5"/>
     </row>
-    <row r="25" spans="1:51" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:51" ht="12.75">
       <c r="A25" s="13"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -2565,7 +2565,7 @@
       <c r="AI25" s="5"/>
       <c r="AJ25" s="5"/>
     </row>
-    <row r="26" spans="1:51" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:51" ht="12.75">
       <c r="A26" s="13"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -2603,7 +2603,7 @@
       <c r="AI26" s="5"/>
       <c r="AJ26" s="5"/>
     </row>
-    <row r="27" spans="1:51" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:51" ht="12.75">
       <c r="A27" s="13"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -2641,7 +2641,7 @@
       <c r="AI27" s="5"/>
       <c r="AJ27" s="5"/>
     </row>
-    <row r="28" spans="1:51" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:51" ht="12.75">
       <c r="A28" s="13"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -2679,7 +2679,7 @@
       <c r="AI28" s="5"/>
       <c r="AJ28" s="5"/>
     </row>
-    <row r="29" spans="1:51" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:51" ht="12.75">
       <c r="A29" s="13"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -2717,7 +2717,7 @@
       <c r="AI29" s="5"/>
       <c r="AJ29" s="5"/>
     </row>
-    <row r="30" spans="1:51" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:51" ht="12.75">
       <c r="A30" s="13"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -2755,7 +2755,7 @@
       <c r="AI30" s="5"/>
       <c r="AJ30" s="5"/>
     </row>
-    <row r="31" spans="1:51" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:51" ht="12.75">
       <c r="A31" s="13"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -2793,7 +2793,7 @@
       <c r="AI31" s="5"/>
       <c r="AJ31" s="5"/>
     </row>
-    <row r="32" spans="1:51" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:51" ht="12.75">
       <c r="A32" s="13"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -2831,7 +2831,7 @@
       <c r="AI32" s="5"/>
       <c r="AJ32" s="5"/>
     </row>
-    <row r="33" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:36" ht="12.75">
       <c r="A33" s="13"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -2869,7 +2869,7 @@
       <c r="AI33" s="5"/>
       <c r="AJ33" s="5"/>
     </row>
-    <row r="34" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:36" ht="12.75">
       <c r="A34" s="13"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -2907,7 +2907,7 @@
       <c r="AI34" s="5"/>
       <c r="AJ34" s="5"/>
     </row>
-    <row r="35" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:36" ht="12.75">
       <c r="A35" s="13"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -2945,7 +2945,7 @@
       <c r="AI35" s="5"/>
       <c r="AJ35" s="5"/>
     </row>
-    <row r="36" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:36" ht="12.75">
       <c r="A36" s="13"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -2983,7 +2983,7 @@
       <c r="AI36" s="5"/>
       <c r="AJ36" s="5"/>
     </row>
-    <row r="37" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:36" ht="12.75">
       <c r="A37" s="13"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -3021,7 +3021,7 @@
       <c r="AI37" s="5"/>
       <c r="AJ37" s="5"/>
     </row>
-    <row r="38" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:36" ht="12.75">
       <c r="A38" s="13"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -3059,7 +3059,7 @@
       <c r="AI38" s="5"/>
       <c r="AJ38" s="5"/>
     </row>
-    <row r="39" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:36" ht="12.75">
       <c r="A39" s="13"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -3097,7 +3097,7 @@
       <c r="AI39" s="5"/>
       <c r="AJ39" s="5"/>
     </row>
-    <row r="40" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:36" ht="12.75">
       <c r="A40" s="13"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -3135,7 +3135,7 @@
       <c r="AI40" s="5"/>
       <c r="AJ40" s="5"/>
     </row>
-    <row r="41" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:36" ht="12.75">
       <c r="A41" s="5" t="s">
         <v>13</v>
       </c>
@@ -3175,7 +3175,7 @@
       <c r="AI41" s="5"/>
       <c r="AJ41" s="5"/>
     </row>
-    <row r="42" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:36" ht="12.75">
       <c r="A42" s="5" t="s">
         <v>14</v>
       </c>
@@ -3215,7 +3215,7 @@
       <c r="AI42" s="5"/>
       <c r="AJ42" s="5"/>
     </row>
-    <row r="43" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:36" ht="12.75">
       <c r="A43" s="5" t="s">
         <v>15</v>
       </c>
@@ -3255,7 +3255,7 @@
       <c r="AI43" s="5"/>
       <c r="AJ43" s="5"/>
     </row>
-    <row r="44" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:36" ht="12.75">
       <c r="A44" s="5" t="s">
         <v>78</v>
       </c>
@@ -3295,7 +3295,7 @@
       <c r="AI44" s="5"/>
       <c r="AJ44" s="5"/>
     </row>
-    <row r="45" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:36" ht="12.75">
       <c r="A45" s="6" t="s">
         <v>16</v>
       </c>
@@ -3337,7 +3337,7 @@
       <c r="AI45" s="5"/>
       <c r="AJ45" s="5"/>
     </row>
-    <row r="46" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:36" ht="12.75">
       <c r="A46" s="6" t="s">
         <v>17</v>
       </c>
@@ -3380,7 +3380,7 @@
       <c r="AI46" s="5"/>
       <c r="AJ46" s="5"/>
     </row>
-    <row r="47" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:36" ht="12.75">
       <c r="A47" s="13"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
@@ -3418,7 +3418,7 @@
       <c r="AI47" s="5"/>
       <c r="AJ47" s="5"/>
     </row>
-    <row r="48" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:36" ht="12.75">
       <c r="A48" s="13"/>
       <c r="B48" s="13">
         <v>2022</v>
@@ -3514,7 +3514,7 @@
       <c r="AI48" s="5"/>
       <c r="AJ48" s="5"/>
     </row>
-    <row r="49" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:36" ht="12.75">
       <c r="A49" s="15" t="s">
         <v>18</v>
       </c>
@@ -3612,7 +3612,7 @@
       <c r="AI49" s="5"/>
       <c r="AJ49" s="5"/>
     </row>
-    <row r="50" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:36" ht="12.75">
       <c r="A50" s="15" t="s">
         <v>19</v>
       </c>
@@ -3711,7 +3711,7 @@
       <c r="AI50" s="5"/>
       <c r="AJ50" s="5"/>
     </row>
-    <row r="51" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:36" ht="12.75">
       <c r="A51" s="13"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
@@ -3749,7 +3749,7 @@
       <c r="AI51" s="5"/>
       <c r="AJ51" s="5"/>
     </row>
-    <row r="52" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:36" ht="12.75">
       <c r="A52" s="9" t="s">
         <v>20</v>
       </c>
@@ -3789,7 +3789,7 @@
       <c r="AI52" s="10"/>
       <c r="AJ52" s="10"/>
     </row>
-    <row r="53" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:36" ht="12.75">
       <c r="A53" s="5" t="s">
         <v>21</v>
       </c>
@@ -3829,7 +3829,7 @@
       <c r="AI53" s="5"/>
       <c r="AJ53" s="5"/>
     </row>
-    <row r="54" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:36" ht="12.75">
       <c r="A54" s="16" t="s">
         <v>22</v>
       </c>
@@ -3869,7 +3869,7 @@
       <c r="AI54" s="5"/>
       <c r="AJ54" s="5"/>
     </row>
-    <row r="55" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:36" ht="12.75">
       <c r="A55" s="13"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -3907,7 +3907,7 @@
       <c r="AI55" s="5"/>
       <c r="AJ55" s="5"/>
     </row>
-    <row r="56" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:36" ht="12.75">
       <c r="A56" s="17" t="s">
         <v>23</v>
       </c>
@@ -3951,7 +3951,7 @@
       <c r="AI56" s="5"/>
       <c r="AJ56" s="5"/>
     </row>
-    <row r="57" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:36" ht="12.75">
       <c r="A57" s="19" t="s">
         <v>26</v>
       </c>
@@ -3993,7 +3993,7 @@
       <c r="AI57" s="5"/>
       <c r="AJ57" s="5"/>
     </row>
-    <row r="58" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:36" ht="12.75">
       <c r="A58" s="21" t="s">
         <v>28</v>
       </c>
@@ -4037,7 +4037,7 @@
       <c r="AI58" s="5"/>
       <c r="AJ58" s="5"/>
     </row>
-    <row r="59" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:36" ht="12.75">
       <c r="A59" s="21" t="s">
         <v>29</v>
       </c>
@@ -4081,7 +4081,7 @@
       <c r="AI59" s="5"/>
       <c r="AJ59" s="5"/>
     </row>
-    <row r="60" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:36" ht="12.75">
       <c r="A60" s="21" t="s">
         <v>30</v>
       </c>
@@ -4125,7 +4125,7 @@
       <c r="AI60" s="5"/>
       <c r="AJ60" s="5"/>
     </row>
-    <row r="61" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:36" ht="12.75">
       <c r="A61" s="21" t="s">
         <v>31</v>
       </c>
@@ -4167,7 +4167,7 @@
       <c r="AI61" s="5"/>
       <c r="AJ61" s="5"/>
     </row>
-    <row r="62" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:36" ht="12.75">
       <c r="A62" s="21" t="s">
         <v>32</v>
       </c>
@@ -4209,7 +4209,7 @@
       <c r="AI62" s="5"/>
       <c r="AJ62" s="5"/>
     </row>
-    <row r="63" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:36" ht="12.75">
       <c r="A63" s="21" t="s">
         <v>33</v>
       </c>
@@ -4251,7 +4251,7 @@
       <c r="AI63" s="5"/>
       <c r="AJ63" s="5"/>
     </row>
-    <row r="64" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:36" ht="12.75">
       <c r="A64" s="21" t="s">
         <v>34</v>
       </c>
@@ -4293,7 +4293,7 @@
       <c r="AI64" s="5"/>
       <c r="AJ64" s="5"/>
     </row>
-    <row r="65" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:36" ht="12.75">
       <c r="A65" s="21" t="s">
         <v>35</v>
       </c>
@@ -4335,7 +4335,7 @@
       <c r="AI65" s="5"/>
       <c r="AJ65" s="5"/>
     </row>
-    <row r="66" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:36" ht="12.75">
       <c r="A66" s="21" t="s">
         <v>36</v>
       </c>
@@ -4377,7 +4377,7 @@
       <c r="AI66" s="5"/>
       <c r="AJ66" s="5"/>
     </row>
-    <row r="67" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:36" ht="12.75">
       <c r="A67" s="24" t="s">
         <v>37</v>
       </c>
@@ -4419,7 +4419,7 @@
       <c r="AI67" s="5"/>
       <c r="AJ67" s="5"/>
     </row>
-    <row r="68" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:36" ht="12.75">
       <c r="A68" s="13"/>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
@@ -4457,7 +4457,7 @@
       <c r="AI68" s="5"/>
       <c r="AJ68" s="5"/>
     </row>
-    <row r="69" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:36" ht="12.75">
       <c r="A69" s="5" t="s">
         <v>38</v>
       </c>
@@ -4500,7 +4500,7 @@
       <c r="AI69" s="5"/>
       <c r="AJ69" s="5"/>
     </row>
-    <row r="70" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:36" ht="12.75">
       <c r="A70" s="5" t="s">
         <v>39</v>
       </c>
@@ -4543,7 +4543,7 @@
       <c r="AI70" s="5"/>
       <c r="AJ70" s="5"/>
     </row>
-    <row r="71" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:36" ht="12.75">
       <c r="A71" s="5"/>
       <c r="B71" s="23"/>
       <c r="C71" s="5"/>
@@ -4581,7 +4581,7 @@
       <c r="AI71" s="5"/>
       <c r="AJ71" s="5"/>
     </row>
-    <row r="72" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:36" ht="12.75">
       <c r="A72" s="5"/>
       <c r="B72" s="13">
         <v>2022</v>
@@ -4633,7 +4633,7 @@
       <c r="AI72" s="5"/>
       <c r="AJ72" s="5"/>
     </row>
-    <row r="73" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:36" ht="12.75">
       <c r="A73" s="7" t="s">
         <v>40</v>
       </c>
@@ -4694,7 +4694,7 @@
       <c r="AI73" s="5"/>
       <c r="AJ73" s="5"/>
     </row>
-    <row r="74" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:36" ht="12.75">
       <c r="A74" s="7"/>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
@@ -4732,7 +4732,7 @@
       <c r="AI74" s="5"/>
       <c r="AJ74" s="5"/>
     </row>
-    <row r="75" spans="1:36" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:36" ht="25.5">
       <c r="A75" s="7" t="s">
         <v>41</v>
       </c>
@@ -4772,7 +4772,7 @@
       <c r="AI75" s="5"/>
       <c r="AJ75" s="5"/>
     </row>
-    <row r="76" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:36" ht="12.75">
       <c r="A76" s="7"/>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
@@ -4810,7 +4810,7 @@
       <c r="AI76" s="13"/>
       <c r="AJ76" s="13"/>
     </row>
-    <row r="77" spans="1:36" s="26" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:36" s="26" customFormat="1" ht="12.75">
       <c r="A77" s="15"/>
       <c r="B77" s="15">
         <v>2022</v>
@@ -4906,7 +4906,7 @@
       <c r="AI77" s="13"/>
       <c r="AJ77" s="13"/>
     </row>
-    <row r="78" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:36" ht="12.75">
       <c r="A78" s="23" t="s">
         <v>42</v>
       </c>
@@ -5004,7 +5004,7 @@
       <c r="AI78" s="23"/>
       <c r="AJ78" s="23"/>
     </row>
-    <row r="79" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:36" ht="12.75">
       <c r="A79" s="23" t="s">
         <v>43</v>
       </c>
@@ -5131,7 +5131,7 @@
       <c r="AI79" s="23"/>
       <c r="AJ79" s="23"/>
     </row>
-    <row r="80" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:36" ht="12.75">
       <c r="A80" s="5" t="s">
         <v>44</v>
       </c>
@@ -5258,7 +5258,7 @@
       <c r="AI80" s="5"/>
       <c r="AJ80" s="5"/>
     </row>
-    <row r="81" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:36" ht="12.75">
       <c r="A81" s="11"/>
       <c r="B81" s="27"/>
       <c r="C81" s="27"/>
@@ -5296,7 +5296,7 @@
       <c r="AI81" s="13"/>
       <c r="AJ81" s="13"/>
     </row>
-    <row r="82" spans="1:36" s="29" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:36" s="29" customFormat="1" ht="25.5">
       <c r="A82" s="7" t="s">
         <v>45</v>
       </c>
@@ -5394,7 +5394,7 @@
       <c r="AI82" s="15"/>
       <c r="AJ82" s="15"/>
     </row>
-    <row r="83" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:36" ht="12.75">
       <c r="A83" s="13"/>
       <c r="B83" s="13"/>
       <c r="C83" s="13"/>
@@ -5432,7 +5432,7 @@
       <c r="AI83" s="13"/>
       <c r="AJ83" s="13"/>
     </row>
-    <row r="84" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:36" ht="12.75">
       <c r="A84" s="9" t="s">
         <v>1</v>
       </c>
@@ -5472,7 +5472,7 @@
       <c r="AI84" s="10"/>
       <c r="AJ84" s="10"/>
     </row>
-    <row r="85" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:36" ht="12.75">
       <c r="A85" s="11" t="s">
         <v>46</v>
       </c>
@@ -5512,7 +5512,7 @@
       <c r="AI85" s="5"/>
       <c r="AJ85" s="5"/>
     </row>
-    <row r="86" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:36" ht="12.75">
       <c r="A86" s="11" t="s">
         <v>47</v>
       </c>
@@ -5552,7 +5552,7 @@
       <c r="AI86" s="5"/>
       <c r="AJ86" s="5"/>
     </row>
-    <row r="87" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:36" ht="12.75">
       <c r="A87" s="11" t="s">
         <v>48</v>
       </c>
@@ -5592,7 +5592,7 @@
       <c r="AI87" s="5"/>
       <c r="AJ87" s="5"/>
     </row>
-    <row r="88" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:36" ht="12.75">
       <c r="A88" s="11" t="s">
         <v>79</v>
       </c>
@@ -5632,7 +5632,7 @@
       <c r="AI88" s="5"/>
       <c r="AJ88" s="5"/>
     </row>
-    <row r="89" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:36" ht="12.75">
       <c r="A89" s="11" t="s">
         <v>80</v>
       </c>
@@ -5672,7 +5672,7 @@
       <c r="AI89" s="5"/>
       <c r="AJ89" s="5"/>
     </row>
-    <row r="90" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:36" ht="12.75">
       <c r="A90" s="5"/>
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
@@ -5710,7 +5710,7 @@
       <c r="AI90" s="5"/>
       <c r="AJ90" s="5"/>
     </row>
-    <row r="91" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:36" ht="12.75">
       <c r="A91" s="9" t="s">
         <v>81</v>
       </c>
@@ -5750,7 +5750,7 @@
       <c r="AI91" s="9"/>
       <c r="AJ91" s="9"/>
     </row>
-    <row r="92" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:36" ht="12.75">
       <c r="A92" s="30"/>
       <c r="B92" s="30"/>
       <c r="C92" s="5"/>
@@ -5788,7 +5788,7 @@
       <c r="AI92" s="5"/>
       <c r="AJ92" s="5"/>
     </row>
-    <row r="93" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:36" ht="12.75">
       <c r="A93" s="30" t="s">
         <v>82</v>
       </c>
@@ -5830,7 +5830,7 @@
       <c r="AI93" s="5"/>
       <c r="AJ93" s="5"/>
     </row>
-    <row r="94" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:36" ht="12.75">
       <c r="A94" s="30" t="s">
         <v>83</v>
       </c>
@@ -5872,7 +5872,7 @@
       <c r="AI94" s="5"/>
       <c r="AJ94" s="5"/>
     </row>
-    <row r="95" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:36" ht="12.75">
       <c r="A95" s="30" t="s">
         <v>84</v>
       </c>
@@ -5916,7 +5916,7 @@
       <c r="AI95" s="5"/>
       <c r="AJ95" s="5"/>
     </row>
-    <row r="96" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:36" ht="12.75">
       <c r="A96" s="30" t="s">
         <v>86</v>
       </c>
@@ -5958,7 +5958,7 @@
       <c r="AI96" s="5"/>
       <c r="AJ96" s="5"/>
     </row>
-    <row r="97" spans="1:36" ht="17.25" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:36" ht="17.25">
       <c r="A97" s="30" t="s">
         <v>87</v>
       </c>
@@ -6000,7 +6000,7 @@
       <c r="AI97" s="5"/>
       <c r="AJ97" s="5"/>
     </row>
-    <row r="98" spans="1:36" ht="17.25" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:36" ht="17.25">
       <c r="A98" s="30"/>
       <c r="B98" s="46"/>
       <c r="C98" s="5"/>
@@ -6038,7 +6038,7 @@
       <c r="AI98" s="5"/>
       <c r="AJ98" s="5"/>
     </row>
-    <row r="99" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:36" ht="12.75">
       <c r="A99" s="30" t="s">
         <v>88</v>
       </c>
@@ -6081,7 +6081,7 @@
       <c r="AI99" s="5"/>
       <c r="AJ99" s="5"/>
     </row>
-    <row r="100" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:36" ht="12.75">
       <c r="A100" s="30" t="s">
         <v>89</v>
       </c>
@@ -6124,7 +6124,7 @@
       <c r="AI100" s="5"/>
       <c r="AJ100" s="5"/>
     </row>
-    <row r="101" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:36" ht="12.75">
       <c r="A101" s="30" t="s">
         <v>49</v>
       </c>
@@ -6166,7 +6166,7 @@
       <c r="AI101" s="5"/>
       <c r="AJ101" s="5"/>
     </row>
-    <row r="102" spans="1:36" ht="17.25" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:36" ht="17.25">
       <c r="A102" s="30" t="s">
         <v>50</v>
       </c>
@@ -6208,7 +6208,7 @@
       <c r="AI102" s="5"/>
       <c r="AJ102" s="5"/>
     </row>
-    <row r="103" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:36" ht="12.75">
       <c r="A103" s="30" t="s">
         <v>90</v>
       </c>
@@ -6252,7 +6252,7 @@
       <c r="AI103" s="5"/>
       <c r="AJ103" s="5"/>
     </row>
-    <row r="104" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:36" ht="12.75">
       <c r="A104" s="30" t="s">
         <v>51</v>
       </c>
@@ -6296,7 +6296,7 @@
       <c r="AI104" s="5"/>
       <c r="AJ104" s="5"/>
     </row>
-    <row r="105" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:36" ht="12.75">
       <c r="A105" s="30" t="s">
         <v>52</v>
       </c>
@@ -6338,7 +6338,7 @@
       <c r="AI105" s="5"/>
       <c r="AJ105" s="5"/>
     </row>
-    <row r="106" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:36" ht="12.75">
       <c r="A106" s="30" t="s">
         <v>53</v>
       </c>
@@ -6380,7 +6380,7 @@
       <c r="AI106" s="5"/>
       <c r="AJ106" s="5"/>
     </row>
-    <row r="107" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:36" ht="12.75">
       <c r="A107" s="30"/>
       <c r="B107" s="30"/>
       <c r="C107" s="5"/>
@@ -6418,7 +6418,7 @@
       <c r="AI107" s="5"/>
       <c r="AJ107" s="5"/>
     </row>
-    <row r="108" spans="1:36" s="35" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:36" s="35" customFormat="1" ht="12.75">
       <c r="A108" s="32" t="s">
         <v>93</v>
       </c>
@@ -6458,7 +6458,7 @@
       <c r="AI108" s="34"/>
       <c r="AJ108" s="34"/>
     </row>
-    <row r="109" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:36" ht="12.75">
       <c r="A109" s="51"/>
       <c r="B109" s="30" t="s">
         <v>94</v>
@@ -6500,7 +6500,7 @@
       <c r="AI109" s="5"/>
       <c r="AJ109" s="5"/>
     </row>
-    <row r="110" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:36" ht="12.75">
       <c r="A110" s="51" t="s">
         <v>96</v>
       </c>
@@ -6544,7 +6544,7 @@
       <c r="AI110" s="5"/>
       <c r="AJ110" s="5"/>
     </row>
-    <row r="111" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:36" ht="12.75">
       <c r="A111" s="51"/>
       <c r="B111" s="30"/>
       <c r="C111" s="5"/>
@@ -6582,7 +6582,7 @@
       <c r="AI111" s="5"/>
       <c r="AJ111" s="5"/>
     </row>
-    <row r="112" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:36" ht="12.75">
       <c r="A112" s="30"/>
       <c r="B112" s="30">
         <v>2023</v>
@@ -6675,7 +6675,7 @@
       <c r="AH112" s="5"/>
       <c r="AI112" s="5"/>
     </row>
-    <row r="113" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:36" ht="12.75">
       <c r="A113" s="30" t="s">
         <v>97</v>
       </c>
@@ -6749,15 +6749,15 @@
       </c>
       <c r="S113" s="36">
         <f t="shared" si="4"/>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="T113" s="36">
         <f t="shared" si="4"/>
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="U113" s="36">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="V113" s="36">
         <f t="shared" si="4"/>
@@ -6798,7 +6798,7 @@
       <c r="AH113" s="5"/>
       <c r="AI113" s="5"/>
     </row>
-    <row r="114" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:36" ht="12.75">
       <c r="A114" s="30" t="s">
         <v>98</v>
       </c>
@@ -6864,15 +6864,15 @@
       </c>
       <c r="Q114" s="36">
         <f t="shared" si="5"/>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="R114" s="36">
         <f t="shared" si="5"/>
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="S114" s="36">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="T114" s="36">
         <f t="shared" si="5"/>
@@ -6921,7 +6921,7 @@
       <c r="AH114" s="5"/>
       <c r="AI114" s="5"/>
     </row>
-    <row r="115" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:36" ht="12.75">
       <c r="A115" s="30"/>
       <c r="B115" s="30"/>
       <c r="C115" s="5"/>
@@ -6959,7 +6959,7 @@
       <c r="AI115" s="5"/>
       <c r="AJ115" s="5"/>
     </row>
-    <row r="116" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:36" ht="12.75">
       <c r="A116" s="30" t="s">
         <v>99</v>
       </c>
@@ -6999,7 +6999,7 @@
       <c r="AI116" s="5"/>
       <c r="AJ116" s="5"/>
     </row>
-    <row r="117" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:36" ht="12.75">
       <c r="A117" s="30"/>
       <c r="B117" s="30">
         <v>2023</v>
@@ -7093,7 +7093,7 @@
       <c r="AI117" s="5"/>
       <c r="AJ117" s="5"/>
     </row>
-    <row r="118" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:36" ht="12.75">
       <c r="A118" s="30" t="s">
         <v>100</v>
       </c>
@@ -7167,15 +7167,15 @@
       </c>
       <c r="S118" s="37">
         <f t="shared" si="6"/>
-        <v>17.715285878499422</v>
+        <v>23.620381171332561</v>
       </c>
       <c r="T118" s="37">
         <f t="shared" si="6"/>
-        <v>11.81019058566628</v>
+        <v>17.715285878499422</v>
       </c>
       <c r="U118" s="37">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>11.81019058566628</v>
       </c>
       <c r="V118" s="37">
         <f t="shared" si="6"/>
@@ -7217,7 +7217,7 @@
       <c r="AI118" s="5"/>
       <c r="AJ118" s="5"/>
     </row>
-    <row r="119" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:36" ht="12.75">
       <c r="A119" s="30"/>
       <c r="B119" s="37"/>
       <c r="C119" s="37"/>
@@ -7255,7 +7255,7 @@
       <c r="AI119" s="5"/>
       <c r="AJ119" s="5"/>
     </row>
-    <row r="120" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:36" ht="12.75">
       <c r="A120" s="30" t="s">
         <v>101</v>
       </c>
@@ -7318,15 +7318,15 @@
       </c>
       <c r="Q120" s="37">
         <f t="shared" si="7"/>
-        <v>17.288537268858313</v>
+        <v>23.051383025144418</v>
       </c>
       <c r="R120" s="37">
         <f t="shared" si="7"/>
-        <v>11.525691512572209</v>
+        <v>17.288537268858313</v>
       </c>
       <c r="S120" s="37">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>11.525691512572209</v>
       </c>
       <c r="T120" s="37">
         <f t="shared" si="7"/>
@@ -7376,7 +7376,7 @@
       <c r="AI120" s="5"/>
       <c r="AJ120" s="5"/>
     </row>
-    <row r="121" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:36" ht="12.75">
       <c r="A121" s="30" t="s">
         <v>102</v>
       </c>
@@ -7416,7 +7416,7 @@
       <c r="AI121" s="5"/>
       <c r="AJ121" s="5"/>
     </row>
-    <row r="122" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:36" ht="12.75">
       <c r="A122" s="30"/>
       <c r="B122" s="37"/>
       <c r="C122" s="37"/>
@@ -7454,7 +7454,7 @@
       <c r="AI122" s="5"/>
       <c r="AJ122" s="5"/>
     </row>
-    <row r="123" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:36" ht="12.75">
       <c r="A123" s="30" t="s">
         <v>103</v>
       </c>
@@ -7560,7 +7560,7 @@
       <c r="AI123" s="5"/>
       <c r="AJ123" s="5"/>
     </row>
-    <row r="124" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:36" ht="12.75">
       <c r="A124" s="30"/>
       <c r="B124" s="37"/>
       <c r="C124" s="37"/>
@@ -7598,7 +7598,7 @@
       <c r="AI124" s="5"/>
       <c r="AJ124" s="5"/>
     </row>
-    <row r="125" spans="1:36" s="35" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:36" s="35" customFormat="1" ht="12.75">
       <c r="A125" s="32" t="s">
         <v>54</v>
       </c>
@@ -7638,7 +7638,7 @@
       <c r="AI125" s="34"/>
       <c r="AJ125" s="34"/>
     </row>
-    <row r="126" spans="1:36" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:36" ht="25.5">
       <c r="A126" s="51"/>
       <c r="B126" s="5" t="s">
         <v>104</v>
@@ -7685,7 +7685,7 @@
       <c r="AH126" s="5"/>
       <c r="AI126" s="5"/>
     </row>
-    <row r="127" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:36" ht="12.75">
       <c r="A127" s="51" t="s">
         <v>96</v>
       </c>
@@ -7734,7 +7734,7 @@
       <c r="AH127" s="5"/>
       <c r="AI127" s="5"/>
     </row>
-    <row r="128" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:36" ht="12.75">
       <c r="A128" s="51"/>
       <c r="B128" s="37"/>
       <c r="C128" s="37"/>
@@ -7772,7 +7772,7 @@
       <c r="AI128" s="5"/>
       <c r="AJ128" s="5"/>
     </row>
-    <row r="129" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:36" ht="12.75">
       <c r="A129" s="30" t="s">
         <v>55</v>
       </c>
@@ -7867,7 +7867,7 @@
       <c r="AH129" s="5"/>
       <c r="AI129" s="5"/>
     </row>
-    <row r="130" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:36" ht="12.75">
       <c r="A130" s="30" t="s">
         <v>108</v>
       </c>
@@ -7941,15 +7941,15 @@
       </c>
       <c r="S130" s="36">
         <f t="shared" si="9"/>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="T130" s="36">
         <f t="shared" si="9"/>
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="U130" s="36">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="V130" s="36">
         <f t="shared" si="9"/>
@@ -7990,7 +7990,7 @@
       <c r="AH130" s="5"/>
       <c r="AI130" s="5"/>
     </row>
-    <row r="131" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:36" ht="12.75">
       <c r="A131" s="30" t="s">
         <v>109</v>
       </c>
@@ -8064,15 +8064,15 @@
       </c>
       <c r="S131" s="36">
         <f t="shared" si="10"/>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="T131" s="36">
         <f t="shared" si="10"/>
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="U131" s="36">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="V131" s="36">
         <f t="shared" si="10"/>
@@ -8113,7 +8113,7 @@
       <c r="AH131" s="5"/>
       <c r="AI131" s="5"/>
     </row>
-    <row r="132" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:36" ht="12.75">
       <c r="A132" s="30" t="s">
         <v>110</v>
       </c>
@@ -8183,15 +8183,15 @@
       </c>
       <c r="R132" s="36">
         <f t="shared" si="11"/>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="S132" s="36">
         <f t="shared" si="11"/>
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="T132" s="36">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="U132" s="36">
         <f t="shared" si="11"/>
@@ -8236,7 +8236,7 @@
       <c r="AH132" s="5"/>
       <c r="AI132" s="5"/>
     </row>
-    <row r="133" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:36" ht="12.75">
       <c r="A133" s="30" t="s">
         <v>111</v>
       </c>
@@ -8310,15 +8310,15 @@
       </c>
       <c r="S133" s="36">
         <f t="shared" si="12"/>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="T133" s="36">
         <f t="shared" si="12"/>
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="U133" s="36">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="V133" s="36">
         <f t="shared" si="12"/>
@@ -8359,7 +8359,7 @@
       <c r="AH133" s="5"/>
       <c r="AI133" s="5"/>
     </row>
-    <row r="134" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:36" ht="12.75">
       <c r="A134" s="30" t="s">
         <v>129</v>
       </c>
@@ -8425,15 +8425,15 @@
       </c>
       <c r="Q134" s="36">
         <f t="shared" si="13"/>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="R134" s="36">
         <f t="shared" si="13"/>
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="S134" s="36">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="T134" s="36">
         <f t="shared" si="13"/>
@@ -8483,7 +8483,7 @@
       <c r="AI134" s="5"/>
       <c r="AJ134" s="5"/>
     </row>
-    <row r="135" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:36" ht="12.75">
       <c r="A135" s="13"/>
       <c r="B135" s="5"/>
       <c r="C135" s="5"/>
@@ -8521,7 +8521,7 @@
       <c r="AI135" s="5"/>
       <c r="AJ135" s="5"/>
     </row>
-    <row r="136" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:36" ht="12.75">
       <c r="A136" s="30" t="s">
         <v>56</v>
       </c>
@@ -8563,7 +8563,7 @@
       <c r="AI136" s="5"/>
       <c r="AJ136" s="5"/>
     </row>
-    <row r="137" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:36" ht="12.75">
       <c r="A137" s="30" t="s">
         <v>57</v>
       </c>
@@ -8605,7 +8605,7 @@
       <c r="AI137" s="5"/>
       <c r="AJ137" s="5"/>
     </row>
-    <row r="138" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:36" ht="12.75">
       <c r="A138" s="30" t="s">
         <v>49</v>
       </c>
@@ -8647,7 +8647,7 @@
       <c r="AI138" s="5"/>
       <c r="AJ138" s="5"/>
     </row>
-    <row r="139" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:36" ht="12.75">
       <c r="A139" s="30" t="s">
         <v>50</v>
       </c>
@@ -8689,7 +8689,7 @@
       <c r="AI139" s="5"/>
       <c r="AJ139" s="5"/>
     </row>
-    <row r="140" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:36" ht="12.75">
       <c r="A140" s="5" t="s">
         <v>51</v>
       </c>
@@ -8731,7 +8731,7 @@
       <c r="AI140" s="5"/>
       <c r="AJ140" s="5"/>
     </row>
-    <row r="141" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:36" ht="12.75">
       <c r="A141" s="30" t="s">
         <v>52</v>
       </c>
@@ -8773,7 +8773,7 @@
       <c r="AI141" s="5"/>
       <c r="AJ141" s="5"/>
     </row>
-    <row r="142" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:36" ht="12.75">
       <c r="A142" s="30" t="s">
         <v>53</v>
       </c>
@@ -8815,7 +8815,7 @@
       <c r="AI142" s="5"/>
       <c r="AJ142" s="5"/>
     </row>
-    <row r="143" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:36" ht="12.75">
       <c r="A143" s="13"/>
       <c r="B143" s="5"/>
       <c r="C143" s="5"/>
@@ -8853,7 +8853,7 @@
       <c r="AI143" s="5"/>
       <c r="AJ143" s="5"/>
     </row>
-    <row r="144" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:36" ht="12.75">
       <c r="A144" s="40" t="s">
         <v>58</v>
       </c>
@@ -8893,7 +8893,7 @@
       <c r="AI144" s="5"/>
       <c r="AJ144" s="5"/>
     </row>
-    <row r="145" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:74" ht="12.75">
       <c r="A145" s="30"/>
       <c r="B145" s="30">
         <v>2023</v>
@@ -8987,7 +8987,7 @@
       <c r="AI145" s="5"/>
       <c r="AJ145" s="5"/>
     </row>
-    <row r="146" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:74" ht="12.75">
       <c r="A146" s="5" t="s">
         <v>112</v>
       </c>
@@ -9086,7 +9086,7 @@
       <c r="AI146" s="5"/>
       <c r="AJ146" s="5"/>
     </row>
-    <row r="147" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:74" ht="12.75">
       <c r="A147" s="30" t="s">
         <v>102</v>
       </c>
@@ -9126,7 +9126,7 @@
       <c r="AI147" s="5"/>
       <c r="AJ147" s="5"/>
     </row>
-    <row r="148" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:74" ht="12.75">
       <c r="A148" s="30"/>
       <c r="B148" s="37">
         <v>2023</v>
@@ -9220,7 +9220,7 @@
       <c r="AI148" s="5"/>
       <c r="AJ148" s="5"/>
     </row>
-    <row r="149" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:74" ht="12.75">
       <c r="A149" s="5" t="s">
         <v>113</v>
       </c>
@@ -9294,15 +9294,15 @@
       </c>
       <c r="S149" s="37">
         <f t="shared" si="14"/>
-        <v>0.31218750000000001</v>
+        <v>0.41625000000000001</v>
       </c>
       <c r="T149" s="37">
         <f t="shared" si="14"/>
-        <v>0.208125</v>
+        <v>0.31218750000000001</v>
       </c>
       <c r="U149" s="37">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>0.208125</v>
       </c>
       <c r="V149" s="37">
         <f t="shared" si="14"/>
@@ -9344,7 +9344,7 @@
       <c r="AI149" s="5"/>
       <c r="AJ149" s="5"/>
     </row>
-    <row r="150" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:74" ht="12.75">
       <c r="A150" s="5"/>
       <c r="B150" s="37"/>
       <c r="C150" s="37"/>
@@ -9382,7 +9382,7 @@
       <c r="AI150" s="5"/>
       <c r="AJ150" s="5"/>
     </row>
-    <row r="151" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:74" ht="12.75">
       <c r="A151" s="30"/>
       <c r="B151" s="37">
         <v>2023</v>
@@ -9476,7 +9476,7 @@
       <c r="AI151" s="5"/>
       <c r="AJ151" s="5"/>
     </row>
-    <row r="152" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:74" ht="12.75">
       <c r="A152" s="5" t="s">
         <v>114</v>
       </c>
@@ -9546,15 +9546,15 @@
       </c>
       <c r="R152" s="37">
         <f t="shared" si="15"/>
-        <v>0.31218750000000001</v>
+        <v>0.41625000000000001</v>
       </c>
       <c r="S152" s="37">
         <f t="shared" si="15"/>
-        <v>0.208125</v>
+        <v>0.31218750000000001</v>
       </c>
       <c r="T152" s="37">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>0.208125</v>
       </c>
       <c r="U152" s="37">
         <f t="shared" si="15"/>
@@ -9600,7 +9600,7 @@
       <c r="AI152" s="5"/>
       <c r="AJ152" s="5"/>
     </row>
-    <row r="153" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:74" ht="12.75">
       <c r="A153" s="30"/>
       <c r="B153" s="37"/>
       <c r="C153" s="37"/>
@@ -9638,7 +9638,7 @@
       <c r="AI153" s="5"/>
       <c r="AJ153" s="5"/>
     </row>
-    <row r="154" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:74" ht="12.75">
       <c r="A154" s="30"/>
       <c r="B154" s="37">
         <v>2023</v>
@@ -9732,7 +9732,7 @@
       <c r="AI154" s="5"/>
       <c r="AJ154" s="5"/>
     </row>
-    <row r="155" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:74" ht="12.75">
       <c r="A155" s="5" t="s">
         <v>59</v>
       </c>
@@ -9806,15 +9806,15 @@
       </c>
       <c r="S155" s="37">
         <f t="shared" si="16"/>
-        <v>0.31218750000000001</v>
+        <v>0.41625000000000001</v>
       </c>
       <c r="T155" s="37">
         <f t="shared" si="16"/>
-        <v>0.208125</v>
+        <v>0.31218750000000001</v>
       </c>
       <c r="U155" s="37">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>0.208125</v>
       </c>
       <c r="V155" s="37">
         <f t="shared" si="16"/>
@@ -9856,7 +9856,7 @@
       <c r="AI155" s="5"/>
       <c r="AJ155" s="5"/>
     </row>
-    <row r="156" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:74" ht="12.75">
       <c r="A156" s="5"/>
       <c r="B156" s="37"/>
       <c r="C156" s="37"/>
@@ -9894,7 +9894,7 @@
       <c r="AI156" s="5"/>
       <c r="AJ156" s="5"/>
     </row>
-    <row r="157" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:74" ht="12.75">
       <c r="A157" s="30"/>
       <c r="B157" s="37">
         <v>2023</v>
@@ -9988,7 +9988,7 @@
       <c r="AI157" s="5"/>
       <c r="AJ157" s="5"/>
     </row>
-    <row r="158" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:74" ht="12.75">
       <c r="A158" s="5" t="s">
         <v>127</v>
       </c>
@@ -10054,15 +10054,15 @@
       </c>
       <c r="Q158" s="37">
         <f t="shared" si="17"/>
-        <v>0.31218750000000001</v>
+        <v>0.41625000000000001</v>
       </c>
       <c r="R158" s="37">
         <f t="shared" si="17"/>
-        <v>0.208125</v>
+        <v>0.31218750000000001</v>
       </c>
       <c r="S158" s="37">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>0.208125</v>
       </c>
       <c r="T158" s="37">
         <f t="shared" si="17"/>
@@ -10112,7 +10112,7 @@
       <c r="AI158" s="5"/>
       <c r="AJ158" s="5"/>
     </row>
-    <row r="159" spans="1:74" s="35" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:74" s="35" customFormat="1" ht="12.75">
       <c r="A159" s="32" t="s">
         <v>115</v>
       </c>
@@ -10152,7 +10152,7 @@
       <c r="AI159" s="34"/>
       <c r="AJ159" s="34"/>
     </row>
-    <row r="160" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:74" ht="12.75">
       <c r="A160" s="5"/>
       <c r="B160" s="5">
         <v>2023</v>
@@ -10284,7 +10284,7 @@
       <c r="BU160" s="5"/>
       <c r="BV160" s="5"/>
     </row>
-    <row r="161" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:74" ht="12.75">
       <c r="A161" s="5" t="s">
         <v>116</v>
       </c>
@@ -10446,7 +10446,7 @@
       <c r="BU161" s="5"/>
       <c r="BV161" s="5"/>
     </row>
-    <row r="162" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:74" ht="12.75">
       <c r="A162" s="5" t="s">
         <v>117</v>
       </c>
@@ -10580,7 +10580,7 @@
       <c r="BU162" s="5"/>
       <c r="BV162" s="5"/>
     </row>
-    <row r="163" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:74" ht="12.75">
       <c r="A163" s="5"/>
       <c r="B163" s="27"/>
       <c r="C163" s="27"/>
@@ -10656,7 +10656,7 @@
       <c r="BU163" s="5"/>
       <c r="BV163" s="5"/>
     </row>
-    <row r="164" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:74" ht="12.75">
       <c r="A164" s="5" t="s">
         <v>54</v>
       </c>
@@ -10818,7 +10818,7 @@
       <c r="BU164" s="5"/>
       <c r="BV164" s="5"/>
     </row>
-    <row r="165" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:74" ht="12.75">
       <c r="A165" s="5" t="s">
         <v>93</v>
       </c>
@@ -10884,15 +10884,15 @@
       </c>
       <c r="Q165" s="53">
         <f t="shared" si="19"/>
-        <v>17.288537268858313</v>
+        <v>23.051383025144418</v>
       </c>
       <c r="R165" s="53">
         <f t="shared" si="19"/>
-        <v>11.525691512572209</v>
+        <v>17.288537268858313</v>
       </c>
       <c r="S165" s="53">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>11.525691512572209</v>
       </c>
       <c r="T165" s="53">
         <f t="shared" si="19"/>
@@ -10980,7 +10980,7 @@
       <c r="BU165" s="5"/>
       <c r="BV165" s="5"/>
     </row>
-    <row r="166" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:74" ht="12.75">
       <c r="A166" s="5"/>
       <c r="B166" s="53"/>
       <c r="C166" s="53"/>
@@ -11056,7 +11056,7 @@
       <c r="BU166" s="5"/>
       <c r="BV166" s="5"/>
     </row>
-    <row r="167" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:74" ht="12.75">
       <c r="A167" s="5" t="s">
         <v>118</v>
       </c>
@@ -11136,7 +11136,7 @@
       <c r="BU167" s="5"/>
       <c r="BV167" s="5"/>
     </row>
-    <row r="168" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:74" ht="12.75">
       <c r="A168" s="5" t="s">
         <v>119</v>
       </c>
@@ -11298,7 +11298,7 @@
       <c r="BU168" s="5"/>
       <c r="BV168" s="5"/>
     </row>
-    <row r="169" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:74" ht="12.75">
       <c r="A169" s="5" t="s">
         <v>120</v>
       </c>
@@ -11378,7 +11378,7 @@
       <c r="BU169" s="5"/>
       <c r="BV169" s="5"/>
     </row>
-    <row r="170" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:74" ht="12.75">
       <c r="A170" s="5" t="s">
         <v>121</v>
       </c>
@@ -11458,7 +11458,7 @@
       <c r="BU170" s="5"/>
       <c r="BV170" s="5"/>
     </row>
-    <row r="171" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:74" ht="12.75">
       <c r="A171" s="5"/>
       <c r="B171" s="5"/>
       <c r="C171" s="5"/>
@@ -11534,7 +11534,7 @@
       <c r="BU171" s="5"/>
       <c r="BV171" s="5"/>
     </row>
-    <row r="172" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:74" ht="12.75">
       <c r="A172" s="5" t="s">
         <v>122</v>
       </c>
@@ -11696,7 +11696,7 @@
       <c r="BU172" s="5"/>
       <c r="BV172" s="5"/>
     </row>
-    <row r="173" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:74" ht="12.75">
       <c r="A173" s="5" t="s">
         <v>123</v>
       </c>
@@ -11762,15 +11762,15 @@
       </c>
       <c r="Q173" s="54">
         <f t="shared" si="22"/>
-        <v>3786189.6618799707</v>
+        <v>5048252.8825066276</v>
       </c>
       <c r="R173" s="54">
         <f t="shared" si="22"/>
-        <v>2524126.4412533138</v>
+        <v>3786189.6618799707</v>
       </c>
       <c r="S173" s="54">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>2524126.4412533138</v>
       </c>
       <c r="T173" s="54">
         <f t="shared" si="22"/>
@@ -11858,7 +11858,7 @@
       <c r="BU173" s="5"/>
       <c r="BV173" s="5"/>
     </row>
-    <row r="174" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:74" ht="12.75">
       <c r="A174" s="5" t="s">
         <v>124</v>
       </c>
@@ -11924,15 +11924,15 @@
       </c>
       <c r="Q174" s="54">
         <f t="shared" si="23"/>
-        <v>35384950.111027762</v>
+        <v>47179933.481370352</v>
       </c>
       <c r="R174" s="54">
         <f t="shared" si="23"/>
-        <v>23589966.740685176</v>
+        <v>35384950.111027762</v>
       </c>
       <c r="S174" s="54">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>23589966.740685176</v>
       </c>
       <c r="T174" s="54">
         <f t="shared" si="23"/>
@@ -12020,7 +12020,7 @@
       <c r="BU174" s="5"/>
       <c r="BV174" s="5"/>
     </row>
-    <row r="175" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:74" ht="12.75">
       <c r="A175" s="5" t="s">
         <v>125</v>
       </c>
@@ -12086,15 +12086,15 @@
       </c>
       <c r="Q175" s="54">
         <f t="shared" si="24"/>
-        <v>37861896.618799709</v>
+        <v>50482528.825066276</v>
       </c>
       <c r="R175" s="54">
         <f t="shared" si="24"/>
-        <v>25241264.412533138</v>
+        <v>37861896.618799709</v>
       </c>
       <c r="S175" s="54">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>25241264.412533138</v>
       </c>
       <c r="T175" s="54">
         <f t="shared" si="24"/>
@@ -12182,7 +12182,7 @@
       <c r="BU175" s="5"/>
       <c r="BV175" s="5"/>
     </row>
-    <row r="176" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:74" ht="12.75">
       <c r="A176" s="5"/>
       <c r="B176" s="5"/>
       <c r="C176" s="5"/>
@@ -12258,7 +12258,7 @@
       <c r="BU176" s="5"/>
       <c r="BV176" s="5"/>
     </row>
-    <row r="177" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:74" ht="12.75">
       <c r="A177" s="5" t="s">
         <v>126</v>
       </c>
@@ -12420,7 +12420,7 @@
       <c r="BU177" s="5"/>
       <c r="BV177" s="5"/>
     </row>
-    <row r="178" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:74" ht="12.75">
       <c r="A178" s="5"/>
       <c r="B178" s="5"/>
       <c r="C178" s="5"/>
@@ -12496,7 +12496,7 @@
       <c r="BU178" s="5"/>
       <c r="BV178" s="5"/>
     </row>
-    <row r="179" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:74" ht="12.75">
       <c r="A179" s="5"/>
       <c r="B179" s="5"/>
       <c r="C179" s="5"/>
@@ -12572,7 +12572,7 @@
       <c r="BU179" s="5"/>
       <c r="BV179" s="5"/>
     </row>
-    <row r="180" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:74" ht="12.75">
       <c r="A180" s="5"/>
       <c r="B180" s="5"/>
       <c r="C180" s="5"/>
@@ -12648,7 +12648,7 @@
       <c r="BU180" s="5"/>
       <c r="BV180" s="5"/>
     </row>
-    <row r="181" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:74" ht="12.75">
       <c r="A181" s="5"/>
       <c r="B181" s="5"/>
       <c r="C181" s="5"/>
@@ -12724,7 +12724,7 @@
       <c r="BU181" s="5"/>
       <c r="BV181" s="5"/>
     </row>
-    <row r="182" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:74" ht="12.75">
       <c r="A182" s="5"/>
       <c r="B182" s="5"/>
       <c r="C182" s="5"/>
@@ -12800,7 +12800,7 @@
       <c r="BU182" s="5"/>
       <c r="BV182" s="5"/>
     </row>
-    <row r="183" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:74" ht="12.75">
       <c r="A183" s="5"/>
       <c r="B183" s="5"/>
       <c r="C183" s="5"/>
@@ -12876,7 +12876,7 @@
       <c r="BU183" s="5"/>
       <c r="BV183" s="5"/>
     </row>
-    <row r="184" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:74" ht="12.75">
       <c r="A184" s="5"/>
       <c r="B184" s="5"/>
       <c r="C184" s="5"/>
@@ -12952,7 +12952,7 @@
       <c r="BU184" s="5"/>
       <c r="BV184" s="5"/>
     </row>
-    <row r="185" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:74" ht="12.75">
       <c r="A185" s="5"/>
       <c r="B185" s="5"/>
       <c r="C185" s="5"/>
@@ -13028,7 +13028,7 @@
       <c r="BU185" s="5"/>
       <c r="BV185" s="5"/>
     </row>
-    <row r="186" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:74" ht="12.75">
       <c r="A186" s="5"/>
       <c r="B186" s="5"/>
       <c r="C186" s="5"/>
@@ -13104,7 +13104,7 @@
       <c r="BU186" s="5"/>
       <c r="BV186" s="5"/>
     </row>
-    <row r="187" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:74" ht="12.75">
       <c r="A187" s="5"/>
       <c r="B187" s="5"/>
       <c r="C187" s="5"/>
@@ -13180,7 +13180,7 @@
       <c r="BU187" s="5"/>
       <c r="BV187" s="5"/>
     </row>
-    <row r="188" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:74" ht="12.75">
       <c r="A188" s="5"/>
       <c r="B188" s="5"/>
       <c r="C188" s="5"/>
@@ -13256,7 +13256,7 @@
       <c r="BU188" s="5"/>
       <c r="BV188" s="5"/>
     </row>
-    <row r="189" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:74" ht="12.75">
       <c r="A189" s="5"/>
       <c r="B189" s="5"/>
       <c r="C189" s="5"/>
@@ -13332,7 +13332,7 @@
       <c r="BU189" s="5"/>
       <c r="BV189" s="5"/>
     </row>
-    <row r="190" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:74" ht="12.75">
       <c r="A190" s="5"/>
       <c r="B190" s="5"/>
       <c r="C190" s="5"/>
@@ -13408,7 +13408,7 @@
       <c r="BU190" s="5"/>
       <c r="BV190" s="5"/>
     </row>
-    <row r="191" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:74" ht="12.75">
       <c r="A191" s="5"/>
       <c r="B191" s="5"/>
       <c r="C191" s="5"/>
@@ -13484,7 +13484,7 @@
       <c r="BU191" s="5"/>
       <c r="BV191" s="5"/>
     </row>
-    <row r="192" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:74" ht="12.75">
       <c r="A192" s="5"/>
       <c r="B192" s="5"/>
       <c r="C192" s="5"/>
@@ -13560,7 +13560,7 @@
       <c r="BU192" s="5"/>
       <c r="BV192" s="5"/>
     </row>
-    <row r="193" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:74" ht="12.75">
       <c r="A193" s="5"/>
       <c r="B193" s="5"/>
       <c r="C193" s="5"/>
@@ -13636,7 +13636,7 @@
       <c r="BU193" s="5"/>
       <c r="BV193" s="5"/>
     </row>
-    <row r="194" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:74" ht="12.75">
       <c r="A194" s="5"/>
       <c r="B194" s="5"/>
       <c r="C194" s="5"/>
@@ -13712,7 +13712,7 @@
       <c r="BU194" s="5"/>
       <c r="BV194" s="5"/>
     </row>
-    <row r="195" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:74" ht="12.75">
       <c r="A195" s="5"/>
       <c r="B195" s="5"/>
       <c r="C195" s="5"/>
@@ -13788,7 +13788,7 @@
       <c r="BU195" s="5"/>
       <c r="BV195" s="5"/>
     </row>
-    <row r="196" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:74" ht="12.75">
       <c r="A196" s="5"/>
       <c r="B196" s="5"/>
       <c r="C196" s="5"/>
@@ -13864,7 +13864,7 @@
       <c r="BU196" s="5"/>
       <c r="BV196" s="5"/>
     </row>
-    <row r="197" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:74" ht="12.75">
       <c r="A197" s="5"/>
       <c r="B197" s="5"/>
       <c r="C197" s="5"/>
@@ -13940,7 +13940,7 @@
       <c r="BU197" s="5"/>
       <c r="BV197" s="5"/>
     </row>
-    <row r="198" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:74" ht="12.75">
       <c r="A198" s="5"/>
       <c r="B198" s="5"/>
       <c r="C198" s="5"/>
@@ -14016,7 +14016,7 @@
       <c r="BU198" s="5"/>
       <c r="BV198" s="5"/>
     </row>
-    <row r="199" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:74" ht="12.75">
       <c r="A199" s="5"/>
       <c r="B199" s="5"/>
       <c r="C199" s="5"/>
@@ -14092,7 +14092,7 @@
       <c r="BU199" s="5"/>
       <c r="BV199" s="5"/>
     </row>
-    <row r="200" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:74" ht="12.75">
       <c r="A200" s="5"/>
       <c r="B200" s="5"/>
       <c r="C200" s="5"/>
@@ -14168,7 +14168,7 @@
       <c r="BU200" s="5"/>
       <c r="BV200" s="5"/>
     </row>
-    <row r="201" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:74" ht="12.75">
       <c r="A201" s="5"/>
       <c r="B201" s="5"/>
       <c r="C201" s="5"/>
@@ -14244,7 +14244,7 @@
       <c r="BU201" s="5"/>
       <c r="BV201" s="5"/>
     </row>
-    <row r="202" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:74" ht="12.75">
       <c r="A202" s="5"/>
       <c r="B202" s="5"/>
       <c r="C202" s="5"/>
@@ -14320,7 +14320,7 @@
       <c r="BU202" s="5"/>
       <c r="BV202" s="5"/>
     </row>
-    <row r="203" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:74" ht="12.75">
       <c r="A203" s="5"/>
       <c r="B203" s="5"/>
       <c r="C203" s="5"/>
@@ -14396,7 +14396,7 @@
       <c r="BU203" s="5"/>
       <c r="BV203" s="5"/>
     </row>
-    <row r="204" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:74" ht="12.75">
       <c r="A204" s="5"/>
       <c r="B204" s="5"/>
       <c r="C204" s="5"/>
@@ -14472,7 +14472,7 @@
       <c r="BU204" s="5"/>
       <c r="BV204" s="5"/>
     </row>
-    <row r="205" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:74" ht="12.75">
       <c r="A205" s="5"/>
       <c r="B205" s="5"/>
       <c r="C205" s="5"/>
@@ -14548,7 +14548,7 @@
       <c r="BU205" s="5"/>
       <c r="BV205" s="5"/>
     </row>
-    <row r="206" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:74" ht="12.75">
       <c r="A206" s="5"/>
       <c r="B206" s="5"/>
       <c r="C206" s="5"/>
@@ -14624,7 +14624,7 @@
       <c r="BU206" s="5"/>
       <c r="BV206" s="5"/>
     </row>
-    <row r="207" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:74" ht="12.75">
       <c r="A207" s="5"/>
       <c r="B207" s="5"/>
       <c r="C207" s="5"/>
@@ -14700,7 +14700,7 @@
       <c r="BU207" s="5"/>
       <c r="BV207" s="5"/>
     </row>
-    <row r="208" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:74" ht="12.75">
       <c r="A208" s="5"/>
       <c r="B208" s="5"/>
       <c r="C208" s="5"/>
@@ -14776,7 +14776,7 @@
       <c r="BU208" s="5"/>
       <c r="BV208" s="5"/>
     </row>
-    <row r="209" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:74" ht="12.75">
       <c r="A209" s="5"/>
       <c r="B209" s="5"/>
       <c r="C209" s="5"/>
@@ -14852,7 +14852,7 @@
       <c r="BU209" s="5"/>
       <c r="BV209" s="5"/>
     </row>
-    <row r="210" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:74" ht="12.75">
       <c r="A210" s="5"/>
       <c r="B210" s="5"/>
       <c r="C210" s="5"/>
@@ -14928,7 +14928,7 @@
       <c r="BU210" s="5"/>
       <c r="BV210" s="5"/>
     </row>
-    <row r="211" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:74" ht="12.75">
       <c r="A211" s="5"/>
       <c r="B211" s="5"/>
       <c r="C211" s="5"/>
@@ -15004,7 +15004,7 @@
       <c r="BU211" s="5"/>
       <c r="BV211" s="5"/>
     </row>
-    <row r="212" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:74" ht="12.75">
       <c r="A212" s="5"/>
       <c r="B212" s="5"/>
       <c r="C212" s="5"/>
@@ -15080,7 +15080,7 @@
       <c r="BU212" s="5"/>
       <c r="BV212" s="5"/>
     </row>
-    <row r="213" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:74" ht="12.75">
       <c r="A213" s="5"/>
       <c r="B213" s="5"/>
       <c r="C213" s="5"/>
@@ -15156,7 +15156,7 @@
       <c r="BU213" s="5"/>
       <c r="BV213" s="5"/>
     </row>
-    <row r="214" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:74" ht="12.75">
       <c r="A214" s="5"/>
       <c r="B214" s="5"/>
       <c r="C214" s="5"/>
@@ -15232,7 +15232,7 @@
       <c r="BU214" s="5"/>
       <c r="BV214" s="5"/>
     </row>
-    <row r="215" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:74" ht="12.75">
       <c r="A215" s="5"/>
       <c r="B215" s="5"/>
       <c r="C215" s="5"/>
@@ -15308,7 +15308,7 @@
       <c r="BU215" s="5"/>
       <c r="BV215" s="5"/>
     </row>
-    <row r="216" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:74" ht="12.75">
       <c r="A216" s="5"/>
       <c r="B216" s="5"/>
       <c r="C216" s="5"/>
@@ -15384,7 +15384,7 @@
       <c r="BU216" s="5"/>
       <c r="BV216" s="5"/>
     </row>
-    <row r="217" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:74" ht="12.75">
       <c r="A217" s="5"/>
       <c r="B217" s="5"/>
       <c r="C217" s="5"/>
@@ -15460,7 +15460,7 @@
       <c r="BU217" s="5"/>
       <c r="BV217" s="5"/>
     </row>
-    <row r="218" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:74" ht="12.75">
       <c r="A218" s="5"/>
       <c r="B218" s="5"/>
       <c r="C218" s="5"/>
@@ -15536,7 +15536,7 @@
       <c r="BU218" s="5"/>
       <c r="BV218" s="5"/>
     </row>
-    <row r="219" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:74" ht="12.75">
       <c r="A219" s="5"/>
       <c r="B219" s="5"/>
       <c r="C219" s="5"/>
@@ -15612,7 +15612,7 @@
       <c r="BU219" s="5"/>
       <c r="BV219" s="5"/>
     </row>
-    <row r="220" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:74" ht="12.75">
       <c r="A220" s="5"/>
       <c r="B220" s="5"/>
       <c r="C220" s="5"/>
@@ -15688,7 +15688,7 @@
       <c r="BU220" s="5"/>
       <c r="BV220" s="5"/>
     </row>
-    <row r="221" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:74" ht="12.75">
       <c r="A221" s="5"/>
       <c r="B221" s="5"/>
       <c r="C221" s="5"/>
@@ -15764,7 +15764,7 @@
       <c r="BU221" s="5"/>
       <c r="BV221" s="5"/>
     </row>
-    <row r="222" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:74" ht="12.75">
       <c r="A222" s="5"/>
       <c r="B222" s="5"/>
       <c r="C222" s="5"/>
@@ -15840,7 +15840,7 @@
       <c r="BU222" s="5"/>
       <c r="BV222" s="5"/>
     </row>
-    <row r="223" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:74" ht="12.75">
       <c r="A223" s="5"/>
       <c r="B223" s="5"/>
       <c r="C223" s="5"/>
@@ -15916,7 +15916,7 @@
       <c r="BU223" s="5"/>
       <c r="BV223" s="5"/>
     </row>
-    <row r="224" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:74" ht="12.75">
       <c r="A224" s="5"/>
       <c r="B224" s="5"/>
       <c r="C224" s="5"/>
@@ -15992,7 +15992,7 @@
       <c r="BU224" s="5"/>
       <c r="BV224" s="5"/>
     </row>
-    <row r="225" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:74" ht="12.75">
       <c r="A225" s="5"/>
       <c r="B225" s="5"/>
       <c r="C225" s="5"/>
@@ -16068,7 +16068,7 @@
       <c r="BU225" s="5"/>
       <c r="BV225" s="5"/>
     </row>
-    <row r="226" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:74" ht="12.75">
       <c r="A226" s="5"/>
       <c r="B226" s="5"/>
       <c r="C226" s="5"/>
@@ -16144,7 +16144,7 @@
       <c r="BU226" s="5"/>
       <c r="BV226" s="5"/>
     </row>
-    <row r="227" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:74" ht="12.75">
       <c r="A227" s="5"/>
       <c r="B227" s="5"/>
       <c r="C227" s="5"/>
@@ -16220,7 +16220,7 @@
       <c r="BU227" s="5"/>
       <c r="BV227" s="5"/>
     </row>
-    <row r="228" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:74" ht="12.75">
       <c r="A228" s="5"/>
       <c r="B228" s="5"/>
       <c r="C228" s="5"/>
@@ -16296,7 +16296,7 @@
       <c r="BU228" s="5"/>
       <c r="BV228" s="5"/>
     </row>
-    <row r="229" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:74" ht="12.75">
       <c r="A229" s="5"/>
       <c r="B229" s="5"/>
       <c r="C229" s="5"/>
@@ -16372,7 +16372,7 @@
       <c r="BU229" s="5"/>
       <c r="BV229" s="5"/>
     </row>
-    <row r="230" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:74" ht="12.75">
       <c r="A230" s="5"/>
       <c r="B230" s="5"/>
       <c r="C230" s="5"/>
@@ -16448,7 +16448,7 @@
       <c r="BU230" s="5"/>
       <c r="BV230" s="5"/>
     </row>
-    <row r="231" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:74" ht="12.75">
       <c r="A231" s="5"/>
       <c r="B231" s="5"/>
       <c r="C231" s="5"/>
@@ -16524,7 +16524,7 @@
       <c r="BU231" s="5"/>
       <c r="BV231" s="5"/>
     </row>
-    <row r="232" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:74" ht="12.75">
       <c r="A232" s="5"/>
       <c r="B232" s="5"/>
       <c r="C232" s="5"/>
@@ -16600,7 +16600,7 @@
       <c r="BU232" s="5"/>
       <c r="BV232" s="5"/>
     </row>
-    <row r="233" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:74" ht="12.75">
       <c r="A233" s="5"/>
       <c r="B233" s="5"/>
       <c r="C233" s="5"/>
@@ -16676,7 +16676,7 @@
       <c r="BU233" s="5"/>
       <c r="BV233" s="5"/>
     </row>
-    <row r="234" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:74" ht="12.75">
       <c r="A234" s="5"/>
       <c r="B234" s="5"/>
       <c r="C234" s="5"/>
@@ -16752,7 +16752,7 @@
       <c r="BU234" s="5"/>
       <c r="BV234" s="5"/>
     </row>
-    <row r="235" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:74" ht="12.75">
       <c r="A235" s="5"/>
       <c r="B235" s="5"/>
       <c r="C235" s="5"/>
@@ -16828,7 +16828,7 @@
       <c r="BU235" s="5"/>
       <c r="BV235" s="5"/>
     </row>
-    <row r="236" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:74" ht="12.75">
       <c r="A236" s="5"/>
       <c r="B236" s="5"/>
       <c r="C236" s="5"/>
@@ -16904,7 +16904,7 @@
       <c r="BU236" s="5"/>
       <c r="BV236" s="5"/>
     </row>
-    <row r="237" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:74" ht="12.75">
       <c r="A237" s="5"/>
       <c r="B237" s="5"/>
       <c r="C237" s="5"/>
@@ -16980,7 +16980,7 @@
       <c r="BU237" s="5"/>
       <c r="BV237" s="5"/>
     </row>
-    <row r="238" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:74" ht="12.75">
       <c r="A238" s="5"/>
       <c r="B238" s="5"/>
       <c r="C238" s="5"/>
@@ -17056,7 +17056,7 @@
       <c r="BU238" s="5"/>
       <c r="BV238" s="5"/>
     </row>
-    <row r="239" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:74" ht="12.75">
       <c r="A239" s="5"/>
       <c r="B239" s="5"/>
       <c r="C239" s="5"/>
@@ -17132,7 +17132,7 @@
       <c r="BU239" s="5"/>
       <c r="BV239" s="5"/>
     </row>
-    <row r="240" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:74" ht="12.75">
       <c r="A240" s="5"/>
       <c r="B240" s="5"/>
       <c r="C240" s="5"/>
@@ -17208,7 +17208,7 @@
       <c r="BU240" s="5"/>
       <c r="BV240" s="5"/>
     </row>
-    <row r="241" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:74" ht="12.75">
       <c r="A241" s="5"/>
       <c r="B241" s="5"/>
       <c r="C241" s="5"/>
@@ -17284,7 +17284,7 @@
       <c r="BU241" s="5"/>
       <c r="BV241" s="5"/>
     </row>
-    <row r="242" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:74" ht="12.75">
       <c r="A242" s="5"/>
       <c r="B242" s="5"/>
       <c r="C242" s="5"/>
@@ -17322,7 +17322,7 @@
       <c r="AI242" s="5"/>
       <c r="AJ242" s="5"/>
     </row>
-    <row r="243" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:74" ht="12.75">
       <c r="A243" s="5"/>
       <c r="B243" s="5"/>
       <c r="C243" s="5"/>
@@ -17360,7 +17360,7 @@
       <c r="AI243" s="5"/>
       <c r="AJ243" s="5"/>
     </row>
-    <row r="244" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:74" ht="12.75">
       <c r="A244" s="5"/>
       <c r="B244" s="5"/>
       <c r="C244" s="5"/>
@@ -17398,7 +17398,7 @@
       <c r="AI244" s="5"/>
       <c r="AJ244" s="5"/>
     </row>
-    <row r="245" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:74" ht="12.75">
       <c r="A245" s="5"/>
       <c r="B245" s="5"/>
       <c r="C245" s="5"/>
@@ -17436,7 +17436,7 @@
       <c r="AI245" s="5"/>
       <c r="AJ245" s="5"/>
     </row>
-    <row r="246" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:74" ht="12.75">
       <c r="A246" s="5"/>
       <c r="B246" s="5"/>
       <c r="C246" s="5"/>
@@ -17474,7 +17474,7 @@
       <c r="AI246" s="5"/>
       <c r="AJ246" s="5"/>
     </row>
-    <row r="247" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:74" ht="12.75">
       <c r="A247" s="5"/>
       <c r="B247" s="5"/>
       <c r="C247" s="5"/>
@@ -17512,7 +17512,7 @@
       <c r="AI247" s="5"/>
       <c r="AJ247" s="5"/>
     </row>
-    <row r="248" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:74" ht="12.75">
       <c r="A248" s="5"/>
       <c r="B248" s="5"/>
       <c r="C248" s="5"/>
@@ -17550,7 +17550,7 @@
       <c r="AI248" s="5"/>
       <c r="AJ248" s="5"/>
     </row>
-    <row r="249" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:74" ht="12.75">
       <c r="A249" s="5"/>
       <c r="B249" s="5"/>
       <c r="C249" s="5"/>
@@ -17588,7 +17588,7 @@
       <c r="AI249" s="5"/>
       <c r="AJ249" s="5"/>
     </row>
-    <row r="250" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:74" ht="12.75">
       <c r="A250" s="5"/>
       <c r="B250" s="5"/>
       <c r="C250" s="5"/>
@@ -17626,7 +17626,7 @@
       <c r="AI250" s="5"/>
       <c r="AJ250" s="5"/>
     </row>
-    <row r="251" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:74" ht="12.75">
       <c r="A251" s="5"/>
       <c r="B251" s="5"/>
       <c r="C251" s="5"/>
@@ -17664,7 +17664,7 @@
       <c r="AI251" s="5"/>
       <c r="AJ251" s="5"/>
     </row>
-    <row r="252" spans="1:74" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:74" ht="12.75">
       <c r="A252" s="5"/>
       <c r="B252" s="5"/>
       <c r="C252" s="5"/>
@@ -17725,12 +17725,12 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -17825,7 +17825,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" ht="30">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -17897,15 +17897,15 @@
       </c>
       <c r="S2" s="2">
         <f>'Inflation Reduction Act - Elec'!Q158</f>
-        <v>0.31218750000000001</v>
+        <v>0.41625000000000001</v>
       </c>
       <c r="T2" s="2">
         <f>'Inflation Reduction Act - Elec'!R158</f>
-        <v>0.208125</v>
+        <v>0.31218750000000001</v>
       </c>
       <c r="U2" s="2">
         <f>'Inflation Reduction Act - Elec'!S158</f>
-        <v>0</v>
+        <v>0.208125</v>
       </c>
       <c r="V2" s="2">
         <f>'Inflation Reduction Act - Elec'!T158</f>

</xml_diff>